<commit_message>
📊 Línea 141: horarios completos del 30/12/2025
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,11 +467,16 @@
           <t>Parada</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 28/12/2025 23:54:47</t>
+          <t>Última actualización: 29/12/2025 22:53:01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -497,11 +502,12 @@
           <t>LP1912</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -527,6 +533,7 @@
           <t>LP1912</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -555,6 +562,162 @@
       <c r="F4" t="inlineStr">
         <is>
           <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>22:52:50</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>23:06</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>14</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>22:52:50</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>23:07</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>22:52:50</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>23:15</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>23</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>22:52:50</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>23:49</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>57</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>22:52:50</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>23:51</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>59</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
         </is>
       </c>
     </row>
@@ -569,7 +732,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,23 +741,96 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>LÍNEA 141 - LP1912-215</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Línea</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Parada</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 28/12/2025 23:54:47</t>
-        </is>
-      </c>
+          <t>Última actualización: 29/12/2025 22:53:01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 0</t>
+          <t>Total filas: 3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>22:52:50</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>23:51</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>59</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -609,7 +845,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,23 +854,96 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>LÍNEA 141 - 6203-6173</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Línea</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Parada</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 28/12/2025 23:54:47</t>
-        </is>
-      </c>
+          <t>Última actualización: 29/12/2025 22:53:01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 0</t>
+          <t>Total filas: 3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>22:53:01</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🚌 141: 30/12 11:08 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 29/12/2025 22:53:01</t>
+          <t>Última actualización: 30/12/2025 08:08:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -718,6 +718,719 @@
       <c r="G9" t="inlineStr">
         <is>
           <t>29/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>08:10</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>14</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>15</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>16</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>20</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>08:33</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>26</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>08:34</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>27</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>28</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>35</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>36</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>08:46</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>39</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>46</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>54</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>56</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>63</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>63</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>09:13</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>66</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>70</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>74</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>76</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>95</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>95</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
         </is>
       </c>
     </row>
@@ -732,7 +1445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,7 +1493,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 29/12/2025 22:53:01</t>
+          <t>Última actualización: 30/12/2025 08:08:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -793,7 +1506,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -829,6 +1542,99 @@
         <v>59</v>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>16</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>54</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08:07:53</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>95</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -845,7 +1651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,7 +1699,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 29/12/2025 22:53:01</t>
+          <t>Última actualización: 30/12/2025 08:08:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -906,7 +1712,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -947,6 +1753,68 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>08:08:04</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>08:39</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>31</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>08:07:59</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>61</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 11:30 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:08:04</t>
+          <t>Última actualización: 30/12/2025 08:30:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 31</t>
+          <t>Total filas: 53</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1429,6 +1429,688 @@
         </is>
       </c>
       <c r="G32" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>08:34</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>4</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>08:39</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>9</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>12</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>13</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>08:48</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>18</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>23</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>31</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>33</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>09:04</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>34</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>40</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>09:13</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>43</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>47</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>51</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>52</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>53</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>62</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>63</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>72</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>73</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>82</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>93</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>10:06</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>96</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -1445,7 +2127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1493,7 +2175,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:08:04</t>
+          <t>Última actualización: 30/12/2025 08:30:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -1506,7 +2188,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -1635,6 +2317,68 @@
         <v>95</v>
       </c>
       <c r="G7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>31</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>08:30:26</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>72</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1651,7 +2395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1699,7 +2443,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:08:04</t>
+          <t>Última actualización: 30/12/2025 08:30:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -1712,7 +2456,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -1815,6 +2559,99 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08:30:37</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>08:38</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>08:30:32</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>39</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>08:30:37</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>93</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 11:45 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:30:37</t>
+          <t>Última actualización: 30/12/2025 08:45:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 53</t>
+          <t>Total filas: 74</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2111,6 +2111,657 @@
         </is>
       </c>
       <c r="G54" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>6</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>8</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>16</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>18</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>23</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>25</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>09:13</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>28</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>31</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>36</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>37</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>38</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>47</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>48</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>57</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>58</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>09:46</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>61</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>67</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>78</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>85</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>87</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>97</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -2127,7 +2778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2175,7 +2826,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:30:37</t>
+          <t>Última actualización: 30/12/2025 08:45:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -2188,7 +2839,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -2379,6 +3030,68 @@
         <v>72</v>
       </c>
       <c r="G9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>16</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>08:45:38</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>57</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2395,7 +3108,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2443,7 +3156,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:30:37</t>
+          <t>Última actualización: 30/12/2025 08:45:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -2456,7 +3169,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -2652,6 +3365,99 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>08:45:49</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>08:47</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>08:45:44</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>24</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>08:45:49</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>77</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 11:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:45:49</t>
+          <t>Última actualización: 30/12/2025 08:56:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 74</t>
+          <t>Total filas: 95</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2762,6 +2762,657 @@
         </is>
       </c>
       <c r="G75" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>6</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>09:04</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>8</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>12</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>09:11</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>15</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>09:13</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>17</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>21</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>25</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>27</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>09:24</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>28</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>36</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>37</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>09:35</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>39</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>46</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>48</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>56</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>57</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>10:04</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>68</v>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>10:11</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>75</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>76</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>86</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>91</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -2778,7 +3429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2826,7 +3477,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:45:49</t>
+          <t>Última actualización: 30/12/2025 08:56:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -2839,7 +3490,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -3092,6 +3743,99 @@
         <v>57</v>
       </c>
       <c r="G11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>46</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>08:56:16</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>91</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3108,7 +3852,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3156,7 +3900,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:45:49</t>
+          <t>Última actualización: 30/12/2025 08:56:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -3169,7 +3913,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -3458,6 +4202,68 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>08:56:21</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>13</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>67</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 12:48 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:56:26</t>
+          <t>Última actualización: 30/12/2025 09:48:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 95</t>
+          <t>Total filas: 114</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3413,6 +3413,595 @@
         </is>
       </c>
       <c r="G96" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>09:51</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>3</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>4</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>15</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>10:04</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>16</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>22</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>24</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>25</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>33</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>34</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>10:23</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>35</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>38</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>46</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>10:41</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>53</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>55</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>68</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>73</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>11:13</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>85</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>93</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>11:22</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>94</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -3429,7 +4018,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3477,7 +4066,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:56:26</t>
+          <t>Última actualización: 30/12/2025 09:48:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -3490,7 +4079,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -3836,6 +4425,68 @@
         <v>91</v>
       </c>
       <c r="G14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>38</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>09:48:46</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>73</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3852,7 +4503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3900,7 +4551,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 08:56:26</t>
+          <t>Última actualización: 30/12/2025 09:48:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -3913,7 +4564,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -4264,6 +4915,99 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>09:48:57</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>09:48:57</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>66</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>09:48:52</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>11:13</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>85</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 13:28 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 09:48:57</t>
+          <t>Última actualización: 30/12/2025 10:28:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 114</t>
+          <t>Total filas: 130</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -4002,6 +4002,502 @@
         </is>
       </c>
       <c r="G115" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>10:35</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>7</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>14</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>15</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>29</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>34</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>11:05</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>37</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>38</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>11:11</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>43</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>53</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>11:35</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>67</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr"/>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>74</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>84</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr"/>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>11:53</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>85</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>94</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>94</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>12:03</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>95</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -4013,491 +4509,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Línea</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Última actualización: 30/12/2025 09:48:57</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Total filas: 15</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>29/12/2025</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>22:52:50</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>23:51</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>59</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>08:07:53</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>08:23</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>16</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>08:07:53</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>09:01</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>54</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>08:07:53</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>09:42</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>95</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>08:30:26</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>09:01</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>31</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>08:30:26</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>09:42</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>72</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>08:45:38</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>09:01</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>16</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>08:45:38</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>09:42</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>57</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>08:56:16</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>09:02</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>6</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>08:56:16</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>09:42</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>46</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>08:56:16</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>10:27</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>91</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>09:48:46</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>10:26</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>38</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>30/12/2025</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>09:48:46</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>11:01</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>73</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4514,7 +4525,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173</t>
+          <t>LÍNEA 141 - LP1912-215</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -4551,7 +4562,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 09:48:57</t>
+          <t>Última actualización: 30/12/2025 10:28:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -4583,25 +4594,25 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22:53:01</t>
+          <t>22:52:50</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>23:08</t>
+          <t>23:51</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4614,25 +4625,25 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>08:08:04</t>
+          <t>08:07:53</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>08:39</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4645,25 +4656,25 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>08:07:59</t>
+          <t>08:07:53</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>09:08</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4676,25 +4687,25 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>08:30:37</t>
+          <t>08:07:53</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>08:38</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4707,25 +4718,25 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>08:30:32</t>
+          <t>08:30:26</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>09:09</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4738,25 +4749,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>08:30:37</t>
+          <t>08:30:26</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4769,25 +4780,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>08:45:49</t>
+          <t>08:45:38</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>08:47</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4800,25 +4811,25 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>08:45:44</t>
+          <t>08:45:38</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>09:09</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4831,25 +4842,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>08:45:49</t>
+          <t>08:56:16</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4862,25 +4873,25 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>08:56:21</t>
+          <t>08:56:16</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>09:09</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4893,25 +4904,25 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>08:56:26</t>
+          <t>08:56:16</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>10:27</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4924,25 +4935,25 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>09:48:57</t>
+          <t>09:48:46</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>10:26</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4955,25 +4966,25 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>09:48:57</t>
+          <t>09:48:46</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>10:54</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>LP1912</t>
         </is>
       </c>
     </row>
@@ -4986,6 +4997,522 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>10:28:23</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>34</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Línea</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Última actualización: 30/12/2025 10:28:34</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Total filas: 19</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>22:53:01</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>08:08:04</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>08:39</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>31</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>08:07:59</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>61</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08:30:37</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>08:38</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>08:30:32</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>39</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>08:30:37</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>93</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>08:45:49</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>08:47</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>08:45:44</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>24</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>08:45:49</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>77</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>08:56:21</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>13</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>08:56:26</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>67</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>09:48:57</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>09:48:57</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>66</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>09:48:52</t>
         </is>
       </c>
@@ -5005,6 +5532,99 @@
       <c r="G17" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>10:28:34</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>26</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>10:28:29</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>46</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>10:28:34</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>96</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🚌 141: 30/12 13:54 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 10:28:34</t>
+          <t>Última actualización: 30/12/2025 10:54:50</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 130</t>
+          <t>Total filas: 152</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -4498,6 +4498,688 @@
         </is>
       </c>
       <c r="G131" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>2</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>2</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr"/>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>7</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>10</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>12</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr"/>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>11:11</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>17</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr"/>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>27</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr"/>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>11:22</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>28</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr"/>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>32</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr"/>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>11:34</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>40</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr"/>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>11:36</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>42</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr"/>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>48</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>11:43</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>49</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>58</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>68</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>72</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>12:08</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>74</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>87</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>87</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>12:23</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>89</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>12:24</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>90</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>12:27</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>93</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -4514,7 +5196,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4562,7 +5244,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 10:28:34</t>
+          <t>Última actualización: 30/12/2025 10:54:50</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -4575,7 +5257,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -5014,6 +5696,37 @@
         <v>34</v>
       </c>
       <c r="G17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>10:54:39</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>7</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5030,7 +5743,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5078,7 +5791,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 10:28:34</t>
+          <t>Última actualización: 30/12/2025 10:54:50</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -5091,7 +5804,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -5628,6 +6341,68 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10:54:45</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>11:13</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>19</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>10:54:50</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>70</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 14:21 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 10:54:50</t>
+          <t>Última actualización: 30/12/2025 11:21:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 152</t>
+          <t>Total filas: 170</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -5180,6 +5180,564 @@
         </is>
       </c>
       <c r="G153" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr"/>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>11:25</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>5</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>6</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>6</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>11:34</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>14</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>21</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr"/>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>11:43</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>23</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr"/>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>32</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr"/>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>42</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr"/>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>44</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr"/>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>46</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr"/>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>60</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr"/>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>60</v>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr"/>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>74</v>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr"/>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>78</v>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr"/>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>88</v>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr"/>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>90</v>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr"/>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>94</v>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr"/>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>11:20:54</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>95</v>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -5244,7 +5802,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 10:54:50</t>
+          <t>Última actualización: 30/12/2025 11:21:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -5743,7 +6301,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5791,7 +6349,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 10:54:50</t>
+          <t>Última actualización: 30/12/2025 11:21:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -5804,7 +6362,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -6403,6 +6961,68 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>11:21:04</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>43</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>11:20:59</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>12:53</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>93</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 14:47 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:G188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:21:04</t>
+          <t>Última actualización: 30/12/2025 11:47:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 170</t>
+          <t>Total filas: 187</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -5738,6 +5738,533 @@
         </is>
       </c>
       <c r="G171" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr"/>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>4</v>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr"/>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>5</v>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr"/>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>11:56</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>9</v>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr"/>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>15</v>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr"/>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>19</v>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr"/>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>12:07</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>20</v>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr"/>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>12:13</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>26</v>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr"/>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>12:16</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>29</v>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr"/>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>33</v>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr"/>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>34</v>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr"/>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>47</v>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr"/>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>51</v>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr"/>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>61</v>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr"/>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>63</v>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr"/>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>68</v>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr"/>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>79</v>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr"/>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>13:16</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>89</v>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -5754,7 +6281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5802,7 +6329,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:21:04</t>
+          <t>Última actualización: 30/12/2025 11:47:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -5815,7 +6342,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -6285,6 +6812,37 @@
         <v>7</v>
       </c>
       <c r="G18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>11:47:33</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>4</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6301,7 +6859,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6349,7 +6907,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:21:04</t>
+          <t>Última actualización: 30/12/2025 11:47:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -6362,7 +6920,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -7023,6 +7581,68 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>11:47:44</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>17</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>11:47:39</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>12:53</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>66</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 14:57 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G188"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:47:44</t>
+          <t>Última actualización: 30/12/2025 11:57:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 187</t>
+          <t>Total filas: 202</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -6265,6 +6265,471 @@
         </is>
       </c>
       <c r="G188" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr"/>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>5</v>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr"/>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>12:07</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>10</v>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr"/>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>12:07</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>10</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr"/>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>24</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr"/>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>24</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr"/>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>38</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr"/>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>41</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr"/>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>51</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr"/>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>12:49</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>52</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr"/>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>53</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr"/>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>58</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr"/>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>70</v>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr"/>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>90</v>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr"/>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>90</v>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr"/>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>11:57:25</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>13:35</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>98</v>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -6329,7 +6794,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:47:44</t>
+          <t>Última actualización: 30/12/2025 11:57:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -6859,7 +7324,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6907,7 +7372,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:47:44</t>
+          <t>Última actualización: 30/12/2025 11:57:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -6920,7 +7385,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -7643,6 +8108,99 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>11:57:36</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>7</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>11:57:31</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>57</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>11:57:36</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>94</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 15:28 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G203"/>
+  <dimension ref="A1:G221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:57:36</t>
+          <t>Última actualización: 30/12/2025 12:28:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 202</t>
+          <t>Total filas: 220</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -6730,6 +6730,564 @@
         </is>
       </c>
       <c r="G203" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr"/>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>7</v>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr"/>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>9</v>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr"/>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>9</v>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr"/>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E207" t="n">
+        <v>10</v>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr"/>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>12:47</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E208" t="n">
+        <v>19</v>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr"/>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>22</v>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr"/>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>27</v>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr"/>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E211" t="n">
+        <v>34</v>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr"/>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>39</v>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr"/>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>13:08</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>40</v>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr"/>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>52</v>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr"/>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>59</v>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr"/>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>68</v>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr"/>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>68</v>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr"/>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>78</v>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr"/>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>89</v>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr"/>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>96</v>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr"/>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>12:28:02</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>14:05</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>97</v>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -6794,7 +7352,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:57:36</t>
+          <t>Última actualización: 30/12/2025 12:28:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -7324,7 +7882,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7372,7 +7930,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 11:57:36</t>
+          <t>Última actualización: 30/12/2025 12:28:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -7385,7 +7943,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -8201,6 +8759,68 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>12:28:08</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>26</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>12:28:13</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>63</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 15:47 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G221"/>
+  <dimension ref="A1:G236"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:28:13</t>
+          <t>Última actualización: 30/12/2025 12:47:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 220</t>
+          <t>Total filas: 235</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7288,6 +7288,471 @@
         </is>
       </c>
       <c r="G221" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr"/>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>9</v>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr"/>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>12:56</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>10</v>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr"/>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>16</v>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr"/>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>18</v>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr"/>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>20</v>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr"/>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>13:08</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>22</v>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr"/>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>13:19</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>33</v>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr"/>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E229" t="n">
+        <v>40</v>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr"/>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>13:34</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E230" t="n">
+        <v>48</v>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr"/>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E231" t="n">
+        <v>50</v>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr"/>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E232" t="n">
+        <v>60</v>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr"/>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E233" t="n">
+        <v>70</v>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr"/>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E234" t="n">
+        <v>78</v>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr"/>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E235" t="n">
+        <v>78</v>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr"/>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>12:46:58</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E236" t="n">
+        <v>95</v>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -7352,7 +7817,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:28:13</t>
+          <t>Última actualización: 30/12/2025 12:47:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -7882,7 +8347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7930,7 +8395,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:28:13</t>
+          <t>Última actualización: 30/12/2025 12:47:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -7943,7 +8408,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -8821,6 +9286,99 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>12:47:04</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>12:47:09</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>44</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>12:47:09</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>82</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 15:58 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G236"/>
+  <dimension ref="A1:G250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:47:09</t>
+          <t>Última actualización: 30/12/2025 12:58:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 235</t>
+          <t>Total filas: 249</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7753,6 +7753,440 @@
         </is>
       </c>
       <c r="G236" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr"/>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E237" t="n">
+        <v>6</v>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr"/>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E238" t="n">
+        <v>8</v>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr"/>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>13:08</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E239" t="n">
+        <v>10</v>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr"/>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>13:19</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E240" t="n">
+        <v>21</v>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr"/>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E241" t="n">
+        <v>28</v>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr"/>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E242" t="n">
+        <v>34</v>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr"/>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>13:34</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E243" t="n">
+        <v>36</v>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr"/>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E244" t="n">
+        <v>38</v>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr"/>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E245" t="n">
+        <v>48</v>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr"/>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E246" t="n">
+        <v>48</v>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr"/>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E247" t="n">
+        <v>58</v>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr"/>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E248" t="n">
+        <v>66</v>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr"/>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E249" t="n">
+        <v>69</v>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr"/>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>12:58:31</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E250" t="n">
+        <v>83</v>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -7817,7 +8251,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:47:09</t>
+          <t>Última actualización: 30/12/2025 12:58:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -8347,7 +8781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8395,7 +8829,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:47:09</t>
+          <t>Última actualización: 30/12/2025 12:58:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -8408,7 +8842,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -9379,6 +9813,68 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>12:58:42</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>32</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>12:58:42</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>71</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 16:37 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G250"/>
+  <dimension ref="A1:G261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:58:42</t>
+          <t>Última actualización: 30/12/2025 13:37:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 249</t>
+          <t>Total filas: 260</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -8187,6 +8187,347 @@
         </is>
       </c>
       <c r="G250" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr"/>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E251" t="n">
+        <v>9</v>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr"/>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E252" t="n">
+        <v>19</v>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr"/>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E253" t="n">
+        <v>27</v>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr"/>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E254" t="n">
+        <v>27</v>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr"/>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>14:06</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E255" t="n">
+        <v>29</v>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr"/>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E256" t="n">
+        <v>44</v>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr"/>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E257" t="n">
+        <v>67</v>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr"/>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E258" t="n">
+        <v>79</v>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr"/>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E259" t="n">
+        <v>81</v>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr"/>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E260" t="n">
+        <v>83</v>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr"/>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E261" t="n">
+        <v>88</v>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -8203,7 +8544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8251,7 +8592,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:58:42</t>
+          <t>Última actualización: 30/12/2025 13:37:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -8264,7 +8605,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -8765,6 +9106,37 @@
         <v>4</v>
       </c>
       <c r="G19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>13:37:39</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>81</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8781,7 +9153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8829,7 +9201,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 12:58:42</t>
+          <t>Última actualización: 30/12/2025 13:37:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -8842,7 +9214,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -9875,6 +10247,68 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>13:37:49</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>32</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>13:37:44</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>14:52</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>75</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 16:57 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G261"/>
+  <dimension ref="A1:G273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 13:37:49</t>
+          <t>Última actualización: 30/12/2025 13:57:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 260</t>
+          <t>Total filas: 272</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -8528,6 +8528,378 @@
         </is>
       </c>
       <c r="G261" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr"/>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E262" t="n">
+        <v>7</v>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr"/>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>14:05</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E263" t="n">
+        <v>8</v>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr"/>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E264" t="n">
+        <v>10</v>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr"/>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E265" t="n">
+        <v>20</v>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr"/>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E266" t="n">
+        <v>24</v>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr"/>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E267" t="n">
+        <v>48</v>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr"/>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>14:57</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E268" t="n">
+        <v>60</v>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr"/>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E269" t="n">
+        <v>61</v>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr"/>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E270" t="n">
+        <v>63</v>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr"/>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E271" t="n">
+        <v>68</v>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr"/>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E272" t="n">
+        <v>83</v>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G272" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr"/>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>15:23</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E273" t="n">
+        <v>86</v>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -8544,7 +8916,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8592,7 +8964,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 13:37:49</t>
+          <t>Última actualización: 30/12/2025 13:57:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -8605,7 +8977,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -9137,6 +9509,37 @@
         <v>81</v>
       </c>
       <c r="G20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>13:57:01</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>61</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9153,7 +9556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9201,7 +9604,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 13:37:49</t>
+          <t>Última actualización: 30/12/2025 13:57:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -9214,7 +9617,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -10309,6 +10712,99 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>13:57:11</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>12</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>13:57:06</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>56</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>13:57:11</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>97</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 17:25 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G273"/>
+  <dimension ref="A1:G286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 13:57:11</t>
+          <t>Última actualización: 30/12/2025 14:25:02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 272</t>
+          <t>Total filas: 285</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -8900,6 +8900,409 @@
         </is>
       </c>
       <c r="G273" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr"/>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E274" t="n">
+        <v>10</v>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr"/>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E275" t="n">
+        <v>20</v>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr"/>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E276" t="n">
+        <v>32</v>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr"/>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E277" t="n">
+        <v>34</v>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr"/>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E278" t="n">
+        <v>36</v>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr"/>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E279" t="n">
+        <v>41</v>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr"/>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E280" t="n">
+        <v>56</v>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr"/>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E281" t="n">
+        <v>57</v>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr"/>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E282" t="n">
+        <v>73</v>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr"/>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E283" t="n">
+        <v>81</v>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr"/>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E284" t="n">
+        <v>81</v>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr"/>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E285" t="n">
+        <v>96</v>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr"/>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E286" t="n">
+        <v>97</v>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -8916,7 +9319,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8964,7 +9367,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 13:57:11</t>
+          <t>Última actualización: 30/12/2025 14:25:02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -8977,7 +9380,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -9540,6 +9943,37 @@
         <v>61</v>
       </c>
       <c r="G21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>34</v>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9556,7 +9990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9604,7 +10038,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 13:57:11</t>
+          <t>Última actualización: 30/12/2025 14:25:02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -9617,7 +10051,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -10805,6 +11239,68 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>14:24:56</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>14:52</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>28</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>14:25:01</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>69</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 17:45 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G286"/>
+  <dimension ref="A1:G303"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:25:02</t>
+          <t>Última actualización: 30/12/2025 14:45:41</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 285</t>
+          <t>Total filas: 302</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -9303,6 +9303,533 @@
         </is>
       </c>
       <c r="G286" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr"/>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E287" t="n">
+        <v>11</v>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr"/>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E288" t="n">
+        <v>13</v>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr"/>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E289" t="n">
+        <v>15</v>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr"/>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E290" t="n">
+        <v>20</v>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr"/>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E291" t="n">
+        <v>20</v>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr"/>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>15:06</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E292" t="n">
+        <v>21</v>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr"/>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E293" t="n">
+        <v>35</v>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr"/>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E294" t="n">
+        <v>36</v>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr"/>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E295" t="n">
+        <v>47</v>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr"/>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>15:42</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E296" t="n">
+        <v>57</v>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr"/>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E297" t="n">
+        <v>60</v>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr"/>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>15:51</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E298" t="n">
+        <v>66</v>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr"/>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E299" t="n">
+        <v>76</v>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr"/>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>16:02</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E300" t="n">
+        <v>77</v>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr"/>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>16:04</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E301" t="n">
+        <v>79</v>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr"/>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E302" t="n">
+        <v>95</v>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr"/>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E303" t="n">
+        <v>96</v>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -9319,7 +9846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9367,7 +9894,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:25:02</t>
+          <t>Última actualización: 30/12/2025 14:45:41</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -9380,7 +9907,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -9974,6 +10501,68 @@
         <v>34</v>
       </c>
       <c r="G22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>13</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>14:45:30</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>95</v>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9990,7 +10579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10038,7 +10627,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:25:02</t>
+          <t>Última actualización: 30/12/2025 14:45:41</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -10051,7 +10640,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -11301,6 +11890,68 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>14:45:36</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>8</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>14:45:41</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>49</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 17:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G303"/>
+  <dimension ref="A1:G320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:45:41</t>
+          <t>Última actualización: 30/12/2025 14:56:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 302</t>
+          <t>Total filas: 319</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -9830,6 +9830,533 @@
         </is>
       </c>
       <c r="G303" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr"/>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E304" t="n">
+        <v>9</v>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr"/>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E305" t="n">
+        <v>9</v>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr"/>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>15:07</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E306" t="n">
+        <v>11</v>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr"/>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E307" t="n">
+        <v>24</v>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr"/>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E308" t="n">
+        <v>25</v>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr"/>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>15:27</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E309" t="n">
+        <v>31</v>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr"/>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E310" t="n">
+        <v>36</v>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr"/>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>15:42</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E311" t="n">
+        <v>46</v>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr"/>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E312" t="n">
+        <v>50</v>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr"/>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E313" t="n">
+        <v>58</v>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr"/>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E314" t="n">
+        <v>58</v>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr"/>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E315" t="n">
+        <v>65</v>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr"/>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>16:07</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E316" t="n">
+        <v>71</v>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr"/>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E317" t="n">
+        <v>84</v>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr"/>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E318" t="n">
+        <v>85</v>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr"/>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>16:26</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E319" t="n">
+        <v>90</v>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr"/>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>16:32</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E320" t="n">
+        <v>96</v>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G320" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -9846,7 +10373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9894,7 +10421,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:45:41</t>
+          <t>Última actualización: 30/12/2025 14:56:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -9907,7 +10434,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -10563,6 +11090,37 @@
         <v>95</v>
       </c>
       <c r="G24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14:56:19</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>84</v>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10579,7 +11137,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10627,7 +11185,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:45:41</t>
+          <t>Última actualización: 30/12/2025 14:56:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -10640,7 +11198,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -11952,6 +12510,37 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>14:56:30</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>38</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 18:35 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G320"/>
+  <dimension ref="A1:G339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:56:30</t>
+          <t>Última actualización: 30/12/2025 15:35:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 319</t>
+          <t>Total filas: 338</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -10357,6 +10357,595 @@
         </is>
       </c>
       <c r="G320" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr"/>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E321" t="n">
+        <v>3</v>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr"/>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E322" t="n">
+        <v>11</v>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr"/>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E323" t="n">
+        <v>19</v>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr"/>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E324" t="n">
+        <v>26</v>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr"/>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>16:03</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E325" t="n">
+        <v>28</v>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr"/>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E326" t="n">
+        <v>30</v>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr"/>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>16:11</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E327" t="n">
+        <v>36</v>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr"/>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E328" t="n">
+        <v>45</v>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr"/>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E329" t="n">
+        <v>46</v>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr"/>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E330" t="n">
+        <v>54</v>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr"/>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>16:37</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E331" t="n">
+        <v>62</v>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr"/>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E332" t="n">
+        <v>68</v>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr"/>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>16:45</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E333" t="n">
+        <v>70</v>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr"/>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>16:45</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E334" t="n">
+        <v>70</v>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr"/>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E335" t="n">
+        <v>73</v>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr"/>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E336" t="n">
+        <v>81</v>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr"/>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E337" t="n">
+        <v>82</v>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr"/>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E338" t="n">
+        <v>90</v>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr"/>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>17:11</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E339" t="n">
+        <v>96</v>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G339" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -10373,7 +10962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10421,7 +11010,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:56:30</t>
+          <t>Última actualización: 30/12/2025 15:35:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -10434,7 +11023,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -11121,6 +11710,68 @@
         <v>84</v>
       </c>
       <c r="G25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>45</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>15:35:11</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>90</v>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11137,7 +11788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11185,7 +11836,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 14:56:30</t>
+          <t>Última actualización: 30/12/2025 15:35:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -11198,7 +11849,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -12541,6 +13192,68 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>15:35:17</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>39</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>15:35:22</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>78</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 18:58 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G339"/>
+  <dimension ref="A1:G362"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 15:35:22</t>
+          <t>Última actualización: 30/12/2025 15:58:16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 338</t>
+          <t>Total filas: 361</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -10946,6 +10946,719 @@
         </is>
       </c>
       <c r="G339" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr"/>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E340" t="n">
+        <v>2</v>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr"/>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>16:03</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E341" t="n">
+        <v>5</v>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr"/>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E342" t="n">
+        <v>7</v>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr"/>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>16:11</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E343" t="n">
+        <v>13</v>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr"/>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E344" t="n">
+        <v>22</v>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr"/>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E345" t="n">
+        <v>23</v>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr"/>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>16:27</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E346" t="n">
+        <v>29</v>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr"/>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E347" t="n">
+        <v>31</v>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G347" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr"/>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>16:35</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E348" t="n">
+        <v>37</v>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G348" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr"/>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>16:37</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E349" t="n">
+        <v>39</v>
+      </c>
+      <c r="F349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G349" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr"/>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E350" t="n">
+        <v>45</v>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G350" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr"/>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E351" t="n">
+        <v>50</v>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G351" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr"/>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>16:51</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E352" t="n">
+        <v>53</v>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G352" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr"/>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E353" t="n">
+        <v>58</v>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr"/>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E354" t="n">
+        <v>59</v>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr"/>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E355" t="n">
+        <v>67</v>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr"/>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E356" t="n">
+        <v>67</v>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr"/>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E357" t="n">
+        <v>67</v>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr"/>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E358" t="n">
+        <v>83</v>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G358" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr"/>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E359" t="n">
+        <v>86</v>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G359" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr"/>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E360" t="n">
+        <v>91</v>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G360" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr"/>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>17:31</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E361" t="n">
+        <v>93</v>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G361" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr"/>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E362" t="n">
+        <v>97</v>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G362" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -10962,7 +11675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11010,7 +11723,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 15:35:22</t>
+          <t>Última actualización: 30/12/2025 15:58:16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -11023,7 +11736,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -11772,6 +12485,68 @@
         <v>90</v>
       </c>
       <c r="G27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>22</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>67</v>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11788,7 +12563,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11836,7 +12611,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 15:35:22</t>
+          <t>Última actualización: 30/12/2025 15:58:16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -11849,7 +12624,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -13254,6 +14029,99 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>15:58:11</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>16</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>15:58:16</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>55</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>15:58:16</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>83</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 19:22 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G362"/>
+  <dimension ref="A1:G385"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 15:58:16</t>
+          <t>Última actualización: 30/12/2025 16:22:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 361</t>
+          <t>Total filas: 384</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -11659,6 +11659,719 @@
         </is>
       </c>
       <c r="G362" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr"/>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>16:27</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E363" t="n">
+        <v>5</v>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr"/>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E364" t="n">
+        <v>7</v>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr"/>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>16:35</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E365" t="n">
+        <v>13</v>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr"/>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>16:37</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E366" t="n">
+        <v>15</v>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr"/>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E367" t="n">
+        <v>21</v>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr"/>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E368" t="n">
+        <v>26</v>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr"/>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E369" t="n">
+        <v>34</v>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G369" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr"/>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E370" t="n">
+        <v>35</v>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G370" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr"/>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>17:01</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E371" t="n">
+        <v>39</v>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G371" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr"/>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E372" t="n">
+        <v>43</v>
+      </c>
+      <c r="F372" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G372" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr"/>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E373" t="n">
+        <v>43</v>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G373" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr"/>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E374" t="n">
+        <v>43</v>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G374" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr"/>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E375" t="n">
+        <v>48</v>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G375" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr"/>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E376" t="n">
+        <v>59</v>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr"/>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E377" t="n">
+        <v>62</v>
+      </c>
+      <c r="F377" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G377" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr"/>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E378" t="n">
+        <v>67</v>
+      </c>
+      <c r="F378" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G378" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr"/>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>17:31</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E379" t="n">
+        <v>69</v>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G379" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr"/>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>17:33</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E380" t="n">
+        <v>71</v>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr"/>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E381" t="n">
+        <v>76</v>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr"/>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E382" t="n">
+        <v>79</v>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr"/>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E383" t="n">
+        <v>83</v>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr"/>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E384" t="n">
+        <v>90</v>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr"/>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>17:54</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E385" t="n">
+        <v>92</v>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G385" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -11675,7 +12388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11723,7 +12436,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 15:58:16</t>
+          <t>Última actualización: 30/12/2025 16:22:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -11736,7 +12449,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -12547,6 +13260,37 @@
         <v>67</v>
       </c>
       <c r="G29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>16:22:17</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>43</v>
+      </c>
+      <c r="G30" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12563,7 +13307,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12611,7 +13355,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 15:58:16</t>
+          <t>Última actualización: 30/12/2025 16:22:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -12624,7 +13368,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 50</t>
+          <t>Total filas: 52</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -14122,6 +14866,68 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>16:22:28</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>31</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>16:22:28</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>17:26</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>64</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 19:38 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G385"/>
+  <dimension ref="A1:G408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:22:28</t>
+          <t>Última actualización: 30/12/2025 16:38:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 384</t>
+          <t>Total filas: 407</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -12372,6 +12372,719 @@
         </is>
       </c>
       <c r="G385" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr"/>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E386" t="n">
+        <v>4</v>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G386" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr"/>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E387" t="n">
+        <v>10</v>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G387" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr"/>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E388" t="n">
+        <v>18</v>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G388" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr"/>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E389" t="n">
+        <v>19</v>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr"/>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E390" t="n">
+        <v>22</v>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr"/>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E391" t="n">
+        <v>26</v>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G391" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr"/>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E392" t="n">
+        <v>26</v>
+      </c>
+      <c r="F392" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr"/>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E393" t="n">
+        <v>32</v>
+      </c>
+      <c r="F393" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr"/>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E394" t="n">
+        <v>43</v>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr"/>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>17:22</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E395" t="n">
+        <v>44</v>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr"/>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E396" t="n">
+        <v>46</v>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr"/>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E397" t="n">
+        <v>50</v>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr"/>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>17:31</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E398" t="n">
+        <v>53</v>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr"/>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E399" t="n">
+        <v>59</v>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr"/>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E400" t="n">
+        <v>60</v>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr"/>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E401" t="n">
+        <v>62</v>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr"/>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E402" t="n">
+        <v>67</v>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr"/>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E403" t="n">
+        <v>72</v>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr"/>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E404" t="n">
+        <v>74</v>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr"/>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>17:56</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E405" t="n">
+        <v>78</v>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr"/>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E406" t="n">
+        <v>86</v>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G406" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr"/>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E407" t="n">
+        <v>88</v>
+      </c>
+      <c r="F407" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G407" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr"/>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>16:38:24</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>18:15</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E408" t="n">
+        <v>97</v>
+      </c>
+      <c r="F408" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G408" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -12436,7 +13149,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:22:28</t>
+          <t>Última actualización: 30/12/2025 16:38:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -13307,7 +14020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13355,7 +14068,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:22:28</t>
+          <t>Última actualización: 30/12/2025 16:38:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -13368,7 +14081,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 52</t>
+          <t>Total filas: 55</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -14928,6 +15641,99 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>16:38:35</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>15</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>16:38:35</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>17:26</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>48</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>16:38:30</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>86</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 19:49 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G408"/>
+  <dimension ref="A1:G431"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:38:35</t>
+          <t>Última actualización: 30/12/2025 16:49:20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 407</t>
+          <t>Total filas: 430</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -13085,6 +13085,719 @@
         </is>
       </c>
       <c r="G408" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr"/>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="E409" t="n">
+        <v>8</v>
+      </c>
+      <c r="F409" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G409" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr"/>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E410" t="n">
+        <v>9</v>
+      </c>
+      <c r="F410" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G410" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr"/>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>17:01</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E411" t="n">
+        <v>12</v>
+      </c>
+      <c r="F411" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G411" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr"/>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E412" t="n">
+        <v>16</v>
+      </c>
+      <c r="F412" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G412" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr"/>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E413" t="n">
+        <v>16</v>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G413" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr"/>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>17:11</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E414" t="n">
+        <v>22</v>
+      </c>
+      <c r="F414" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G414" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr"/>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>17:22</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E415" t="n">
+        <v>33</v>
+      </c>
+      <c r="F415" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G415" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr"/>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>17:23</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E416" t="n">
+        <v>34</v>
+      </c>
+      <c r="F416" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G416" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr"/>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>17:25</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E417" t="n">
+        <v>36</v>
+      </c>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G417" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr"/>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E418" t="n">
+        <v>40</v>
+      </c>
+      <c r="F418" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G418" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr"/>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E419" t="n">
+        <v>43</v>
+      </c>
+      <c r="F419" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G419" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr"/>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E420" t="n">
+        <v>46</v>
+      </c>
+      <c r="F420" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G420" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr"/>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E421" t="n">
+        <v>48</v>
+      </c>
+      <c r="F421" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G421" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr"/>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E422" t="n">
+        <v>50</v>
+      </c>
+      <c r="F422" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G422" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr"/>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E423" t="n">
+        <v>52</v>
+      </c>
+      <c r="F423" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G423" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr"/>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E424" t="n">
+        <v>62</v>
+      </c>
+      <c r="F424" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G424" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr"/>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>17:53</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E425" t="n">
+        <v>64</v>
+      </c>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G425" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr"/>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E426" t="n">
+        <v>76</v>
+      </c>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G426" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr"/>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>18:07</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E427" t="n">
+        <v>78</v>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G427" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr"/>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>18:14</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E428" t="n">
+        <v>85</v>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr"/>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>18:17</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E429" t="n">
+        <v>88</v>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G429" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr"/>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E430" t="n">
+        <v>93</v>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr"/>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>16:49:09</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E431" t="n">
+        <v>96</v>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G431" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -13149,7 +13862,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:38:35</t>
+          <t>Última actualización: 30/12/2025 16:49:20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -14020,7 +14733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14068,7 +14781,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:38:35</t>
+          <t>Última actualización: 30/12/2025 16:49:20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -14081,7 +14794,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 55</t>
+          <t>Total filas: 58</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -15734,6 +16447,99 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>16:49:19</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>4</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>16:49:19</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>41</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>16:49:14</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>75</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 19:59 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G431"/>
+  <dimension ref="A1:G454"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:49:20</t>
+          <t>Última actualización: 30/12/2025 16:59:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 430</t>
+          <t>Total filas: 453</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -13798,6 +13798,719 @@
         </is>
       </c>
       <c r="G431" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr"/>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>17:01</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E432" t="n">
+        <v>2</v>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G432" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr"/>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E433" t="n">
+        <v>6</v>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G433" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr"/>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E434" t="n">
+        <v>6</v>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G434" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr"/>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E435" t="n">
+        <v>11</v>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G435" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr"/>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E436" t="n">
+        <v>22</v>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr"/>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>17:22</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E437" t="n">
+        <v>23</v>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr"/>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E438" t="n">
+        <v>25</v>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr"/>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E439" t="n">
+        <v>30</v>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G439" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr"/>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>17:31</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E440" t="n">
+        <v>32</v>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G440" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr"/>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E441" t="n">
+        <v>36</v>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G441" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr"/>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E442" t="n">
+        <v>38</v>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G442" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr"/>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E443" t="n">
+        <v>39</v>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr"/>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E444" t="n">
+        <v>42</v>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G444" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr"/>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E445" t="n">
+        <v>46</v>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G445" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr"/>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E446" t="n">
+        <v>52</v>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr"/>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E447" t="n">
+        <v>53</v>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr"/>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>18:09</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E448" t="n">
+        <v>70</v>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr"/>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>18:12</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E449" t="n">
+        <v>73</v>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr"/>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>18:16</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E450" t="n">
+        <v>77</v>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr"/>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E451" t="n">
+        <v>82</v>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr"/>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E452" t="n">
+        <v>86</v>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr"/>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E453" t="n">
+        <v>89</v>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr"/>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E454" t="n">
+        <v>93</v>
+      </c>
+      <c r="F454" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G454" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -13814,7 +14527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13862,7 +14575,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:49:20</t>
+          <t>Última actualización: 30/12/2025 16:59:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -13875,7 +14588,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -14717,6 +15430,37 @@
         <v>43</v>
       </c>
       <c r="G30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>16:59:06</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>89</v>
+      </c>
+      <c r="G31" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -14733,7 +15477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14781,7 +15525,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:49:20</t>
+          <t>Última actualización: 30/12/2025 16:59:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -14794,7 +15538,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 58</t>
+          <t>Total filas: 60</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -16540,6 +17284,68 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>16:59:17</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>30</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>16:59:11</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>65</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 20:32 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G454"/>
+  <dimension ref="A1:G477"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:59:17</t>
+          <t>Última actualización: 30/12/2025 17:32:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 453</t>
+          <t>Total filas: 476</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -14511,6 +14511,719 @@
         </is>
       </c>
       <c r="G454" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr"/>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E455" t="n">
+        <v>3</v>
+      </c>
+      <c r="F455" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G455" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr"/>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E456" t="n">
+        <v>5</v>
+      </c>
+      <c r="F456" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G456" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr"/>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E457" t="n">
+        <v>6</v>
+      </c>
+      <c r="F457" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G457" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr"/>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E458" t="n">
+        <v>8</v>
+      </c>
+      <c r="F458" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G458" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr"/>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E459" t="n">
+        <v>13</v>
+      </c>
+      <c r="F459" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G459" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr"/>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E460" t="n">
+        <v>14</v>
+      </c>
+      <c r="F460" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G460" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr"/>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E461" t="n">
+        <v>20</v>
+      </c>
+      <c r="F461" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G461" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr"/>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E462" t="n">
+        <v>28</v>
+      </c>
+      <c r="F462" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G462" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr"/>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E463" t="n">
+        <v>32</v>
+      </c>
+      <c r="F463" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G463" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr"/>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E464" t="n">
+        <v>32</v>
+      </c>
+      <c r="F464" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G464" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr"/>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E465" t="n">
+        <v>38</v>
+      </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G465" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr"/>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>18:16</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E466" t="n">
+        <v>44</v>
+      </c>
+      <c r="F466" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G466" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr"/>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>18:16</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E467" t="n">
+        <v>44</v>
+      </c>
+      <c r="F467" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G467" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr"/>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E468" t="n">
+        <v>49</v>
+      </c>
+      <c r="F468" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G468" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr"/>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E469" t="n">
+        <v>52</v>
+      </c>
+      <c r="F469" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G469" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr"/>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E470" t="n">
+        <v>56</v>
+      </c>
+      <c r="F470" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G470" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr"/>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E471" t="n">
+        <v>60</v>
+      </c>
+      <c r="F471" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G471" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr"/>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E472" t="n">
+        <v>62</v>
+      </c>
+      <c r="F472" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G472" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr"/>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E473" t="n">
+        <v>68</v>
+      </c>
+      <c r="F473" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G473" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr"/>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E474" t="n">
+        <v>76</v>
+      </c>
+      <c r="F474" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G474" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr"/>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>18:56</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E475" t="n">
+        <v>84</v>
+      </c>
+      <c r="F475" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G475" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr"/>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E476" t="n">
+        <v>87</v>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr"/>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E477" t="n">
+        <v>92</v>
+      </c>
+      <c r="F477" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G477" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -14527,7 +15240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14575,7 +15288,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:59:17</t>
+          <t>Última actualización: 30/12/2025 17:32:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -14588,7 +15301,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -15461,6 +16174,37 @@
         <v>89</v>
       </c>
       <c r="G31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>17:32:27</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>56</v>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -15477,7 +16221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15525,7 +16269,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 16:59:17</t>
+          <t>Última actualización: 30/12/2025 17:32:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -15538,7 +16282,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 60</t>
+          <t>Total filas: 62</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -17346,6 +18090,68 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>17:32:32</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>32</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>17:32:38</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>80</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 20:51 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G477"/>
+  <dimension ref="A1:G497"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 17:32:38</t>
+          <t>Última actualización: 30/12/2025 17:51:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 476</t>
+          <t>Total filas: 496</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -15224,6 +15224,626 @@
         </is>
       </c>
       <c r="G477" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr"/>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E478" t="n">
+        <v>9</v>
+      </c>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G478" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr"/>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>18:01</t>
+        </is>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E479" t="n">
+        <v>10</v>
+      </c>
+      <c r="F479" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G479" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr"/>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E480" t="n">
+        <v>13</v>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G480" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr"/>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E481" t="n">
+        <v>15</v>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr"/>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>18:11</t>
+        </is>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E482" t="n">
+        <v>20</v>
+      </c>
+      <c r="F482" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G482" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr"/>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>18:16</t>
+        </is>
+      </c>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E483" t="n">
+        <v>25</v>
+      </c>
+      <c r="F483" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G483" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr"/>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>18:16</t>
+        </is>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E484" t="n">
+        <v>25</v>
+      </c>
+      <c r="F484" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G484" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr"/>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E485" t="n">
+        <v>30</v>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G485" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr"/>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E486" t="n">
+        <v>30</v>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr"/>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E487" t="n">
+        <v>34</v>
+      </c>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G487" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr"/>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E488" t="n">
+        <v>37</v>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G488" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr"/>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E489" t="n">
+        <v>41</v>
+      </c>
+      <c r="F489" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G489" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr"/>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>18:35</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E490" t="n">
+        <v>44</v>
+      </c>
+      <c r="F490" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G490" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr"/>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E491" t="n">
+        <v>49</v>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr"/>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E492" t="n">
+        <v>57</v>
+      </c>
+      <c r="F492" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G492" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr"/>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>18:56</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E493" t="n">
+        <v>65</v>
+      </c>
+      <c r="F493" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G493" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr"/>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E494" t="n">
+        <v>74</v>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G494" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr"/>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>19:08</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E495" t="n">
+        <v>77</v>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G495" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr"/>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E496" t="n">
+        <v>90</v>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G496" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr"/>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E497" t="n">
+        <v>90</v>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -15240,7 +15860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15288,7 +15908,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 17:32:38</t>
+          <t>Última actualización: 30/12/2025 17:51:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -15301,7 +15921,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 31</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -16205,6 +16825,37 @@
         <v>56</v>
       </c>
       <c r="G32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>17:51:04</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>37</v>
+      </c>
+      <c r="G33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -16221,7 +16872,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16269,7 +16920,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 17:32:38</t>
+          <t>Última actualización: 30/12/2025 17:51:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -16282,7 +16933,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 62</t>
+          <t>Total filas: 65</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -18152,6 +18803,99 @@
         </is>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>17:51:10</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>13</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>17:51:15</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>61</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>17:51:15</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>74</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 21:20 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 17:51:15</t>
+          <t>Última actualización: 30/12/2025 18:20:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -15908,7 +15908,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 17:51:15</t>
+          <t>Última actualización: 30/12/2025 18:20:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -16920,7 +16920,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 17:51:15</t>
+          <t>Última actualización: 30/12/2025 18:20:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 30/12 21:38 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G497"/>
+  <dimension ref="A1:G519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:20:11</t>
+          <t>Última actualización: 30/12/2025 18:38:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 496</t>
+          <t>Total filas: 518</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -15844,6 +15844,688 @@
         </is>
       </c>
       <c r="G497" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr"/>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E498" t="n">
+        <v>2</v>
+      </c>
+      <c r="F498" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G498" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr"/>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E499" t="n">
+        <v>3</v>
+      </c>
+      <c r="F499" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr"/>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E500" t="n">
+        <v>10</v>
+      </c>
+      <c r="F500" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G500" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr"/>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>18:51</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E501" t="n">
+        <v>13</v>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G501" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr"/>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E502" t="n">
+        <v>14</v>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr"/>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>18:56</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E503" t="n">
+        <v>18</v>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr"/>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>19:01</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E504" t="n">
+        <v>23</v>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G504" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr"/>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E505" t="n">
+        <v>27</v>
+      </c>
+      <c r="F505" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G505" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr"/>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>19:08</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E506" t="n">
+        <v>30</v>
+      </c>
+      <c r="F506" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G506" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr"/>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>19:12</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E507" t="n">
+        <v>34</v>
+      </c>
+      <c r="F507" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G507" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr"/>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E508" t="n">
+        <v>43</v>
+      </c>
+      <c r="F508" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G508" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr"/>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E509" t="n">
+        <v>50</v>
+      </c>
+      <c r="F509" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G509" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr"/>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E510" t="n">
+        <v>62</v>
+      </c>
+      <c r="F510" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G510" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr"/>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E511" t="n">
+        <v>63</v>
+      </c>
+      <c r="F511" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G511" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr"/>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E512" t="n">
+        <v>72</v>
+      </c>
+      <c r="F512" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G512" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr"/>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E513" t="n">
+        <v>73</v>
+      </c>
+      <c r="F513" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G513" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr"/>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E514" t="n">
+        <v>73</v>
+      </c>
+      <c r="F514" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G514" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr"/>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E515" t="n">
+        <v>81</v>
+      </c>
+      <c r="F515" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G515" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr"/>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E516" t="n">
+        <v>83</v>
+      </c>
+      <c r="F516" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G516" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr"/>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>20:08</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E517" t="n">
+        <v>90</v>
+      </c>
+      <c r="F517" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G517" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr"/>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E518" t="n">
+        <v>93</v>
+      </c>
+      <c r="F518" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G518" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr"/>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>20:13</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E519" t="n">
+        <v>95</v>
+      </c>
+      <c r="F519" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G519" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -15860,7 +16542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15908,7 +16590,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:20:11</t>
+          <t>Última actualización: 30/12/2025 18:38:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -15921,7 +16603,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -16856,6 +17538,37 @@
         <v>37</v>
       </c>
       <c r="G33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>18:38:08</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>62</v>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -16872,7 +17585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16920,7 +17633,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:20:11</t>
+          <t>Última actualización: 30/12/2025 18:38:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -16933,7 +17646,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 65</t>
+          <t>Total filas: 68</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -18896,6 +19609,99 @@
         </is>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>18:38:18</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>14</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>18:38:18</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>26</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>18:38:13</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>76</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 21:50 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G519"/>
+  <dimension ref="A1:G543"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:38:18</t>
+          <t>Última actualización: 30/12/2025 18:50:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 518</t>
+          <t>Total filas: 542</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -16526,6 +16526,750 @@
         </is>
       </c>
       <c r="G519" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr"/>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E520" t="n">
+        <v>2</v>
+      </c>
+      <c r="F520" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G520" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr"/>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>18:56</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E521" t="n">
+        <v>6</v>
+      </c>
+      <c r="F521" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G521" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr"/>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E522" t="n">
+        <v>10</v>
+      </c>
+      <c r="F522" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G522" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr"/>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E523" t="n">
+        <v>14</v>
+      </c>
+      <c r="F523" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr"/>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>19:08</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E524" t="n">
+        <v>18</v>
+      </c>
+      <c r="F524" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G524" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr"/>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>19:12</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E525" t="n">
+        <v>22</v>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G525" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr"/>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E526" t="n">
+        <v>30</v>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G526" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr"/>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E527" t="n">
+        <v>31</v>
+      </c>
+      <c r="F527" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G527" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr"/>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E528" t="n">
+        <v>31</v>
+      </c>
+      <c r="F528" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G528" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr"/>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E529" t="n">
+        <v>38</v>
+      </c>
+      <c r="F529" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G529" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr"/>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E530" t="n">
+        <v>49</v>
+      </c>
+      <c r="F530" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G530" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr"/>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E531" t="n">
+        <v>50</v>
+      </c>
+      <c r="F531" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G531" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr"/>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E532" t="n">
+        <v>60</v>
+      </c>
+      <c r="F532" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G532" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr"/>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E533" t="n">
+        <v>60</v>
+      </c>
+      <c r="F533" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G533" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr"/>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E534" t="n">
+        <v>61</v>
+      </c>
+      <c r="F534" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G534" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr"/>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E535" t="n">
+        <v>69</v>
+      </c>
+      <c r="F535" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G535" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr"/>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E536" t="n">
+        <v>70</v>
+      </c>
+      <c r="F536" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G536" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr"/>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="D537" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E537" t="n">
+        <v>77</v>
+      </c>
+      <c r="F537" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G537" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr"/>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>20:09</t>
+        </is>
+      </c>
+      <c r="D538" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E538" t="n">
+        <v>79</v>
+      </c>
+      <c r="F538" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G538" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr"/>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="D539" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E539" t="n">
+        <v>80</v>
+      </c>
+      <c r="F539" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G539" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr"/>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="D540" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E540" t="n">
+        <v>82</v>
+      </c>
+      <c r="F540" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G540" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr"/>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="D541" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E541" t="n">
+        <v>90</v>
+      </c>
+      <c r="F541" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G541" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr"/>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="D542" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E542" t="n">
+        <v>92</v>
+      </c>
+      <c r="F542" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G542" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr"/>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E543" t="n">
+        <v>93</v>
+      </c>
+      <c r="F543" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G543" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -16542,7 +17286,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16590,7 +17334,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:38:18</t>
+          <t>Última actualización: 30/12/2025 18:50:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -16603,7 +17347,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -17569,6 +18313,68 @@
         <v>62</v>
       </c>
       <c r="G34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>49</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>18:50:44</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>93</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -17585,7 +18391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17633,7 +18439,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:38:18</t>
+          <t>Última actualización: 30/12/2025 18:50:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -17646,7 +18452,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 68</t>
+          <t>Total filas: 70</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -19702,6 +20508,68 @@
         </is>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>18:50:55</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>13</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>18:50:50</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>63</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 22:20 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G543"/>
+  <dimension ref="A1:G565"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:50:55</t>
+          <t>Última actualización: 30/12/2025 19:20:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 542</t>
+          <t>Total filas: 564</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -17270,6 +17270,688 @@
         </is>
       </c>
       <c r="G543" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr"/>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E544" t="n">
+        <v>2</v>
+      </c>
+      <c r="F544" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G544" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr"/>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E545" t="n">
+        <v>2</v>
+      </c>
+      <c r="F545" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G545" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr"/>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E546" t="n">
+        <v>9</v>
+      </c>
+      <c r="F546" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G546" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr"/>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E547" t="n">
+        <v>11</v>
+      </c>
+      <c r="F547" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G547" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr"/>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E548" t="n">
+        <v>20</v>
+      </c>
+      <c r="F548" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G548" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr"/>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E549" t="n">
+        <v>21</v>
+      </c>
+      <c r="F549" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G549" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr"/>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E550" t="n">
+        <v>21</v>
+      </c>
+      <c r="F550" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G550" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr"/>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E551" t="n">
+        <v>31</v>
+      </c>
+      <c r="F551" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G551" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr"/>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E552" t="n">
+        <v>31</v>
+      </c>
+      <c r="F552" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G552" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr"/>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E553" t="n">
+        <v>32</v>
+      </c>
+      <c r="F553" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G553" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr"/>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E554" t="n">
+        <v>40</v>
+      </c>
+      <c r="F554" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G554" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr"/>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E555" t="n">
+        <v>41</v>
+      </c>
+      <c r="F555" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G555" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr"/>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>20:08</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E556" t="n">
+        <v>48</v>
+      </c>
+      <c r="F556" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G556" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr"/>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E557" t="n">
+        <v>50</v>
+      </c>
+      <c r="F557" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G557" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr"/>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E558" t="n">
+        <v>51</v>
+      </c>
+      <c r="F558" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G558" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr"/>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>20:13</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E559" t="n">
+        <v>53</v>
+      </c>
+      <c r="F559" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G559" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr"/>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E560" t="n">
+        <v>61</v>
+      </c>
+      <c r="F560" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G560" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr"/>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E561" t="n">
+        <v>63</v>
+      </c>
+      <c r="F561" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G561" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr"/>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E562" t="n">
+        <v>64</v>
+      </c>
+      <c r="F562" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G562" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr"/>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>20:53</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E563" t="n">
+        <v>93</v>
+      </c>
+      <c r="F563" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G563" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr"/>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E564" t="n">
+        <v>96</v>
+      </c>
+      <c r="F564" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G564" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr"/>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E565" t="n">
+        <v>97</v>
+      </c>
+      <c r="F565" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G565" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -17286,7 +17968,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17334,7 +18016,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:50:55</t>
+          <t>Última actualización: 30/12/2025 19:20:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -17347,7 +18029,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -18375,6 +19057,68 @@
         <v>93</v>
       </c>
       <c r="G36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>20</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>19:20:18</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>64</v>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -18391,7 +19135,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18439,7 +19183,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 18:50:55</t>
+          <t>Última actualización: 30/12/2025 19:20:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -18452,7 +19196,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 70</t>
+          <t>Total filas: 71</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -20570,6 +21314,37 @@
         </is>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>19:20:23</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>34</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 22:40 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G565"/>
+  <dimension ref="A1:G582"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:20:29</t>
+          <t>Última actualización: 30/12/2025 19:40:33</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 564</t>
+          <t>Total filas: 581</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -17952,6 +17952,533 @@
         </is>
       </c>
       <c r="G565" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr"/>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E566" t="n">
+        <v>10</v>
+      </c>
+      <c r="F566" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G566" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr"/>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E567" t="n">
+        <v>10</v>
+      </c>
+      <c r="F567" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G567" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr"/>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E568" t="n">
+        <v>11</v>
+      </c>
+      <c r="F568" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G568" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr"/>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E569" t="n">
+        <v>19</v>
+      </c>
+      <c r="F569" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G569" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr"/>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E570" t="n">
+        <v>20</v>
+      </c>
+      <c r="F570" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G570" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr"/>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E571" t="n">
+        <v>21</v>
+      </c>
+      <c r="F571" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G571" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr"/>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E572" t="n">
+        <v>27</v>
+      </c>
+      <c r="F572" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G572" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr"/>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>20:09</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E573" t="n">
+        <v>29</v>
+      </c>
+      <c r="F573" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G573" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr"/>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E574" t="n">
+        <v>30</v>
+      </c>
+      <c r="F574" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G574" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr"/>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E575" t="n">
+        <v>32</v>
+      </c>
+      <c r="F575" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G575" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr"/>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E576" t="n">
+        <v>41</v>
+      </c>
+      <c r="F576" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G576" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr"/>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E577" t="n">
+        <v>42</v>
+      </c>
+      <c r="F577" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G577" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr"/>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E578" t="n">
+        <v>43</v>
+      </c>
+      <c r="F578" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G578" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr"/>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E579" t="n">
+        <v>72</v>
+      </c>
+      <c r="F579" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G579" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr"/>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E580" t="n">
+        <v>77</v>
+      </c>
+      <c r="F580" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G580" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr"/>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E581" t="n">
+        <v>84</v>
+      </c>
+      <c r="F581" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G581" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr"/>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E582" t="n">
+        <v>87</v>
+      </c>
+      <c r="F582" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G582" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -17968,7 +18495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18016,7 +18543,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:20:29</t>
+          <t>Última actualización: 30/12/2025 19:40:33</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -18029,7 +18556,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -19119,6 +19646,68 @@
         <v>64</v>
       </c>
       <c r="G38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>43</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>19:40:22</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>87</v>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -19135,7 +19724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19183,7 +19772,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:20:29</t>
+          <t>Última actualización: 30/12/2025 19:40:33</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -19196,7 +19785,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 71</t>
+          <t>Total filas: 72</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -21345,6 +21934,37 @@
         </is>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>19:40:28</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>14</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 22:52 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G582"/>
+  <dimension ref="A1:G599"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:40:33</t>
+          <t>Última actualización: 30/12/2025 19:52:46</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 581</t>
+          <t>Total filas: 598</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -18479,6 +18479,533 @@
         </is>
       </c>
       <c r="G582" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr"/>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="D583" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E583" t="n">
+        <v>7</v>
+      </c>
+      <c r="F583" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G583" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr"/>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E584" t="n">
+        <v>8</v>
+      </c>
+      <c r="F584" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G584" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr"/>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E585" t="n">
+        <v>8</v>
+      </c>
+      <c r="F585" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G585" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr"/>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E586" t="n">
+        <v>15</v>
+      </c>
+      <c r="F586" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G586" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr"/>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>20:09</t>
+        </is>
+      </c>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E587" t="n">
+        <v>17</v>
+      </c>
+      <c r="F587" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G587" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr"/>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="E588" t="n">
+        <v>18</v>
+      </c>
+      <c r="F588" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G588" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr"/>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>20:19</t>
+        </is>
+      </c>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E589" t="n">
+        <v>27</v>
+      </c>
+      <c r="F589" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G589" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr"/>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E590" t="n">
+        <v>28</v>
+      </c>
+      <c r="F590" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G590" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr"/>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E591" t="n">
+        <v>30</v>
+      </c>
+      <c r="F591" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G591" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr"/>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E592" t="n">
+        <v>30</v>
+      </c>
+      <c r="F592" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G592" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr"/>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="D593" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E593" t="n">
+        <v>31</v>
+      </c>
+      <c r="F593" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G593" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr"/>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E594" t="n">
+        <v>60</v>
+      </c>
+      <c r="F594" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G594" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr"/>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="D595" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E595" t="n">
+        <v>65</v>
+      </c>
+      <c r="F595" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G595" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr"/>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="D596" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E596" t="n">
+        <v>72</v>
+      </c>
+      <c r="F596" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G596" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr"/>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E597" t="n">
+        <v>75</v>
+      </c>
+      <c r="F597" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G597" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr"/>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="D598" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E598" t="n">
+        <v>88</v>
+      </c>
+      <c r="F598" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G598" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr"/>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E599" t="n">
+        <v>90</v>
+      </c>
+      <c r="F599" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G599" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -18495,7 +19022,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18543,7 +19070,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:40:33</t>
+          <t>Última actualización: 30/12/2025 19:52:46</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -18556,7 +19083,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -19708,6 +20235,68 @@
         <v>87</v>
       </c>
       <c r="G40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>31</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>19:52:35</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>75</v>
+      </c>
+      <c r="G42" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -19724,7 +20313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19772,7 +20361,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:40:33</t>
+          <t>Última actualización: 30/12/2025 19:52:46</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -19785,7 +20374,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 72</t>
+          <t>Total filas: 73</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -21965,6 +22554,37 @@
         </is>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>19:52:40</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>96</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 23:19 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G599"/>
+  <dimension ref="A1:G616"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:52:46</t>
+          <t>Última actualización: 30/12/2025 20:19:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 598</t>
+          <t>Total filas: 615</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -19006,6 +19006,533 @@
         </is>
       </c>
       <c r="G599" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr"/>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E600" t="n">
+        <v>3</v>
+      </c>
+      <c r="F600" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G600" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr"/>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E601" t="n">
+        <v>3</v>
+      </c>
+      <c r="F601" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G601" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr"/>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E602" t="n">
+        <v>4</v>
+      </c>
+      <c r="F602" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G602" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr"/>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>20:34</t>
+        </is>
+      </c>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E603" t="n">
+        <v>15</v>
+      </c>
+      <c r="F603" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G603" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr"/>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E604" t="n">
+        <v>26</v>
+      </c>
+      <c r="F604" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G604" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr"/>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>20:46</t>
+        </is>
+      </c>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E605" t="n">
+        <v>27</v>
+      </c>
+      <c r="F605" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G605" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr"/>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E606" t="n">
+        <v>33</v>
+      </c>
+      <c r="F606" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G606" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr"/>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E607" t="n">
+        <v>38</v>
+      </c>
+      <c r="F607" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G607" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr"/>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E608" t="n">
+        <v>45</v>
+      </c>
+      <c r="F608" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G608" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr"/>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E609" t="n">
+        <v>48</v>
+      </c>
+      <c r="F609" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G609" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr"/>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E610" t="n">
+        <v>61</v>
+      </c>
+      <c r="F610" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G610" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr"/>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E611" t="n">
+        <v>63</v>
+      </c>
+      <c r="F611" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G611" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr"/>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="D612" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E612" t="n">
+        <v>73</v>
+      </c>
+      <c r="F612" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G612" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr"/>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E613" t="n">
+        <v>78</v>
+      </c>
+      <c r="F613" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G613" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr"/>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>21:42</t>
+        </is>
+      </c>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E614" t="n">
+        <v>83</v>
+      </c>
+      <c r="F614" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G614" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr"/>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E615" t="n">
+        <v>88</v>
+      </c>
+      <c r="F615" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G615" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr"/>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>21:51</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E616" t="n">
+        <v>92</v>
+      </c>
+      <c r="F616" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G616" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -19022,7 +19549,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19070,7 +19597,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:52:46</t>
+          <t>Última actualización: 30/12/2025 20:19:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -19083,7 +19610,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -20297,6 +20824,99 @@
         <v>75</v>
       </c>
       <c r="G42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>4</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>48</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>20:19:41</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>88</v>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -20313,7 +20933,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20361,7 +20981,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 19:52:46</t>
+          <t>Última actualización: 30/12/2025 20:19:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -20374,7 +20994,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 73</t>
+          <t>Total filas: 74</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -22585,6 +23205,37 @@
         </is>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>20:19:46</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>70</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 23:35 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G616"/>
+  <dimension ref="A1:G631"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:19:52</t>
+          <t>Última actualización: 30/12/2025 20:35:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 615</t>
+          <t>Total filas: 630</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -19533,6 +19533,471 @@
         </is>
       </c>
       <c r="G616" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr"/>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>20:46</t>
+        </is>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E617" t="n">
+        <v>11</v>
+      </c>
+      <c r="F617" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G617" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr"/>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E618" t="n">
+        <v>17</v>
+      </c>
+      <c r="F618" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G618" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr"/>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E619" t="n">
+        <v>22</v>
+      </c>
+      <c r="F619" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G619" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr"/>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>21:01</t>
+        </is>
+      </c>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E620" t="n">
+        <v>26</v>
+      </c>
+      <c r="F620" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G620" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr"/>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E621" t="n">
+        <v>29</v>
+      </c>
+      <c r="F621" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G621" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr"/>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="D622" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E622" t="n">
+        <v>32</v>
+      </c>
+      <c r="F622" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G622" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr"/>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>21:17</t>
+        </is>
+      </c>
+      <c r="D623" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E623" t="n">
+        <v>42</v>
+      </c>
+      <c r="F623" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G623" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr"/>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="D624" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E624" t="n">
+        <v>45</v>
+      </c>
+      <c r="F624" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G624" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr"/>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="D625" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E625" t="n">
+        <v>47</v>
+      </c>
+      <c r="F625" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G625" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr"/>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>21:31</t>
+        </is>
+      </c>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E626" t="n">
+        <v>56</v>
+      </c>
+      <c r="F626" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G626" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr"/>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E627" t="n">
+        <v>57</v>
+      </c>
+      <c r="F627" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G627" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr"/>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E628" t="n">
+        <v>62</v>
+      </c>
+      <c r="F628" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G628" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr"/>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="D629" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E629" t="n">
+        <v>72</v>
+      </c>
+      <c r="F629" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G629" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr"/>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>21:51</t>
+        </is>
+      </c>
+      <c r="D630" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E630" t="n">
+        <v>76</v>
+      </c>
+      <c r="F630" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G630" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr"/>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>22:07</t>
+        </is>
+      </c>
+      <c r="D631" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E631" t="n">
+        <v>92</v>
+      </c>
+      <c r="F631" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G631" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -19549,7 +20014,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19597,7 +20062,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:19:52</t>
+          <t>Última actualización: 30/12/2025 20:35:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -19610,7 +20075,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -20917,6 +21382,68 @@
         <v>88</v>
       </c>
       <c r="G45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>32</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>20:35:43</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>72</v>
+      </c>
+      <c r="G47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -20933,7 +21460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20981,7 +21508,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:19:52</t>
+          <t>Última actualización: 30/12/2025 20:35:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -20994,7 +21521,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 74</t>
+          <t>Total filas: 76</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -23236,6 +23763,68 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>20:35:48</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>53</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>20:35:54</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>89</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 23:47 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G631"/>
+  <dimension ref="A1:G647"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:35:54</t>
+          <t>Última actualización: 30/12/2025 20:47:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 630</t>
+          <t>Total filas: 646</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -19998,6 +19998,502 @@
         </is>
       </c>
       <c r="G631" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr"/>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="D632" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E632" t="n">
+        <v>5</v>
+      </c>
+      <c r="F632" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G632" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr"/>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="D633" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E633" t="n">
+        <v>10</v>
+      </c>
+      <c r="F633" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G633" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr"/>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E634" t="n">
+        <v>17</v>
+      </c>
+      <c r="F634" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G634" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr"/>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="D635" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E635" t="n">
+        <v>20</v>
+      </c>
+      <c r="F635" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G635" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr"/>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>21:14</t>
+        </is>
+      </c>
+      <c r="D636" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E636" t="n">
+        <v>27</v>
+      </c>
+      <c r="F636" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G636" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr"/>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>21:18</t>
+        </is>
+      </c>
+      <c r="D637" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E637" t="n">
+        <v>31</v>
+      </c>
+      <c r="F637" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G637" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr"/>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E638" t="n">
+        <v>34</v>
+      </c>
+      <c r="F638" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G638" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr"/>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E639" t="n">
+        <v>36</v>
+      </c>
+      <c r="F639" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G639" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr"/>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E640" t="n">
+        <v>45</v>
+      </c>
+      <c r="F640" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G640" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr"/>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E641" t="n">
+        <v>45</v>
+      </c>
+      <c r="F641" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G641" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr"/>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E642" t="n">
+        <v>51</v>
+      </c>
+      <c r="F642" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G642" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr"/>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E643" t="n">
+        <v>60</v>
+      </c>
+      <c r="F643" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G643" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr"/>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>21:51</t>
+        </is>
+      </c>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E644" t="n">
+        <v>64</v>
+      </c>
+      <c r="F644" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G644" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr"/>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E645" t="n">
+        <v>81</v>
+      </c>
+      <c r="F645" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G645" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr"/>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>22:23</t>
+        </is>
+      </c>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E646" t="n">
+        <v>96</v>
+      </c>
+      <c r="F646" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G646" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr"/>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>22:25</t>
+        </is>
+      </c>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E647" t="n">
+        <v>98</v>
+      </c>
+      <c r="F647" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G647" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -20014,7 +20510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20062,7 +20558,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:35:54</t>
+          <t>Última actualización: 30/12/2025 20:47:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -20075,7 +20571,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -21444,6 +21940,68 @@
         <v>72</v>
       </c>
       <c r="G47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>20</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>20:47:31</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>60</v>
+      </c>
+      <c r="G49" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -21460,7 +22018,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21508,7 +22066,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:35:54</t>
+          <t>Última actualización: 30/12/2025 20:47:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -21521,7 +22079,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 76</t>
+          <t>Total filas: 79</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -23825,6 +24383,99 @@
         </is>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>20:47:37</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>42</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>20:47:42</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>77</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>20:47:42</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>93</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 30/12 23:58 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G647"/>
+  <dimension ref="A1:G663"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:47:42</t>
+          <t>Última actualización: 30/12/2025 20:58:21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 646</t>
+          <t>Total filas: 662</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -20494,6 +20494,502 @@
         </is>
       </c>
       <c r="G647" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr"/>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E648" t="n">
+        <v>6</v>
+      </c>
+      <c r="F648" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G648" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr"/>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="D649" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E649" t="n">
+        <v>9</v>
+      </c>
+      <c r="F649" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G649" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr"/>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>21:18</t>
+        </is>
+      </c>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E650" t="n">
+        <v>20</v>
+      </c>
+      <c r="F650" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G650" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr"/>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E651" t="n">
+        <v>23</v>
+      </c>
+      <c r="F651" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G651" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr"/>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E652" t="n">
+        <v>25</v>
+      </c>
+      <c r="F652" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G652" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr"/>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>21:25</t>
+        </is>
+      </c>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E653" t="n">
+        <v>27</v>
+      </c>
+      <c r="F653" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G653" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr"/>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E654" t="n">
+        <v>34</v>
+      </c>
+      <c r="F654" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G654" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr"/>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E655" t="n">
+        <v>34</v>
+      </c>
+      <c r="F655" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G655" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr"/>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="D656" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E656" t="n">
+        <v>40</v>
+      </c>
+      <c r="F656" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G656" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr"/>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E657" t="n">
+        <v>49</v>
+      </c>
+      <c r="F657" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G657" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr"/>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="D658" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E658" t="n">
+        <v>49</v>
+      </c>
+      <c r="F658" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G658" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr"/>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>21:51</t>
+        </is>
+      </c>
+      <c r="D659" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E659" t="n">
+        <v>53</v>
+      </c>
+      <c r="F659" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G659" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr"/>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="D660" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E660" t="n">
+        <v>70</v>
+      </c>
+      <c r="F660" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G660" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr"/>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>22:23</t>
+        </is>
+      </c>
+      <c r="D661" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E661" t="n">
+        <v>85</v>
+      </c>
+      <c r="F661" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G661" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr"/>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>22:25</t>
+        </is>
+      </c>
+      <c r="D662" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E662" t="n">
+        <v>87</v>
+      </c>
+      <c r="F662" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G662" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr"/>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="D663" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E663" t="n">
+        <v>90</v>
+      </c>
+      <c r="F663" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G663" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -20510,7 +21006,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20558,7 +21054,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:47:42</t>
+          <t>Última actualización: 30/12/2025 20:58:21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -20571,7 +21067,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -22002,6 +22498,68 @@
         <v>60</v>
       </c>
       <c r="G49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>9</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>49</v>
+      </c>
+      <c r="G51" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -22018,7 +22576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22066,7 +22624,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:47:42</t>
+          <t>Última actualización: 30/12/2025 20:58:21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22079,7 +22637,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 79</t>
+          <t>Total filas: 82</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -24476,6 +25034,99 @@
         </is>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>20:58:15</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>31</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>20:58:20</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>67</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>20:58:20</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>83</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 02:10 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G663"/>
+  <dimension ref="A1:G667"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:58:21</t>
+          <t>Última actualización: 30/12/2025 23:10:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 662</t>
+          <t>Total filas: 666</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -20990,6 +20990,130 @@
         </is>
       </c>
       <c r="G663" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr"/>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>23:10:30</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>00:36</t>
+        </is>
+      </c>
+      <c r="D664" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E664" t="n">
+        <v>86</v>
+      </c>
+      <c r="F664" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G664" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr"/>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>23:10:30</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>00:42</t>
+        </is>
+      </c>
+      <c r="D665" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="E665" t="n">
+        <v>92</v>
+      </c>
+      <c r="F665" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G665" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr"/>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>23:10:30</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>23:13</t>
+        </is>
+      </c>
+      <c r="D666" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E666" t="n">
+        <v>3</v>
+      </c>
+      <c r="F666" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G666" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr"/>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>23:10:30</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="D667" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E667" t="n">
+        <v>36</v>
+      </c>
+      <c r="F667" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G667" t="inlineStr">
         <is>
           <t>30/12/2025</t>
         </is>
@@ -21006,7 +21130,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21054,7 +21178,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:58:21</t>
+          <t>Última actualización: 30/12/2025 23:10:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -21067,7 +21191,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 50</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -22560,6 +22684,37 @@
         <v>49</v>
       </c>
       <c r="G51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>30/12/2025</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>23:10:30</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>00:42</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>92</v>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -22624,7 +22779,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 20:58:21</t>
+          <t>Última actualización: 30/12/2025 23:10:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 03:44 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 23:10:40</t>
+          <t>Última actualización: 31/12/2025 00:44:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -21178,7 +21178,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 23:10:40</t>
+          <t>Última actualización: 31/12/2025 00:44:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22779,7 +22779,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 30/12/2025 23:10:40</t>
+          <t>Última actualización: 31/12/2025 00:44:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 04:26 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 00:44:42</t>
+          <t>Última actualización: 31/12/2025 01:26:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -21178,7 +21178,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 00:44:42</t>
+          <t>Última actualización: 31/12/2025 01:26:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22779,7 +22779,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 00:44:42</t>
+          <t>Última actualización: 31/12/2025 01:26:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 04:57 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G667"/>
+  <dimension ref="A1:G668"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 01:26:17</t>
+          <t>Última actualización: 31/12/2025 01:57:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 666</t>
+          <t>Total filas: 667</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21116,6 +21116,37 @@
       <c r="G667" t="inlineStr">
         <is>
           <t>30/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr"/>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>01:57:03</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>03:08</t>
+        </is>
+      </c>
+      <c r="D668" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E668" t="n">
+        <v>71</v>
+      </c>
+      <c r="F668" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G668" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
         </is>
       </c>
     </row>
@@ -21178,7 +21209,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 01:26:17</t>
+          <t>Última actualización: 31/12/2025 01:57:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22779,7 +22810,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 01:26:17</t>
+          <t>Última actualización: 31/12/2025 01:57:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 05:29 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 01:57:13</t>
+          <t>Última actualización: 31/12/2025 02:29:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -21209,7 +21209,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 01:57:13</t>
+          <t>Última actualización: 31/12/2025 02:29:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22810,7 +22810,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 01:57:13</t>
+          <t>Última actualización: 31/12/2025 02:29:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 05:50 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 02:29:44</t>
+          <t>Última actualización: 31/12/2025 02:50:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -21209,7 +21209,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 02:29:44</t>
+          <t>Última actualización: 31/12/2025 02:50:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22810,7 +22810,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 02:29:44</t>
+          <t>Última actualización: 31/12/2025 02:50:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 06:00 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 02:50:11</t>
+          <t>Última actualización: 31/12/2025 03:00:32</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -21209,7 +21209,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 02:50:11</t>
+          <t>Última actualización: 31/12/2025 03:00:32</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22810,7 +22810,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 02:50:11</t>
+          <t>Última actualización: 31/12/2025 03:00:32</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 06:47 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G668"/>
+  <dimension ref="A1:G669"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 03:00:32</t>
+          <t>Última actualización: 31/12/2025 03:47:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 667</t>
+          <t>Total filas: 668</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21145,6 +21145,37 @@
         </is>
       </c>
       <c r="G668" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr"/>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>03:47:18</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>05:11</t>
+        </is>
+      </c>
+      <c r="D669" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E669" t="n">
+        <v>84</v>
+      </c>
+      <c r="F669" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G669" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21209,7 +21240,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 03:00:32</t>
+          <t>Última actualización: 31/12/2025 03:47:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22810,7 +22841,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 03:00:32</t>
+          <t>Última actualización: 31/12/2025 03:47:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 07:03 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G669"/>
+  <dimension ref="A1:G670"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 03:47:28</t>
+          <t>Última actualización: 31/12/2025 04:03:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 668</t>
+          <t>Total filas: 669</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21176,6 +21176,37 @@
         </is>
       </c>
       <c r="G669" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr"/>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>04:03:43</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>05:11</t>
+        </is>
+      </c>
+      <c r="D670" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E670" t="n">
+        <v>68</v>
+      </c>
+      <c r="F670" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G670" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21240,7 +21271,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 03:47:28</t>
+          <t>Última actualización: 31/12/2025 04:03:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22841,7 +22872,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 03:47:28</t>
+          <t>Última actualización: 31/12/2025 04:03:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 07:33 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G670"/>
+  <dimension ref="A1:G671"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:03:54</t>
+          <t>Última actualización: 31/12/2025 04:33:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 669</t>
+          <t>Total filas: 670</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21207,6 +21207,37 @@
         </is>
       </c>
       <c r="G670" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr"/>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>04:33:18</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>05:11</t>
+        </is>
+      </c>
+      <c r="D671" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E671" t="n">
+        <v>38</v>
+      </c>
+      <c r="F671" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G671" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21271,7 +21302,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:03:54</t>
+          <t>Última actualización: 31/12/2025 04:33:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22872,7 +22903,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:03:54</t>
+          <t>Última actualización: 31/12/2025 04:33:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 07:49 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G671"/>
+  <dimension ref="A1:G672"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:33:29</t>
+          <t>Última actualización: 31/12/2025 04:49:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 670</t>
+          <t>Total filas: 671</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21238,6 +21238,37 @@
         </is>
       </c>
       <c r="G671" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr"/>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>04:49:26</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>05:11</t>
+        </is>
+      </c>
+      <c r="D672" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E672" t="n">
+        <v>22</v>
+      </c>
+      <c r="F672" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G672" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21302,7 +21333,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:33:29</t>
+          <t>Última actualización: 31/12/2025 04:49:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22903,7 +22934,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:33:29</t>
+          <t>Última actualización: 31/12/2025 04:49:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 08:00 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G672"/>
+  <dimension ref="A1:G675"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:49:36</t>
+          <t>Última actualización: 31/12/2025 05:00:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 671</t>
+          <t>Total filas: 674</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21269,6 +21269,99 @@
         </is>
       </c>
       <c r="G672" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr"/>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>05:00:11</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>05:12</t>
+        </is>
+      </c>
+      <c r="D673" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E673" t="n">
+        <v>12</v>
+      </c>
+      <c r="F673" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G673" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr"/>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>05:00:11</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="D674" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E674" t="n">
+        <v>52</v>
+      </c>
+      <c r="F674" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G674" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr"/>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>05:00:11</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>06:01</t>
+        </is>
+      </c>
+      <c r="D675" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E675" t="n">
+        <v>61</v>
+      </c>
+      <c r="F675" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G675" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21333,7 +21426,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:49:36</t>
+          <t>Última actualización: 31/12/2025 05:00:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -22934,7 +23027,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 04:49:36</t>
+          <t>Última actualización: 31/12/2025 05:00:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 08:40 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G675"/>
+  <dimension ref="A1:G680"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:00:22</t>
+          <t>Última actualización: 31/12/2025 05:40:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 674</t>
+          <t>Total filas: 679</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21362,6 +21362,161 @@
         </is>
       </c>
       <c r="G675" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr"/>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>05:40:08</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>05:52</t>
+        </is>
+      </c>
+      <c r="D676" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E676" t="n">
+        <v>12</v>
+      </c>
+      <c r="F676" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G676" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr"/>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>05:40:08</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>06:02</t>
+        </is>
+      </c>
+      <c r="D677" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E677" t="n">
+        <v>22</v>
+      </c>
+      <c r="F677" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G677" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr"/>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>05:40:08</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>06:32</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E678" t="n">
+        <v>52</v>
+      </c>
+      <c r="F678" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G678" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr"/>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>05:40:08</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>06:55</t>
+        </is>
+      </c>
+      <c r="D679" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E679" t="n">
+        <v>75</v>
+      </c>
+      <c r="F679" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G679" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr"/>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>05:40:08</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>07:02</t>
+        </is>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E680" t="n">
+        <v>82</v>
+      </c>
+      <c r="F680" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G680" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21426,7 +21581,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:00:22</t>
+          <t>Última actualización: 31/12/2025 05:40:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23027,7 +23182,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:00:22</t>
+          <t>Última actualización: 31/12/2025 05:40:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 08:59 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G680"/>
+  <dimension ref="A1:G685"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:40:19</t>
+          <t>Última actualización: 31/12/2025 05:59:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 679</t>
+          <t>Total filas: 684</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21517,6 +21517,161 @@
         </is>
       </c>
       <c r="G680" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr"/>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>05:59:11</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E681" t="n">
+        <v>32</v>
+      </c>
+      <c r="F681" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G681" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr"/>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>05:59:11</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E682" t="n">
+        <v>55</v>
+      </c>
+      <c r="F682" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G682" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr"/>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>05:59:11</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>07:01</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E683" t="n">
+        <v>62</v>
+      </c>
+      <c r="F683" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G683" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr"/>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>05:59:11</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E684" t="n">
+        <v>82</v>
+      </c>
+      <c r="F684" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G684" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr"/>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>05:59:11</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="D685" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E685" t="n">
+        <v>97</v>
+      </c>
+      <c r="F685" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G685" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21533,7 +21688,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21581,7 +21736,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:40:19</t>
+          <t>Última actualización: 31/12/2025 05:59:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -21594,7 +21749,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 52</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -23118,6 +23273,37 @@
         <v>92</v>
       </c>
       <c r="G52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>05:59:11</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>82</v>
+      </c>
+      <c r="G53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -23182,7 +23368,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:40:19</t>
+          <t>Última actualización: 31/12/2025 05:59:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 09:34 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G685"/>
+  <dimension ref="A1:G693"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:59:22</t>
+          <t>Última actualización: 31/12/2025 06:34:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 684</t>
+          <t>Total filas: 692</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21672,6 +21672,254 @@
         </is>
       </c>
       <c r="G685" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr"/>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>06:34:29</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="D686" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E686" t="n">
+        <v>20</v>
+      </c>
+      <c r="F686" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G686" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr"/>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>06:34:29</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>07:01</t>
+        </is>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E687" t="n">
+        <v>27</v>
+      </c>
+      <c r="F687" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G687" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr"/>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>06:34:29</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>07:13</t>
+        </is>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E688" t="n">
+        <v>39</v>
+      </c>
+      <c r="F688" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G688" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr"/>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>06:34:29</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E689" t="n">
+        <v>42</v>
+      </c>
+      <c r="F689" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G689" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr"/>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>06:34:29</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E690" t="n">
+        <v>77</v>
+      </c>
+      <c r="F690" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G690" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr"/>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>06:34:29</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>08:02</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E691" t="n">
+        <v>88</v>
+      </c>
+      <c r="F691" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G691" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr"/>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>06:34:29</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E692" t="n">
+        <v>89</v>
+      </c>
+      <c r="F692" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G692" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr"/>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>06:34:29</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E693" t="n">
+        <v>99</v>
+      </c>
+      <c r="F693" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G693" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21736,7 +21984,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:59:22</t>
+          <t>Última actualización: 31/12/2025 06:34:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23320,7 +23568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23368,7 +23616,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 05:59:22</t>
+          <t>Última actualización: 31/12/2025 06:34:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23381,7 +23629,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 82</t>
+          <t>Total filas: 83</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -25871,6 +26119,37 @@
         </is>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>06:34:39</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>53</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 09:51 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G693"/>
+  <dimension ref="A1:G703"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 06:34:40</t>
+          <t>Última actualización: 31/12/2025 06:51:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 692</t>
+          <t>Total filas: 702</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21920,6 +21920,316 @@
         </is>
       </c>
       <c r="G693" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr"/>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>06:54</t>
+        </is>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E694" t="n">
+        <v>3</v>
+      </c>
+      <c r="F694" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G694" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr"/>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>07:01</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E695" t="n">
+        <v>10</v>
+      </c>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G695" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr"/>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E696" t="n">
+        <v>25</v>
+      </c>
+      <c r="F696" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G696" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr"/>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>07:29</t>
+        </is>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E697" t="n">
+        <v>38</v>
+      </c>
+      <c r="F697" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G697" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr"/>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E698" t="n">
+        <v>46</v>
+      </c>
+      <c r="F698" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G698" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr"/>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E699" t="n">
+        <v>60</v>
+      </c>
+      <c r="F699" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G699" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr"/>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E700" t="n">
+        <v>72</v>
+      </c>
+      <c r="F700" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G700" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr"/>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E701" t="n">
+        <v>72</v>
+      </c>
+      <c r="F701" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G701" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr"/>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>08:14</t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E702" t="n">
+        <v>83</v>
+      </c>
+      <c r="F702" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G702" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr"/>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>06:51:26</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>08:30</t>
+        </is>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E703" t="n">
+        <v>99</v>
+      </c>
+      <c r="F703" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G703" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -21984,7 +22294,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 06:34:40</t>
+          <t>Última actualización: 31/12/2025 06:51:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23568,7 +23878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23616,7 +23926,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 06:34:40</t>
+          <t>Última actualización: 31/12/2025 06:51:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23629,7 +23939,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 83</t>
+          <t>Total filas: 85</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -26150,6 +26460,68 @@
         </is>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>06:51:36</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>36</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>06:51:36</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>08:10</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>79</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 10:23 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G703"/>
+  <dimension ref="A1:G716"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 06:51:36</t>
+          <t>Última actualización: 31/12/2025 07:23:07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 702</t>
+          <t>Total filas: 715</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -22230,6 +22230,409 @@
         </is>
       </c>
       <c r="G703" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr"/>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>07:28</t>
+        </is>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E704" t="n">
+        <v>6</v>
+      </c>
+      <c r="F704" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G704" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr"/>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>07:33</t>
+        </is>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E705" t="n">
+        <v>11</v>
+      </c>
+      <c r="F705" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G705" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr"/>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E706" t="n">
+        <v>13</v>
+      </c>
+      <c r="F706" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G706" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr"/>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E707" t="n">
+        <v>14</v>
+      </c>
+      <c r="F707" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr"/>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E708" t="n">
+        <v>29</v>
+      </c>
+      <c r="F708" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G708" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr"/>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>07:58</t>
+        </is>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E709" t="n">
+        <v>36</v>
+      </c>
+      <c r="F709" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G709" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr"/>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E710" t="n">
+        <v>39</v>
+      </c>
+      <c r="F710" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G710" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr"/>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E711" t="n">
+        <v>41</v>
+      </c>
+      <c r="F711" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G711" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr"/>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E712" t="n">
+        <v>51</v>
+      </c>
+      <c r="F712" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G712" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr"/>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>08:15</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E713" t="n">
+        <v>53</v>
+      </c>
+      <c r="F713" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G713" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr"/>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E714" t="n">
+        <v>67</v>
+      </c>
+      <c r="F714" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G714" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr"/>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E715" t="n">
+        <v>81</v>
+      </c>
+      <c r="F715" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G715" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr"/>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>07:22:56</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>08:49</t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E716" t="n">
+        <v>87</v>
+      </c>
+      <c r="F716" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G716" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -22294,7 +22697,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 06:51:36</t>
+          <t>Última actualización: 31/12/2025 07:23:07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23878,7 +24281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23926,7 +24329,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 06:51:36</t>
+          <t>Última actualización: 31/12/2025 07:23:07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23939,7 +24342,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 85</t>
+          <t>Total filas: 88</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -26522,6 +26925,99 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>07:23:06</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>07:30</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>7</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>07:23:06</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>08:10</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>47</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>07:23:01</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>08:36</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>73</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 10:46 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G716"/>
+  <dimension ref="A1:G730"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:23:07</t>
+          <t>Última actualización: 31/12/2025 07:46:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 715</t>
+          <t>Total filas: 729</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -22633,6 +22633,440 @@
         </is>
       </c>
       <c r="G716" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr"/>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E717" t="n">
+        <v>5</v>
+      </c>
+      <c r="F717" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G717" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr"/>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>07:58</t>
+        </is>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E718" t="n">
+        <v>12</v>
+      </c>
+      <c r="F718" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G718" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr"/>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E719" t="n">
+        <v>15</v>
+      </c>
+      <c r="F719" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G719" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr"/>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E720" t="n">
+        <v>17</v>
+      </c>
+      <c r="F720" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G720" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr"/>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E721" t="n">
+        <v>25</v>
+      </c>
+      <c r="F721" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G721" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr"/>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>08:14</t>
+        </is>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E722" t="n">
+        <v>28</v>
+      </c>
+      <c r="F722" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G722" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr"/>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>08:15</t>
+        </is>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E723" t="n">
+        <v>29</v>
+      </c>
+      <c r="F723" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G723" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr"/>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E724" t="n">
+        <v>43</v>
+      </c>
+      <c r="F724" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G724" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr"/>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E725" t="n">
+        <v>58</v>
+      </c>
+      <c r="F725" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G725" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr"/>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>08:49</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E726" t="n">
+        <v>63</v>
+      </c>
+      <c r="F726" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G726" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr"/>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="D727" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E727" t="n">
+        <v>76</v>
+      </c>
+      <c r="F727" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G727" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr"/>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="D728" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E728" t="n">
+        <v>76</v>
+      </c>
+      <c r="F728" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G728" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr"/>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>09:14</t>
+        </is>
+      </c>
+      <c r="D729" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E729" t="n">
+        <v>88</v>
+      </c>
+      <c r="F729" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G729" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr"/>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>07:46:38</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E730" t="n">
+        <v>90</v>
+      </c>
+      <c r="F730" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G730" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -22697,7 +23131,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:23:07</t>
+          <t>Última actualización: 31/12/2025 07:46:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -24281,7 +24715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24329,7 +24763,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:23:07</t>
+          <t>Última actualización: 31/12/2025 07:46:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -24342,7 +24776,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 88</t>
+          <t>Total filas: 89</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -27018,6 +27452,37 @@
         </is>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>07:46:49</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>08:09</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>23</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 10:57 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G730"/>
+  <dimension ref="A1:G743"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:46:49</t>
+          <t>Última actualización: 31/12/2025 07:57:39</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 729</t>
+          <t>Total filas: 742</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -23067,6 +23067,409 @@
         </is>
       </c>
       <c r="G730" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr"/>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="D731" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E731" t="n">
+        <v>4</v>
+      </c>
+      <c r="F731" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G731" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr"/>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="D732" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E732" t="n">
+        <v>6</v>
+      </c>
+      <c r="F732" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G732" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr"/>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="D733" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E733" t="n">
+        <v>14</v>
+      </c>
+      <c r="F733" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G733" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr"/>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>08:14</t>
+        </is>
+      </c>
+      <c r="D734" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E734" t="n">
+        <v>17</v>
+      </c>
+      <c r="F734" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G734" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr"/>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="D735" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E735" t="n">
+        <v>32</v>
+      </c>
+      <c r="F735" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G735" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr"/>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="D736" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E736" t="n">
+        <v>47</v>
+      </c>
+      <c r="F736" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G736" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr"/>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="D737" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E737" t="n">
+        <v>54</v>
+      </c>
+      <c r="F737" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G737" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr"/>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="D738" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E738" t="n">
+        <v>65</v>
+      </c>
+      <c r="F738" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G738" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr"/>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="D739" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E739" t="n">
+        <v>66</v>
+      </c>
+      <c r="F739" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G739" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr"/>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>09:14</t>
+        </is>
+      </c>
+      <c r="D740" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E740" t="n">
+        <v>77</v>
+      </c>
+      <c r="F740" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G740" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr"/>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D741" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E741" t="n">
+        <v>80</v>
+      </c>
+      <c r="F741" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G741" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr"/>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>09:27</t>
+        </is>
+      </c>
+      <c r="D742" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E742" t="n">
+        <v>90</v>
+      </c>
+      <c r="F742" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G742" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr"/>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="D743" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E743" t="n">
+        <v>96</v>
+      </c>
+      <c r="F743" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G743" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -23083,7 +23486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23131,7 +23534,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:46:49</t>
+          <t>Última actualización: 31/12/2025 07:57:39</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23144,7 +23547,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 52</t>
+          <t>Total filas: 53</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -24699,6 +25102,37 @@
         <v>82</v>
       </c>
       <c r="G53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>07:57:29</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>09:27</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>90</v>
+      </c>
+      <c r="G54" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -24715,7 +25149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24763,7 +25197,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:46:49</t>
+          <t>Última actualización: 31/12/2025 07:57:39</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -24776,7 +25210,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 89</t>
+          <t>Total filas: 90</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -27483,6 +27917,37 @@
         </is>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>07:57:39</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>08:10</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>13</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 11:23 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G743"/>
+  <dimension ref="A1:G759"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:57:39</t>
+          <t>Última actualización: 31/12/2025 08:23:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 742</t>
+          <t>Total filas: 758</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -23470,6 +23470,502 @@
         </is>
       </c>
       <c r="G743" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr"/>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="D744" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E744" t="n">
+        <v>6</v>
+      </c>
+      <c r="F744" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G744" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr"/>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="D745" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E745" t="n">
+        <v>21</v>
+      </c>
+      <c r="F745" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G745" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr"/>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>08:50</t>
+        </is>
+      </c>
+      <c r="D746" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E746" t="n">
+        <v>27</v>
+      </c>
+      <c r="F746" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G746" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr"/>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="D747" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E747" t="n">
+        <v>28</v>
+      </c>
+      <c r="F747" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G747" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr"/>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="D748" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E748" t="n">
+        <v>39</v>
+      </c>
+      <c r="F748" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G748" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr"/>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="D749" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E749" t="n">
+        <v>40</v>
+      </c>
+      <c r="F749" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G749" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr"/>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="D750" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E750" t="n">
+        <v>45</v>
+      </c>
+      <c r="F750" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G750" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr"/>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>09:14</t>
+        </is>
+      </c>
+      <c r="D751" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E751" t="n">
+        <v>51</v>
+      </c>
+      <c r="F751" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G751" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr"/>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E752" t="n">
+        <v>54</v>
+      </c>
+      <c r="F752" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G752" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr"/>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="D753" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E753" t="n">
+        <v>58</v>
+      </c>
+      <c r="F753" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G753" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr"/>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>09:27</t>
+        </is>
+      </c>
+      <c r="D754" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E754" t="n">
+        <v>64</v>
+      </c>
+      <c r="F754" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G754" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr"/>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>09:36</t>
+        </is>
+      </c>
+      <c r="D755" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E755" t="n">
+        <v>73</v>
+      </c>
+      <c r="F755" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G755" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr"/>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>09:39</t>
+        </is>
+      </c>
+      <c r="D756" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E756" t="n">
+        <v>76</v>
+      </c>
+      <c r="F756" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G756" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr"/>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="D757" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E757" t="n">
+        <v>81</v>
+      </c>
+      <c r="F757" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G757" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr"/>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>09:51</t>
+        </is>
+      </c>
+      <c r="D758" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E758" t="n">
+        <v>88</v>
+      </c>
+      <c r="F758" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G758" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr"/>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="D759" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E759" t="n">
+        <v>95</v>
+      </c>
+      <c r="F759" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G759" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -23486,7 +23982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23534,7 +24030,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:57:39</t>
+          <t>Última actualización: 31/12/2025 08:23:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -23547,7 +24043,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 53</t>
+          <t>Total filas: 54</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -25133,6 +25629,37 @@
         <v>90</v>
       </c>
       <c r="G54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>08:23:26</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>09:27</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>64</v>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -25197,7 +25724,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 07:57:39</t>
+          <t>Última actualización: 31/12/2025 08:23:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 31/12 11:40 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G759"/>
+  <dimension ref="A1:G776"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:23:37</t>
+          <t>Última actualización: 31/12/2025 08:40:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 758</t>
+          <t>Total filas: 775</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -23966,6 +23966,533 @@
         </is>
       </c>
       <c r="G759" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr"/>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="D760" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E760" t="n">
+        <v>4</v>
+      </c>
+      <c r="F760" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G760" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr"/>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="D761" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E761" t="n">
+        <v>12</v>
+      </c>
+      <c r="F761" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G761" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr"/>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="D762" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E762" t="n">
+        <v>23</v>
+      </c>
+      <c r="F762" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G762" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr"/>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="D763" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E763" t="n">
+        <v>24</v>
+      </c>
+      <c r="F763" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G763" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr"/>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="D764" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E764" t="n">
+        <v>27</v>
+      </c>
+      <c r="F764" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G764" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr"/>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="D765" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E765" t="n">
+        <v>29</v>
+      </c>
+      <c r="F765" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G765" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr"/>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>09:14</t>
+        </is>
+      </c>
+      <c r="D766" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E766" t="n">
+        <v>35</v>
+      </c>
+      <c r="F766" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G766" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr"/>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="D767" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E767" t="n">
+        <v>42</v>
+      </c>
+      <c r="F767" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G767" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr"/>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>09:26</t>
+        </is>
+      </c>
+      <c r="D768" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E768" t="n">
+        <v>47</v>
+      </c>
+      <c r="F768" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G768" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr"/>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>09:35</t>
+        </is>
+      </c>
+      <c r="D769" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E769" t="n">
+        <v>56</v>
+      </c>
+      <c r="F769" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G769" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr"/>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="D770" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E770" t="n">
+        <v>65</v>
+      </c>
+      <c r="F770" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G770" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr"/>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>09:51</t>
+        </is>
+      </c>
+      <c r="D771" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E771" t="n">
+        <v>72</v>
+      </c>
+      <c r="F771" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G771" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr"/>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="D772" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E772" t="n">
+        <v>74</v>
+      </c>
+      <c r="F772" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G772" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr"/>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="D773" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E773" t="n">
+        <v>83</v>
+      </c>
+      <c r="F773" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G773" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr"/>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>10:04</t>
+        </is>
+      </c>
+      <c r="D774" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E774" t="n">
+        <v>85</v>
+      </c>
+      <c r="F774" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G774" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr"/>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>10:14</t>
+        </is>
+      </c>
+      <c r="D775" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E775" t="n">
+        <v>95</v>
+      </c>
+      <c r="F775" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G775" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr"/>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>10:18</t>
+        </is>
+      </c>
+      <c r="D776" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E776" t="n">
+        <v>99</v>
+      </c>
+      <c r="F776" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G776" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -23982,7 +24509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24030,7 +24557,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:23:37</t>
+          <t>Última actualización: 31/12/2025 08:40:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -24043,7 +24570,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 54</t>
+          <t>Total filas: 56</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -25660,6 +26187,68 @@
         <v>64</v>
       </c>
       <c r="G55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>09:26</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>47</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>08:39:58</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>83</v>
+      </c>
+      <c r="G57" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -25676,7 +26265,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25724,7 +26313,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:23:37</t>
+          <t>Última actualización: 31/12/2025 08:40:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -25737,7 +26326,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 90</t>
+          <t>Total filas: 91</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -28475,6 +29064,37 @@
         </is>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>08:40:03</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>10:09</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>89</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 11:50 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G776"/>
+  <dimension ref="A1:G792"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:40:09</t>
+          <t>Última actualización: 31/12/2025 08:50:45</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 775</t>
+          <t>Total filas: 791</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -24493,6 +24493,502 @@
         </is>
       </c>
       <c r="G776" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr"/>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="D777" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E777" t="n">
+        <v>12</v>
+      </c>
+      <c r="F777" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G777" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr"/>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="D778" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E778" t="n">
+        <v>13</v>
+      </c>
+      <c r="F778" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G778" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr"/>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="D779" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E779" t="n">
+        <v>18</v>
+      </c>
+      <c r="F779" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G779" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr"/>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>09:14</t>
+        </is>
+      </c>
+      <c r="D780" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E780" t="n">
+        <v>24</v>
+      </c>
+      <c r="F780" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G780" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr"/>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="D781" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E781" t="n">
+        <v>26</v>
+      </c>
+      <c r="F781" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G781" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr"/>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D782" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E782" t="n">
+        <v>27</v>
+      </c>
+      <c r="F782" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G782" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr"/>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="D783" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E783" t="n">
+        <v>31</v>
+      </c>
+      <c r="F783" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G783" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr"/>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>09:27</t>
+        </is>
+      </c>
+      <c r="D784" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E784" t="n">
+        <v>37</v>
+      </c>
+      <c r="F784" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G784" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr"/>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="D785" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E785" t="n">
+        <v>43</v>
+      </c>
+      <c r="F785" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G785" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr"/>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="D786" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E786" t="n">
+        <v>54</v>
+      </c>
+      <c r="F786" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G786" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr"/>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>09:51</t>
+        </is>
+      </c>
+      <c r="D787" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E787" t="n">
+        <v>61</v>
+      </c>
+      <c r="F787" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G787" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr"/>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>09:54</t>
+        </is>
+      </c>
+      <c r="D788" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E788" t="n">
+        <v>64</v>
+      </c>
+      <c r="F788" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G788" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr"/>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="D789" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E789" t="n">
+        <v>73</v>
+      </c>
+      <c r="F789" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G789" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr"/>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>10:04</t>
+        </is>
+      </c>
+      <c r="D790" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E790" t="n">
+        <v>74</v>
+      </c>
+      <c r="F790" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G790" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr"/>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>10:24</t>
+        </is>
+      </c>
+      <c r="D791" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E791" t="n">
+        <v>94</v>
+      </c>
+      <c r="F791" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G791" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr"/>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="D792" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E792" t="n">
+        <v>96</v>
+      </c>
+      <c r="F792" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G792" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -24509,7 +25005,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24557,7 +25053,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:40:09</t>
+          <t>Última actualización: 31/12/2025 08:50:45</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -24570,7 +25066,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 56</t>
+          <t>Total filas: 58</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -26249,6 +26745,68 @@
         <v>83</v>
       </c>
       <c r="G57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>09:27</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>37</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>08:50:34</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>73</v>
+      </c>
+      <c r="G59" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -26265,7 +26823,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26313,7 +26871,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:40:09</t>
+          <t>Última actualización: 31/12/2025 08:50:45</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -26326,7 +26884,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 91</t>
+          <t>Total filas: 93</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -29095,6 +29653,68 @@
         </is>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>08:50:39</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>10:08</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>78</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>92</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 12:00 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G792"/>
+  <dimension ref="A1:G811"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:50:45</t>
+          <t>Última actualización: 31/12/2025 09:00:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 791</t>
+          <t>Total filas: 810</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -24989,6 +24989,595 @@
         </is>
       </c>
       <c r="G792" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr"/>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="D793" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E793" t="n">
+        <v>3</v>
+      </c>
+      <c r="F793" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G793" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr"/>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="D794" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E794" t="n">
+        <v>8</v>
+      </c>
+      <c r="F794" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G794" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr"/>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>09:14</t>
+        </is>
+      </c>
+      <c r="D795" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E795" t="n">
+        <v>14</v>
+      </c>
+      <c r="F795" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G795" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr"/>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="D796" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E796" t="n">
+        <v>16</v>
+      </c>
+      <c r="F796" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G796" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr"/>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="D797" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E797" t="n">
+        <v>21</v>
+      </c>
+      <c r="F797" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G797" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr"/>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>09:26</t>
+        </is>
+      </c>
+      <c r="D798" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E798" t="n">
+        <v>26</v>
+      </c>
+      <c r="F798" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G798" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr"/>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>09:27</t>
+        </is>
+      </c>
+      <c r="D799" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E799" t="n">
+        <v>27</v>
+      </c>
+      <c r="F799" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G799" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr"/>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="D800" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E800" t="n">
+        <v>33</v>
+      </c>
+      <c r="F800" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G800" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr"/>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="D801" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E801" t="n">
+        <v>41</v>
+      </c>
+      <c r="F801" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G801" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr"/>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="D802" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E802" t="n">
+        <v>44</v>
+      </c>
+      <c r="F802" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G802" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr"/>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>09:51</t>
+        </is>
+      </c>
+      <c r="D803" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E803" t="n">
+        <v>51</v>
+      </c>
+      <c r="F803" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G803" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr"/>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>09:54</t>
+        </is>
+      </c>
+      <c r="D804" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E804" t="n">
+        <v>54</v>
+      </c>
+      <c r="F804" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G804" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr"/>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="D805" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E805" t="n">
+        <v>62</v>
+      </c>
+      <c r="F805" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G805" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr"/>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>10:04</t>
+        </is>
+      </c>
+      <c r="D806" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E806" t="n">
+        <v>64</v>
+      </c>
+      <c r="F806" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G806" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr"/>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>10:14</t>
+        </is>
+      </c>
+      <c r="D807" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E807" t="n">
+        <v>74</v>
+      </c>
+      <c r="F807" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G807" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr"/>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>10:24</t>
+        </is>
+      </c>
+      <c r="D808" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E808" t="n">
+        <v>84</v>
+      </c>
+      <c r="F808" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G808" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr"/>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="D809" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E809" t="n">
+        <v>86</v>
+      </c>
+      <c r="F809" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G809" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr"/>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="D810" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E810" t="n">
+        <v>94</v>
+      </c>
+      <c r="F810" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G810" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr"/>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>10:37</t>
+        </is>
+      </c>
+      <c r="D811" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E811" t="n">
+        <v>97</v>
+      </c>
+      <c r="F811" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G811" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -25005,7 +25594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25053,7 +25642,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:50:45</t>
+          <t>Última actualización: 31/12/2025 09:00:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -25066,7 +25655,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 58</t>
+          <t>Total filas: 60</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -26807,6 +27396,68 @@
         <v>73</v>
       </c>
       <c r="G59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>09:26</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>26</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>09:00:46</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>62</v>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -26823,7 +27474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26871,7 +27522,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 08:50:45</t>
+          <t>Última actualización: 31/12/2025 09:00:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -26884,7 +27535,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 93</t>
+          <t>Total filas: 96</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -29715,6 +30366,99 @@
         </is>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>09:00:51</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>10:08</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>68</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>09:00:56</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>82</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>09:00:56</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>90</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 13:02 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G811"/>
+  <dimension ref="A1:G832"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 09:00:57</t>
+          <t>Última actualización: 31/12/2025 10:02:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 810</t>
+          <t>Total filas: 831</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -25578,6 +25578,657 @@
         </is>
       </c>
       <c r="G811" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr"/>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>10:04</t>
+        </is>
+      </c>
+      <c r="D812" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E812" t="n">
+        <v>2</v>
+      </c>
+      <c r="F812" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G812" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr"/>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>10:14</t>
+        </is>
+      </c>
+      <c r="D813" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E813" t="n">
+        <v>12</v>
+      </c>
+      <c r="F813" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G813" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr"/>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>10:25</t>
+        </is>
+      </c>
+      <c r="D814" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E814" t="n">
+        <v>23</v>
+      </c>
+      <c r="F814" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G814" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr"/>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>10:25</t>
+        </is>
+      </c>
+      <c r="D815" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E815" t="n">
+        <v>23</v>
+      </c>
+      <c r="F815" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G815" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr"/>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="D816" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E816" t="n">
+        <v>24</v>
+      </c>
+      <c r="F816" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G816" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr"/>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="D817" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E817" t="n">
+        <v>32</v>
+      </c>
+      <c r="F817" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G817" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr"/>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="D818" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E818" t="n">
+        <v>32</v>
+      </c>
+      <c r="F818" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G818" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr"/>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>10:37</t>
+        </is>
+      </c>
+      <c r="D819" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E819" t="n">
+        <v>35</v>
+      </c>
+      <c r="F819" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G819" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr"/>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>10:39</t>
+        </is>
+      </c>
+      <c r="D820" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E820" t="n">
+        <v>37</v>
+      </c>
+      <c r="F820" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G820" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr"/>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>10:49</t>
+        </is>
+      </c>
+      <c r="D821" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E821" t="n">
+        <v>47</v>
+      </c>
+      <c r="F821" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G821" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr"/>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>10:51</t>
+        </is>
+      </c>
+      <c r="D822" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E822" t="n">
+        <v>49</v>
+      </c>
+      <c r="F822" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G822" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr"/>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="D823" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E823" t="n">
+        <v>52</v>
+      </c>
+      <c r="F823" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G823" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr"/>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="D824" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E824" t="n">
+        <v>55</v>
+      </c>
+      <c r="F824" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G824" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr"/>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="D825" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E825" t="n">
+        <v>59</v>
+      </c>
+      <c r="F825" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G825" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr"/>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>11:03</t>
+        </is>
+      </c>
+      <c r="D826" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E826" t="n">
+        <v>61</v>
+      </c>
+      <c r="F826" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G826" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr"/>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>11:05</t>
+        </is>
+      </c>
+      <c r="D827" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E827" t="n">
+        <v>63</v>
+      </c>
+      <c r="F827" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G827" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr"/>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>11:09</t>
+        </is>
+      </c>
+      <c r="D828" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E828" t="n">
+        <v>67</v>
+      </c>
+      <c r="F828" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G828" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr"/>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>11:11</t>
+        </is>
+      </c>
+      <c r="D829" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E829" t="n">
+        <v>69</v>
+      </c>
+      <c r="F829" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G829" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr"/>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>11:23</t>
+        </is>
+      </c>
+      <c r="D830" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E830" t="n">
+        <v>81</v>
+      </c>
+      <c r="F830" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G830" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr"/>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D831" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E831" t="n">
+        <v>88</v>
+      </c>
+      <c r="F831" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G831" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr"/>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>11:40</t>
+        </is>
+      </c>
+      <c r="D832" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E832" t="n">
+        <v>98</v>
+      </c>
+      <c r="F832" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G832" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -25594,7 +26245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25642,7 +26293,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 09:00:57</t>
+          <t>Última actualización: 31/12/2025 10:02:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -25655,7 +26306,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 60</t>
+          <t>Total filas: 61</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -27458,6 +28109,37 @@
         <v>62</v>
       </c>
       <c r="G61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>11:40</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>98</v>
+      </c>
+      <c r="G62" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -27474,7 +28156,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27522,7 +28204,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 09:00:57</t>
+          <t>Última actualización: 31/12/2025 10:02:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -27535,7 +28217,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 96</t>
+          <t>Total filas: 100</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -30459,6 +31141,130 @@
         </is>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>10:02:12</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>10:09</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>7</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>10:02:17</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>10:23</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>21</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>10:02:17</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>10:31</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>29</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>10:02:17</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>68</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 13:42 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G832"/>
+  <dimension ref="A1:G852"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:02:17</t>
+          <t>Última actualización: 31/12/2025 10:42:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 831</t>
+          <t>Total filas: 851</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -26229,6 +26229,626 @@
         </is>
       </c>
       <c r="G832" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr"/>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="D833" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E833" t="n">
+        <v>2</v>
+      </c>
+      <c r="F833" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G833" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr"/>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>10:49</t>
+        </is>
+      </c>
+      <c r="D834" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E834" t="n">
+        <v>7</v>
+      </c>
+      <c r="F834" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G834" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr"/>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>10:51</t>
+        </is>
+      </c>
+      <c r="D835" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E835" t="n">
+        <v>9</v>
+      </c>
+      <c r="F835" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G835" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr"/>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="D836" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E836" t="n">
+        <v>12</v>
+      </c>
+      <c r="F836" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G836" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr"/>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="D837" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E837" t="n">
+        <v>14</v>
+      </c>
+      <c r="F837" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G837" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr"/>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="D838" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E838" t="n">
+        <v>19</v>
+      </c>
+      <c r="F838" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G838" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr"/>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>11:03</t>
+        </is>
+      </c>
+      <c r="D839" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E839" t="n">
+        <v>21</v>
+      </c>
+      <c r="F839" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G839" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr"/>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="D840" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E840" t="n">
+        <v>22</v>
+      </c>
+      <c r="F840" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G840" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr"/>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>11:09</t>
+        </is>
+      </c>
+      <c r="D841" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E841" t="n">
+        <v>27</v>
+      </c>
+      <c r="F841" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G841" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr"/>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>11:11</t>
+        </is>
+      </c>
+      <c r="D842" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E842" t="n">
+        <v>29</v>
+      </c>
+      <c r="F842" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G842" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr"/>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>11:25</t>
+        </is>
+      </c>
+      <c r="D843" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E843" t="n">
+        <v>43</v>
+      </c>
+      <c r="F843" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G843" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr"/>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>11:27</t>
+        </is>
+      </c>
+      <c r="D844" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E844" t="n">
+        <v>45</v>
+      </c>
+      <c r="F844" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G844" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr"/>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D845" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E845" t="n">
+        <v>48</v>
+      </c>
+      <c r="F845" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G845" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr"/>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>11:33</t>
+        </is>
+      </c>
+      <c r="D846" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E846" t="n">
+        <v>51</v>
+      </c>
+      <c r="F846" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G846" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr"/>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>11:34</t>
+        </is>
+      </c>
+      <c r="D847" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E847" t="n">
+        <v>52</v>
+      </c>
+      <c r="F847" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G847" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr"/>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>11:40</t>
+        </is>
+      </c>
+      <c r="D848" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E848" t="n">
+        <v>58</v>
+      </c>
+      <c r="F848" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G848" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr"/>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="D849" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E849" t="n">
+        <v>63</v>
+      </c>
+      <c r="F849" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G849" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr"/>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>11:53</t>
+        </is>
+      </c>
+      <c r="D850" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E850" t="n">
+        <v>71</v>
+      </c>
+      <c r="F850" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G850" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr"/>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>11:54</t>
+        </is>
+      </c>
+      <c r="D851" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E851" t="n">
+        <v>72</v>
+      </c>
+      <c r="F851" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G851" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr"/>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>12:05</t>
+        </is>
+      </c>
+      <c r="D852" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E852" t="n">
+        <v>83</v>
+      </c>
+      <c r="F852" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G852" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -26245,7 +26865,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26293,7 +26913,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:02:17</t>
+          <t>Última actualización: 31/12/2025 10:42:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -26306,7 +26926,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 61</t>
+          <t>Total filas: 62</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -28140,6 +28760,37 @@
         <v>98</v>
       </c>
       <c r="G62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>10:42:40</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>11:40</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>58</v>
+      </c>
+      <c r="G63" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -28156,7 +28807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28204,7 +28855,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:02:17</t>
+          <t>Última actualización: 31/12/2025 10:42:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -28217,7 +28868,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 100</t>
+          <t>Total filas: 101</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -31265,6 +31916,37 @@
         </is>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>10:42:45</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>11:43</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>61</v>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 13:58 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G852"/>
+  <dimension ref="A1:G871"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:42:51</t>
+          <t>Última actualización: 31/12/2025 10:58:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 851</t>
+          <t>Total filas: 870</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -26849,6 +26849,595 @@
         </is>
       </c>
       <c r="G852" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr"/>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="D853" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E853" t="n">
+        <v>3</v>
+      </c>
+      <c r="F853" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G853" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr"/>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="D854" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E854" t="n">
+        <v>6</v>
+      </c>
+      <c r="F854" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G854" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr"/>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>11:05</t>
+        </is>
+      </c>
+      <c r="D855" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E855" t="n">
+        <v>7</v>
+      </c>
+      <c r="F855" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G855" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr"/>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>11:09</t>
+        </is>
+      </c>
+      <c r="D856" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E856" t="n">
+        <v>11</v>
+      </c>
+      <c r="F856" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G856" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr"/>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>11:11</t>
+        </is>
+      </c>
+      <c r="D857" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E857" t="n">
+        <v>13</v>
+      </c>
+      <c r="F857" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G857" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr"/>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="D858" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="E858" t="n">
+        <v>16</v>
+      </c>
+      <c r="F858" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G858" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr"/>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>11:25</t>
+        </is>
+      </c>
+      <c r="D859" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E859" t="n">
+        <v>27</v>
+      </c>
+      <c r="F859" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G859" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr"/>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="D860" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E860" t="n">
+        <v>28</v>
+      </c>
+      <c r="F860" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G860" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr"/>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>11:34</t>
+        </is>
+      </c>
+      <c r="D861" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E861" t="n">
+        <v>36</v>
+      </c>
+      <c r="F861" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G861" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr"/>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>11:34</t>
+        </is>
+      </c>
+      <c r="D862" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E862" t="n">
+        <v>36</v>
+      </c>
+      <c r="F862" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G862" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr"/>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>11:40</t>
+        </is>
+      </c>
+      <c r="D863" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E863" t="n">
+        <v>42</v>
+      </c>
+      <c r="F863" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G863" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr"/>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="D864" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E864" t="n">
+        <v>47</v>
+      </c>
+      <c r="F864" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G864" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr"/>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>11:53</t>
+        </is>
+      </c>
+      <c r="D865" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E865" t="n">
+        <v>55</v>
+      </c>
+      <c r="F865" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G865" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr"/>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>11:54</t>
+        </is>
+      </c>
+      <c r="D866" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E866" t="n">
+        <v>56</v>
+      </c>
+      <c r="F866" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G866" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr"/>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>11:57</t>
+        </is>
+      </c>
+      <c r="D867" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E867" t="n">
+        <v>59</v>
+      </c>
+      <c r="F867" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G867" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr"/>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>12:03</t>
+        </is>
+      </c>
+      <c r="D868" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E868" t="n">
+        <v>65</v>
+      </c>
+      <c r="F868" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G868" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr"/>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>12:17</t>
+        </is>
+      </c>
+      <c r="D869" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E869" t="n">
+        <v>79</v>
+      </c>
+      <c r="F869" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G869" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr"/>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="D870" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E870" t="n">
+        <v>80</v>
+      </c>
+      <c r="F870" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G870" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr"/>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>12:29</t>
+        </is>
+      </c>
+      <c r="D871" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E871" t="n">
+        <v>91</v>
+      </c>
+      <c r="F871" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G871" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -26865,7 +27454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26913,7 +27502,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:42:51</t>
+          <t>Última actualización: 31/12/2025 10:58:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -26926,7 +27515,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 62</t>
+          <t>Total filas: 64</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -28791,6 +29380,68 @@
         <v>58</v>
       </c>
       <c r="G63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>11:40</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>42</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>10:58:06</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>12:29</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>91</v>
+      </c>
+      <c r="G65" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -28807,7 +29458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28855,7 +29506,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:42:51</t>
+          <t>Última actualización: 31/12/2025 10:58:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -28868,7 +29519,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 101</t>
+          <t>Total filas: 102</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -31947,6 +32598,37 @@
         </is>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>10:58:11</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>11:44</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>46</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 14:27 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G871"/>
+  <dimension ref="A1:G885"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:58:17</t>
+          <t>Última actualización: 31/12/2025 11:27:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 870</t>
+          <t>Total filas: 884</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -27438,6 +27438,440 @@
         </is>
       </c>
       <c r="G871" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr"/>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D872" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E872" t="n">
+        <v>3</v>
+      </c>
+      <c r="F872" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G872" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr"/>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>11:34</t>
+        </is>
+      </c>
+      <c r="D873" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E873" t="n">
+        <v>7</v>
+      </c>
+      <c r="F873" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G873" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr"/>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>11:35</t>
+        </is>
+      </c>
+      <c r="D874" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E874" t="n">
+        <v>8</v>
+      </c>
+      <c r="F874" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G874" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr"/>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="D875" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E875" t="n">
+        <v>14</v>
+      </c>
+      <c r="F875" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G875" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr"/>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>11:46</t>
+        </is>
+      </c>
+      <c r="D876" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E876" t="n">
+        <v>19</v>
+      </c>
+      <c r="F876" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G876" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr"/>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>11:54</t>
+        </is>
+      </c>
+      <c r="D877" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E877" t="n">
+        <v>27</v>
+      </c>
+      <c r="F877" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G877" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr"/>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>11:55</t>
+        </is>
+      </c>
+      <c r="D878" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E878" t="n">
+        <v>28</v>
+      </c>
+      <c r="F878" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G878" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr"/>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="D879" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E879" t="n">
+        <v>31</v>
+      </c>
+      <c r="F879" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G879" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr"/>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="D880" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E880" t="n">
+        <v>37</v>
+      </c>
+      <c r="F880" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G880" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr"/>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="D881" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E881" t="n">
+        <v>51</v>
+      </c>
+      <c r="F881" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G881" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr"/>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>12:19</t>
+        </is>
+      </c>
+      <c r="D882" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E882" t="n">
+        <v>52</v>
+      </c>
+      <c r="F882" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G882" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr"/>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="D883" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E883" t="n">
+        <v>63</v>
+      </c>
+      <c r="F883" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G883" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr"/>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="D884" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E884" t="n">
+        <v>67</v>
+      </c>
+      <c r="F884" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G884" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr"/>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="D885" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E885" t="n">
+        <v>95</v>
+      </c>
+      <c r="F885" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G885" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -27454,7 +27888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27502,7 +27936,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:58:17</t>
+          <t>Última actualización: 31/12/2025 11:27:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -27515,7 +27949,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 64</t>
+          <t>Total filas: 67</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -29442,6 +29876,99 @@
         <v>91</v>
       </c>
       <c r="G65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>14</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>63</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>11:27:00</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>95</v>
+      </c>
+      <c r="G68" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -29458,7 +29985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29506,7 +30033,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 10:58:17</t>
+          <t>Última actualización: 31/12/2025 11:27:11</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -29519,7 +30046,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 102</t>
+          <t>Total filas: 103</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -32629,6 +33156,37 @@
         </is>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>11:27:06</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>11:44</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>17</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 14:46 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G885"/>
+  <dimension ref="A1:G902"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:27:11</t>
+          <t>Última actualización: 31/12/2025 11:46:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 884</t>
+          <t>Total filas: 901</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -27872,6 +27872,533 @@
         </is>
       </c>
       <c r="G885" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr"/>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>11:50</t>
+        </is>
+      </c>
+      <c r="D886" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E886" t="n">
+        <v>4</v>
+      </c>
+      <c r="F886" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G886" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr"/>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>11:53</t>
+        </is>
+      </c>
+      <c r="D887" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E887" t="n">
+        <v>7</v>
+      </c>
+      <c r="F887" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G887" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr"/>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>11:54</t>
+        </is>
+      </c>
+      <c r="D888" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E888" t="n">
+        <v>8</v>
+      </c>
+      <c r="F888" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G888" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr"/>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>11:57</t>
+        </is>
+      </c>
+      <c r="D889" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E889" t="n">
+        <v>11</v>
+      </c>
+      <c r="F889" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G889" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr"/>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="D890" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E890" t="n">
+        <v>18</v>
+      </c>
+      <c r="F890" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G890" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr"/>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>12:05</t>
+        </is>
+      </c>
+      <c r="D891" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E891" t="n">
+        <v>19</v>
+      </c>
+      <c r="F891" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G891" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr"/>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>12:09</t>
+        </is>
+      </c>
+      <c r="D892" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E892" t="n">
+        <v>23</v>
+      </c>
+      <c r="F892" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G892" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr"/>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>12:17</t>
+        </is>
+      </c>
+      <c r="D893" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E893" t="n">
+        <v>31</v>
+      </c>
+      <c r="F893" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G893" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr"/>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="D894" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E894" t="n">
+        <v>32</v>
+      </c>
+      <c r="F894" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G894" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr"/>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="D895" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E895" t="n">
+        <v>32</v>
+      </c>
+      <c r="F895" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G895" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr"/>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>12:29</t>
+        </is>
+      </c>
+      <c r="D896" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E896" t="n">
+        <v>43</v>
+      </c>
+      <c r="F896" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G896" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr"/>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>12:39</t>
+        </is>
+      </c>
+      <c r="D897" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E897" t="n">
+        <v>53</v>
+      </c>
+      <c r="F897" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G897" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr"/>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>12:40</t>
+        </is>
+      </c>
+      <c r="D898" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E898" t="n">
+        <v>54</v>
+      </c>
+      <c r="F898" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G898" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr"/>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>12:51</t>
+        </is>
+      </c>
+      <c r="D899" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E899" t="n">
+        <v>65</v>
+      </c>
+      <c r="F899" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G899" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr"/>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="D900" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E900" t="n">
+        <v>78</v>
+      </c>
+      <c r="F900" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G900" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr"/>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="D901" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E901" t="n">
+        <v>81</v>
+      </c>
+      <c r="F901" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G901" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr"/>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="D902" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E902" t="n">
+        <v>95</v>
+      </c>
+      <c r="F902" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G902" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -27888,7 +28415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27936,7 +28463,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:27:11</t>
+          <t>Última actualización: 31/12/2025 11:46:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -27949,7 +28476,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 67</t>
+          <t>Total filas: 68</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -29969,6 +30496,37 @@
         <v>95</v>
       </c>
       <c r="G68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>11:46:08</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>12:29</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>43</v>
+      </c>
+      <c r="G69" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -29985,7 +30543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30033,7 +30591,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:27:11</t>
+          <t>Última actualización: 31/12/2025 11:46:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -30046,7 +30604,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 103</t>
+          <t>Total filas: 105</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -33187,6 +33745,68 @@
         </is>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>11:46:18</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>13:09</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>83</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>11:46:18</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>88</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 14:57 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G902"/>
+  <dimension ref="A1:G919"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:46:18</t>
+          <t>Última actualización: 31/12/2025 11:57:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 901</t>
+          <t>Total filas: 918</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -28399,6 +28399,533 @@
         </is>
       </c>
       <c r="G902" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr"/>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>11:59</t>
+        </is>
+      </c>
+      <c r="D903" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E903" t="n">
+        <v>2</v>
+      </c>
+      <c r="F903" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G903" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr"/>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="D904" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E904" t="n">
+        <v>7</v>
+      </c>
+      <c r="F904" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G904" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr"/>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="D905" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E905" t="n">
+        <v>9</v>
+      </c>
+      <c r="F905" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G905" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr"/>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="D906" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E906" t="n">
+        <v>13</v>
+      </c>
+      <c r="F906" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G906" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr"/>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="D907" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E907" t="n">
+        <v>21</v>
+      </c>
+      <c r="F907" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G907" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr"/>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="D908" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E908" t="n">
+        <v>21</v>
+      </c>
+      <c r="F908" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G908" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr"/>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>12:29</t>
+        </is>
+      </c>
+      <c r="D909" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E909" t="n">
+        <v>32</v>
+      </c>
+      <c r="F909" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G909" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr"/>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="D910" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E910" t="n">
+        <v>37</v>
+      </c>
+      <c r="F910" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G910" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr"/>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="D911" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E911" t="n">
+        <v>44</v>
+      </c>
+      <c r="F911" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G911" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr"/>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>12:52</t>
+        </is>
+      </c>
+      <c r="D912" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E912" t="n">
+        <v>55</v>
+      </c>
+      <c r="F912" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G912" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr"/>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>12:59</t>
+        </is>
+      </c>
+      <c r="D913" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E913" t="n">
+        <v>62</v>
+      </c>
+      <c r="F913" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G913" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr"/>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>13:01</t>
+        </is>
+      </c>
+      <c r="D914" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E914" t="n">
+        <v>64</v>
+      </c>
+      <c r="F914" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G914" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr"/>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>13:05</t>
+        </is>
+      </c>
+      <c r="D915" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E915" t="n">
+        <v>68</v>
+      </c>
+      <c r="F915" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G915" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr"/>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="D916" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E916" t="n">
+        <v>70</v>
+      </c>
+      <c r="F916" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G916" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr"/>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>13:22</t>
+        </is>
+      </c>
+      <c r="D917" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E917" t="n">
+        <v>85</v>
+      </c>
+      <c r="F917" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G917" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr"/>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="D918" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E918" t="n">
+        <v>93</v>
+      </c>
+      <c r="F918" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G918" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr"/>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="D919" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E919" t="n">
+        <v>95</v>
+      </c>
+      <c r="F919" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G919" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -28415,7 +28942,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28463,7 +28990,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:46:18</t>
+          <t>Última actualización: 31/12/2025 11:57:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -28476,7 +29003,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 68</t>
+          <t>Total filas: 70</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -30527,6 +31054,68 @@
         <v>43</v>
       </c>
       <c r="G69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>12:29</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>32</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>13:01</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>64</v>
+      </c>
+      <c r="G71" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -30543,7 +31132,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30591,7 +31180,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:46:18</t>
+          <t>Última actualización: 31/12/2025 11:57:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -30604,7 +31193,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 105</t>
+          <t>Total filas: 107</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -33807,6 +34396,68 @@
         </is>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>11:57:24</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>13:09</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>72</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>11:57:24</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>77</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 15:26 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G919"/>
+  <dimension ref="A1:G933"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:57:24</t>
+          <t>Última actualización: 31/12/2025 12:26:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 918</t>
+          <t>Total filas: 932</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -28926,6 +28926,440 @@
         </is>
       </c>
       <c r="G919" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr"/>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>12:33</t>
+        </is>
+      </c>
+      <c r="D920" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E920" t="n">
+        <v>7</v>
+      </c>
+      <c r="F920" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G920" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr"/>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>12:40</t>
+        </is>
+      </c>
+      <c r="D921" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E921" t="n">
+        <v>14</v>
+      </c>
+      <c r="F921" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G921" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr"/>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>12:51</t>
+        </is>
+      </c>
+      <c r="D922" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E922" t="n">
+        <v>25</v>
+      </c>
+      <c r="F922" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G922" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr"/>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="D923" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E923" t="n">
+        <v>28</v>
+      </c>
+      <c r="F923" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G923" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr"/>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>12:58</t>
+        </is>
+      </c>
+      <c r="D924" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E924" t="n">
+        <v>32</v>
+      </c>
+      <c r="F924" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G924" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr"/>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>13:01</t>
+        </is>
+      </c>
+      <c r="D925" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E925" t="n">
+        <v>35</v>
+      </c>
+      <c r="F925" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G925" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr"/>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="D926" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E926" t="n">
+        <v>40</v>
+      </c>
+      <c r="F926" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G926" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr"/>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>13:10</t>
+        </is>
+      </c>
+      <c r="D927" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E927" t="n">
+        <v>44</v>
+      </c>
+      <c r="F927" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G927" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr"/>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>13:11</t>
+        </is>
+      </c>
+      <c r="D928" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E928" t="n">
+        <v>45</v>
+      </c>
+      <c r="F928" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G928" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr"/>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="D929" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E929" t="n">
+        <v>55</v>
+      </c>
+      <c r="F929" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G929" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr"/>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="D930" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E930" t="n">
+        <v>64</v>
+      </c>
+      <c r="F930" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G930" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr"/>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="D931" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E931" t="n">
+        <v>65</v>
+      </c>
+      <c r="F931" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G931" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr"/>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="D932" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E932" t="n">
+        <v>67</v>
+      </c>
+      <c r="F932" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G932" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr"/>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="D933" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E933" t="n">
+        <v>85</v>
+      </c>
+      <c r="F933" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G933" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -28942,7 +29376,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28990,7 +29424,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:57:24</t>
+          <t>Última actualización: 31/12/2025 12:26:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -29003,7 +29437,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 70</t>
+          <t>Total filas: 71</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -31116,6 +31550,37 @@
         <v>64</v>
       </c>
       <c r="G71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>12:26:24</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>13:01</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>35</v>
+      </c>
+      <c r="G72" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -31132,7 +31597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31180,7 +31645,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 11:57:24</t>
+          <t>Última actualización: 31/12/2025 12:26:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -31193,7 +31658,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 107</t>
+          <t>Total filas: 110</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -34458,6 +34923,99 @@
         </is>
       </c>
     </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>12:26:34</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>13:09</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>43</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>12:26:34</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>48</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>12:26:29</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>88</v>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 15:43 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G933"/>
+  <dimension ref="A1:G947"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:26:35</t>
+          <t>Última actualización: 31/12/2025 12:43:43</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 932</t>
+          <t>Total filas: 946</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -29360,6 +29360,440 @@
         </is>
       </c>
       <c r="G933" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr"/>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>12:51</t>
+        </is>
+      </c>
+      <c r="D934" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E934" t="n">
+        <v>8</v>
+      </c>
+      <c r="F934" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G934" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr"/>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>12:58</t>
+        </is>
+      </c>
+      <c r="D935" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E935" t="n">
+        <v>15</v>
+      </c>
+      <c r="F935" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G935" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr"/>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>13:01</t>
+        </is>
+      </c>
+      <c r="D936" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E936" t="n">
+        <v>18</v>
+      </c>
+      <c r="F936" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G936" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr"/>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="D937" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E937" t="n">
+        <v>20</v>
+      </c>
+      <c r="F937" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G937" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr"/>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="D938" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E938" t="n">
+        <v>23</v>
+      </c>
+      <c r="F938" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G938" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr"/>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>13:11</t>
+        </is>
+      </c>
+      <c r="D939" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E939" t="n">
+        <v>28</v>
+      </c>
+      <c r="F939" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G939" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr"/>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>13:18</t>
+        </is>
+      </c>
+      <c r="D940" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E940" t="n">
+        <v>35</v>
+      </c>
+      <c r="F940" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G940" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr"/>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="D941" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E941" t="n">
+        <v>38</v>
+      </c>
+      <c r="F941" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G941" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr"/>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="D942" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E942" t="n">
+        <v>38</v>
+      </c>
+      <c r="F942" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G942" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr"/>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="D943" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E943" t="n">
+        <v>47</v>
+      </c>
+      <c r="F943" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G943" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr"/>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="D944" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E944" t="n">
+        <v>48</v>
+      </c>
+      <c r="F944" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G944" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr"/>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="D945" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E945" t="n">
+        <v>50</v>
+      </c>
+      <c r="F945" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G945" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr"/>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="D946" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E946" t="n">
+        <v>68</v>
+      </c>
+      <c r="F946" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G946" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr"/>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D947" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E947" t="n">
+        <v>81</v>
+      </c>
+      <c r="F947" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G947" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -29376,7 +29810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29424,7 +29858,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:26:35</t>
+          <t>Última actualización: 31/12/2025 12:43:43</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -29437,7 +29871,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 71</t>
+          <t>Total filas: 72</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -31581,6 +32015,37 @@
         <v>35</v>
       </c>
       <c r="G72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>13:01</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>18</v>
+      </c>
+      <c r="G73" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -31597,7 +32062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31645,7 +32110,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:26:35</t>
+          <t>Última actualización: 31/12/2025 12:43:43</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -31658,7 +32123,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 110</t>
+          <t>Total filas: 113</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -35016,6 +35481,99 @@
         </is>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>12:43:43</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>13:08</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>25</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>12:43:43</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>30</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>12:43:38</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>13:53</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>70</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 15:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G947"/>
+  <dimension ref="A1:G964"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:43:43</t>
+          <t>Última actualización: 31/12/2025 12:56:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 946</t>
+          <t>Total filas: 963</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -29794,6 +29794,533 @@
         </is>
       </c>
       <c r="G947" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr"/>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>12:58</t>
+        </is>
+      </c>
+      <c r="D948" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E948" t="n">
+        <v>2</v>
+      </c>
+      <c r="F948" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G948" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr"/>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>12:59</t>
+        </is>
+      </c>
+      <c r="D949" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E949" t="n">
+        <v>3</v>
+      </c>
+      <c r="F949" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G949" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr"/>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>13:01</t>
+        </is>
+      </c>
+      <c r="D950" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E950" t="n">
+        <v>5</v>
+      </c>
+      <c r="F950" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G950" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr"/>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="D951" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E951" t="n">
+        <v>8</v>
+      </c>
+      <c r="F951" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G951" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr"/>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="D952" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E952" t="n">
+        <v>11</v>
+      </c>
+      <c r="F952" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G952" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr"/>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>13:11</t>
+        </is>
+      </c>
+      <c r="D953" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E953" t="n">
+        <v>15</v>
+      </c>
+      <c r="F953" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G953" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr"/>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>13:19</t>
+        </is>
+      </c>
+      <c r="D954" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E954" t="n">
+        <v>23</v>
+      </c>
+      <c r="F954" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G954" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr"/>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="D955" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E955" t="n">
+        <v>25</v>
+      </c>
+      <c r="F955" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G955" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr"/>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="D956" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E956" t="n">
+        <v>25</v>
+      </c>
+      <c r="F956" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G956" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr"/>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="D957" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E957" t="n">
+        <v>34</v>
+      </c>
+      <c r="F957" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G957" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr"/>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="D958" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E958" t="n">
+        <v>35</v>
+      </c>
+      <c r="F958" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G958" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr"/>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>13:34</t>
+        </is>
+      </c>
+      <c r="D959" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E959" t="n">
+        <v>38</v>
+      </c>
+      <c r="F959" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G959" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr"/>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="D960" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E960" t="n">
+        <v>55</v>
+      </c>
+      <c r="F960" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G960" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr"/>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>14:01</t>
+        </is>
+      </c>
+      <c r="D961" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E961" t="n">
+        <v>65</v>
+      </c>
+      <c r="F961" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G961" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr"/>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="D962" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E962" t="n">
+        <v>68</v>
+      </c>
+      <c r="F962" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G962" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr"/>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>14:11</t>
+        </is>
+      </c>
+      <c r="D963" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E963" t="n">
+        <v>75</v>
+      </c>
+      <c r="F963" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G963" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr"/>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>14:25</t>
+        </is>
+      </c>
+      <c r="D964" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E964" t="n">
+        <v>89</v>
+      </c>
+      <c r="F964" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G964" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -29810,7 +30337,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29858,7 +30385,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:43:43</t>
+          <t>Última actualización: 31/12/2025 12:56:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -29871,7 +30398,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 72</t>
+          <t>Total filas: 73</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -32046,6 +32573,37 @@
         <v>18</v>
       </c>
       <c r="G73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>12:56:02</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>13:01</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>5</v>
+      </c>
+      <c r="G74" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -32062,7 +32620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32110,7 +32668,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:43:43</t>
+          <t>Última actualización: 31/12/2025 12:56:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -32123,7 +32681,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 113</t>
+          <t>Total filas: 117</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -35574,6 +36132,130 @@
         </is>
       </c>
     </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>12:56:12</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>13:09</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>13</v>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>12:56:12</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>18</v>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>12:56:07</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>58</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>12:56:07</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>98</v>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 16:28 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G964"/>
+  <dimension ref="A1:G978"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:56:12</t>
+          <t>Última actualización: 31/12/2025 13:28:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 963</t>
+          <t>Total filas: 977</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -30321,6 +30321,440 @@
         </is>
       </c>
       <c r="G964" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr"/>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="D965" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E965" t="n">
+        <v>3</v>
+      </c>
+      <c r="F965" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G965" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr"/>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>13:34</t>
+        </is>
+      </c>
+      <c r="D966" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E966" t="n">
+        <v>6</v>
+      </c>
+      <c r="F966" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G966" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr"/>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>13:41</t>
+        </is>
+      </c>
+      <c r="D967" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E967" t="n">
+        <v>13</v>
+      </c>
+      <c r="F967" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G967" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr"/>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="D968" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E968" t="n">
+        <v>23</v>
+      </c>
+      <c r="F968" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G968" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr"/>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="D969" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E969" t="n">
+        <v>23</v>
+      </c>
+      <c r="F969" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G969" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr"/>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>14:01</t>
+        </is>
+      </c>
+      <c r="D970" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E970" t="n">
+        <v>33</v>
+      </c>
+      <c r="F970" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G970" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr"/>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>14:01</t>
+        </is>
+      </c>
+      <c r="D971" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E971" t="n">
+        <v>33</v>
+      </c>
+      <c r="F971" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G971" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr"/>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>14:03</t>
+        </is>
+      </c>
+      <c r="D972" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E972" t="n">
+        <v>35</v>
+      </c>
+      <c r="F972" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G972" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr"/>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>14:11</t>
+        </is>
+      </c>
+      <c r="D973" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E973" t="n">
+        <v>43</v>
+      </c>
+      <c r="F973" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G973" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr"/>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>14:24</t>
+        </is>
+      </c>
+      <c r="D974" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E974" t="n">
+        <v>56</v>
+      </c>
+      <c r="F974" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G974" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr"/>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="D975" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E975" t="n">
+        <v>69</v>
+      </c>
+      <c r="F975" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G975" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr"/>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="D976" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E976" t="n">
+        <v>71</v>
+      </c>
+      <c r="F976" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G976" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr"/>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>14:40</t>
+        </is>
+      </c>
+      <c r="D977" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E977" t="n">
+        <v>72</v>
+      </c>
+      <c r="F977" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G977" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr"/>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>13:28:29</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>15:04</t>
+        </is>
+      </c>
+      <c r="D978" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E978" t="n">
+        <v>96</v>
+      </c>
+      <c r="F978" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G978" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -30385,7 +30819,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:56:12</t>
+          <t>Última actualización: 31/12/2025 13:28:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -32620,7 +33054,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32668,7 +33102,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 12:56:12</t>
+          <t>Última actualización: 31/12/2025 13:28:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -32681,7 +33115,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 117</t>
+          <t>Total filas: 119</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -36256,6 +36690,68 @@
         </is>
       </c>
     </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>13:28:34</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>26</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>13:28:34</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>66</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 16:51 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G978"/>
+  <dimension ref="A1:G990"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 13:28:40</t>
+          <t>Última actualización: 31/12/2025 13:51:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 977</t>
+          <t>Total filas: 989</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -30755,6 +30755,378 @@
         </is>
       </c>
       <c r="G978" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr"/>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>14:01</t>
+        </is>
+      </c>
+      <c r="D979" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E979" t="n">
+        <v>10</v>
+      </c>
+      <c r="F979" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G979" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr"/>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>14:01</t>
+        </is>
+      </c>
+      <c r="D980" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E980" t="n">
+        <v>10</v>
+      </c>
+      <c r="F980" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G980" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr"/>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>14:03</t>
+        </is>
+      </c>
+      <c r="D981" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E981" t="n">
+        <v>12</v>
+      </c>
+      <c r="F981" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G981" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr"/>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>14:13</t>
+        </is>
+      </c>
+      <c r="D982" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E982" t="n">
+        <v>22</v>
+      </c>
+      <c r="F982" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G982" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr"/>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>14:25</t>
+        </is>
+      </c>
+      <c r="D983" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E983" t="n">
+        <v>34</v>
+      </c>
+      <c r="F983" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G983" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr"/>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>14:25</t>
+        </is>
+      </c>
+      <c r="D984" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E984" t="n">
+        <v>34</v>
+      </c>
+      <c r="F984" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G984" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr"/>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="D985" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E985" t="n">
+        <v>46</v>
+      </c>
+      <c r="F985" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G985" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr"/>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>14:40</t>
+        </is>
+      </c>
+      <c r="D986" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E986" t="n">
+        <v>49</v>
+      </c>
+      <c r="F986" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G986" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr"/>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>14:41</t>
+        </is>
+      </c>
+      <c r="D987" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E987" t="n">
+        <v>50</v>
+      </c>
+      <c r="F987" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G987" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr"/>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D988" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E988" t="n">
+        <v>82</v>
+      </c>
+      <c r="F988" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G988" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr"/>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>15:14</t>
+        </is>
+      </c>
+      <c r="D989" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E989" t="n">
+        <v>83</v>
+      </c>
+      <c r="F989" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G989" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr"/>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="D990" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E990" t="n">
+        <v>94</v>
+      </c>
+      <c r="F990" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G990" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -30819,7 +31191,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 13:28:40</t>
+          <t>Última actualización: 31/12/2025 13:51:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -33054,7 +33426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33102,7 +33474,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 13:28:40</t>
+          <t>Última actualización: 31/12/2025 13:51:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -33115,7 +33487,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 119</t>
+          <t>Total filas: 121</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -36752,6 +37124,68 @@
         </is>
       </c>
     </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>13:51:25</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>43</v>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>13:51:30</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>69</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 17:19 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G990"/>
+  <dimension ref="A1:G1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 13:51:30</t>
+          <t>Última actualización: 31/12/2025 14:19:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 989</t>
+          <t>Total filas: 1001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -31127,6 +31127,378 @@
         </is>
       </c>
       <c r="G990" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr"/>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>14:25</t>
+        </is>
+      </c>
+      <c r="D991" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E991" t="n">
+        <v>7</v>
+      </c>
+      <c r="F991" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G991" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr"/>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="D992" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E992" t="n">
+        <v>15</v>
+      </c>
+      <c r="F992" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G992" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr"/>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>14:37</t>
+        </is>
+      </c>
+      <c r="D993" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E993" t="n">
+        <v>19</v>
+      </c>
+      <c r="F993" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G993" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr"/>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>14:40</t>
+        </is>
+      </c>
+      <c r="D994" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E994" t="n">
+        <v>22</v>
+      </c>
+      <c r="F994" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G994" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr"/>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>14:49</t>
+        </is>
+      </c>
+      <c r="D995" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E995" t="n">
+        <v>31</v>
+      </c>
+      <c r="F995" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G995" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr"/>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D996" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E996" t="n">
+        <v>55</v>
+      </c>
+      <c r="F996" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G996" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr"/>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>15:14</t>
+        </is>
+      </c>
+      <c r="D997" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E997" t="n">
+        <v>56</v>
+      </c>
+      <c r="F997" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G997" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr"/>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>15:19</t>
+        </is>
+      </c>
+      <c r="D998" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E998" t="n">
+        <v>61</v>
+      </c>
+      <c r="F998" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G998" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr"/>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="D999" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E999" t="n">
+        <v>66</v>
+      </c>
+      <c r="F999" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G999" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr"/>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="D1000" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1000" t="n">
+        <v>75</v>
+      </c>
+      <c r="F1000" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1000" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr"/>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="D1001" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1001" t="n">
+        <v>78</v>
+      </c>
+      <c r="F1001" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1001" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr"/>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>14:18:57</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="D1002" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1002" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1002" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1002" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -31191,7 +31563,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 13:51:30</t>
+          <t>Última actualización: 31/12/2025 14:19:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -33426,7 +33798,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33474,7 +33846,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 13:51:30</t>
+          <t>Última actualización: 31/12/2025 14:19:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -33487,7 +33859,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 121</t>
+          <t>Total filas: 123</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -37186,6 +37558,68 @@
         </is>
       </c>
     </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>14:19:03</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>14:35</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>16</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>14:19:08</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>15:01</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>42</v>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 17:38 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1002"/>
+  <dimension ref="A1:G1013"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:19:08</t>
+          <t>Última actualización: 31/12/2025 14:38:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1001</t>
+          <t>Total filas: 1012</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -31499,6 +31499,347 @@
         </is>
       </c>
       <c r="G1002" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr"/>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>14:40</t>
+        </is>
+      </c>
+      <c r="D1003" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1003" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1003" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1003" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr"/>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>14:49</t>
+        </is>
+      </c>
+      <c r="D1004" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1004" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1004" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1004" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr"/>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>15:03</t>
+        </is>
+      </c>
+      <c r="D1005" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1005" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1005" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1005" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr"/>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>15:04</t>
+        </is>
+      </c>
+      <c r="D1006" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1006" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1006" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1006" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr"/>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>15:14</t>
+        </is>
+      </c>
+      <c r="D1007" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1007" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1007" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1007" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr"/>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="D1008" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1008" t="n">
+        <v>46</v>
+      </c>
+      <c r="F1008" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1008" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr"/>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="D1009" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1009" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1009" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1009" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr"/>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="D1010" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1010" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1010" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1010" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr"/>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="D1011" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1011" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1011" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1011" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr"/>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="D1012" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1012" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1012" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1012" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr"/>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>14:38:41</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D1013" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1013" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1013" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1013" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -31563,7 +31904,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:19:08</t>
+          <t>Última actualización: 31/12/2025 14:38:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -33798,7 +34139,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33846,7 +34187,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:19:08</t>
+          <t>Última actualización: 31/12/2025 14:38:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -33859,7 +34200,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 123</t>
+          <t>Total filas: 125</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -37620,6 +37961,68 @@
         </is>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>14:38:51</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>14:59</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>21</v>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr"/>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>14:38:46</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>68</v>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 17:50 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1013"/>
+  <dimension ref="A1:G1025"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:38:51</t>
+          <t>Última actualización: 31/12/2025 14:50:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1012</t>
+          <t>Total filas: 1024</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -31840,6 +31840,378 @@
         </is>
       </c>
       <c r="G1013" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr"/>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>15:03</t>
+        </is>
+      </c>
+      <c r="D1014" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1014" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1014" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1014" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr"/>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>15:04</t>
+        </is>
+      </c>
+      <c r="D1015" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1015" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1015" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1015" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr"/>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D1016" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1016" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1016" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1016" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr"/>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D1017" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1017" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1017" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1017" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr"/>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="D1018" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1018" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1018" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1018" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr"/>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="D1019" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1019" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1019" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1019" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr"/>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="D1020" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1020" t="n">
+        <v>47</v>
+      </c>
+      <c r="F1020" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1020" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr"/>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="D1021" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1021" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1021" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1021" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr"/>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="D1022" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1022" t="n">
+        <v>68</v>
+      </c>
+      <c r="F1022" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1022" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr"/>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D1023" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1023" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1023" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1023" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr"/>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="D1024" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1024" t="n">
+        <v>87</v>
+      </c>
+      <c r="F1024" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1024" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr"/>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>14:49:55</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="D1025" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1025" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1025" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1025" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -31904,7 +32276,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:38:51</t>
+          <t>Última actualización: 31/12/2025 14:50:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -34139,7 +34511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34187,7 +34559,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:38:51</t>
+          <t>Última actualización: 31/12/2025 14:50:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -34200,7 +34572,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 125</t>
+          <t>Total filas: 127</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -38023,6 +38395,68 @@
         </is>
       </c>
     </row>
+    <row r="127">
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>14:50:05</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>14:59</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>9</v>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr"/>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>14:50:00</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>56</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 18:00 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1025"/>
+  <dimension ref="A1:G1040"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:50:06</t>
+          <t>Última actualización: 31/12/2025 15:00:03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1024</t>
+          <t>Total filas: 1039</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -32212,6 +32212,471 @@
         </is>
       </c>
       <c r="G1025" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr"/>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>15:01</t>
+        </is>
+      </c>
+      <c r="D1026" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1026" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1026" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1026" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr"/>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>15:03</t>
+        </is>
+      </c>
+      <c r="D1027" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1027" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1027" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1027" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr"/>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D1028" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1028" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1028" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1028" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr"/>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="D1029" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1029" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1029" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1029" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr"/>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="D1030" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1030" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1030" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1030" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr"/>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="D1031" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1031" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1031" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1031" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr"/>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="D1032" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1032" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1032" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1032" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr"/>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="D1033" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1033" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1033" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1033" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr"/>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D1034" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1034" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1034" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1034" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr"/>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="D1035" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1035" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1035" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1035" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr"/>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="D1036" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1036" t="n">
+        <v>77</v>
+      </c>
+      <c r="F1036" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1036" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr"/>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="D1037" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1037" t="n">
+        <v>85</v>
+      </c>
+      <c r="F1037" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1037" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr"/>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="D1038" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1038" t="n">
+        <v>92</v>
+      </c>
+      <c r="F1038" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1038" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr"/>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="D1039" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1039" t="n">
+        <v>94</v>
+      </c>
+      <c r="F1039" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1039" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr"/>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>14:59:52</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="D1040" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1040" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1040" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1040" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -32276,7 +32741,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:50:06</t>
+          <t>Última actualización: 31/12/2025 15:00:03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -34511,7 +34976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34559,7 +35024,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 14:50:06</t>
+          <t>Última actualización: 31/12/2025 15:00:03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -34572,7 +35037,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 127</t>
+          <t>Total filas: 128</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -38457,6 +38922,37 @@
         </is>
       </c>
     </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>14:59:58</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>47</v>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 18:41 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1040"/>
+  <dimension ref="A1:G1054"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:00:03</t>
+          <t>Última actualización: 31/12/2025 15:41:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1039</t>
+          <t>Total filas: 1053</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -32677,6 +32677,440 @@
         </is>
       </c>
       <c r="G1040" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr"/>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="D1041" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1041" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1041" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1041" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr"/>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D1042" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1042" t="n">
+        <v>21</v>
+      </c>
+      <c r="F1042" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1042" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr"/>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>16:03</t>
+        </is>
+      </c>
+      <c r="D1043" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1043" t="n">
+        <v>23</v>
+      </c>
+      <c r="F1043" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1043" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr"/>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="D1044" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1044" t="n">
+        <v>29</v>
+      </c>
+      <c r="F1044" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1044" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr"/>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>16:13</t>
+        </is>
+      </c>
+      <c r="D1045" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1045" t="n">
+        <v>33</v>
+      </c>
+      <c r="F1045" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1045" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr"/>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="D1046" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1046" t="n">
+        <v>41</v>
+      </c>
+      <c r="F1046" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1046" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr"/>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>16:24</t>
+        </is>
+      </c>
+      <c r="D1047" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1047" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1047" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1047" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr"/>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="D1048" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1048" t="n">
+        <v>51</v>
+      </c>
+      <c r="F1048" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1048" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr"/>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="D1049" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1049" t="n">
+        <v>51</v>
+      </c>
+      <c r="F1049" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1049" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr"/>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="D1050" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1050" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1050" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1050" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr"/>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="D1051" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1051" t="n">
+        <v>73</v>
+      </c>
+      <c r="F1051" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1051" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr"/>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="D1052" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1052" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1052" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1052" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr"/>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="D1053" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1053" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1053" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1053" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr"/>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>15:40:55</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="D1054" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1054" t="n">
+        <v>87</v>
+      </c>
+      <c r="F1054" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1054" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -32741,7 +33175,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:00:03</t>
+          <t>Última actualización: 31/12/2025 15:41:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -34976,7 +35410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35024,7 +35458,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:00:03</t>
+          <t>Última actualización: 31/12/2025 15:41:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -35037,7 +35471,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 128</t>
+          <t>Total filas: 130</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -38953,6 +39387,68 @@
         </is>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>15:41:01</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>5</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>15:41:01</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>16:59</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>78</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 18:59 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1054"/>
+  <dimension ref="A1:G1071"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:41:06</t>
+          <t>Última actualización: 31/12/2025 15:59:25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1053</t>
+          <t>Total filas: 1070</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -33111,6 +33111,533 @@
         </is>
       </c>
       <c r="G1054" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr"/>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>16:04</t>
+        </is>
+      </c>
+      <c r="D1055" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1055" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1055" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1055" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr"/>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>16:10</t>
+        </is>
+      </c>
+      <c r="D1056" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1056" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1056" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1056" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr"/>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="D1057" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1057" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1057" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1057" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr"/>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>16:22</t>
+        </is>
+      </c>
+      <c r="D1058" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1058" t="n">
+        <v>23</v>
+      </c>
+      <c r="F1058" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1058" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr"/>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>16:25</t>
+        </is>
+      </c>
+      <c r="D1059" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1059" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1059" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1059" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr"/>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>16:32</t>
+        </is>
+      </c>
+      <c r="D1060" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1060" t="n">
+        <v>33</v>
+      </c>
+      <c r="F1060" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1060" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr"/>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="D1061" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1061" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1061" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1061" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr"/>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>16:37</t>
+        </is>
+      </c>
+      <c r="D1062" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1062" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1062" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1062" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr"/>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>16:52</t>
+        </is>
+      </c>
+      <c r="D1063" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1063" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1063" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1063" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr"/>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>16:54</t>
+        </is>
+      </c>
+      <c r="D1064" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1064" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1064" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1064" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr"/>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D1065" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1065" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1065" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1065" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr"/>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>17:08</t>
+        </is>
+      </c>
+      <c r="D1066" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1066" t="n">
+        <v>69</v>
+      </c>
+      <c r="F1066" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1066" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr"/>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>17:25</t>
+        </is>
+      </c>
+      <c r="D1067" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1067" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1067" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1067" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr"/>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="D1068" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1068" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1068" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1068" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr"/>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="D1069" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1069" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1069" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1069" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr"/>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D1070" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1070" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1070" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1070" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr"/>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>15:59:15</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="D1071" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1071" t="n">
+        <v>97</v>
+      </c>
+      <c r="F1071" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1071" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -33175,7 +33702,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:41:06</t>
+          <t>Última actualización: 31/12/2025 15:59:25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -35410,7 +35937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35458,7 +35985,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:41:06</t>
+          <t>Última actualización: 31/12/2025 15:59:25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -35471,7 +35998,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 130</t>
+          <t>Total filas: 132</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -39449,6 +39976,68 @@
         </is>
       </c>
     </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>15:59:25</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>16:26</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>27</v>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>15:59:20</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>59</v>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 19:23 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1071"/>
+  <dimension ref="A1:G1089"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:59:25</t>
+          <t>Última actualización: 31/12/2025 16:23:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1070</t>
+          <t>Total filas: 1088</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -33638,6 +33638,564 @@
         </is>
       </c>
       <c r="G1071" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr"/>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>16:31</t>
+        </is>
+      </c>
+      <c r="D1072" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1072" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1072" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1072" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr"/>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="D1073" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1073" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1073" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1073" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr"/>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="D1074" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1074" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1074" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1074" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr"/>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>16:45</t>
+        </is>
+      </c>
+      <c r="D1075" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1075" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1075" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1075" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr"/>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>16:51</t>
+        </is>
+      </c>
+      <c r="D1076" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1076" t="n">
+        <v>28</v>
+      </c>
+      <c r="F1076" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1076" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr"/>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>16:54</t>
+        </is>
+      </c>
+      <c r="D1077" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1077" t="n">
+        <v>31</v>
+      </c>
+      <c r="F1077" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1077" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr"/>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="D1078" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1078" t="n">
+        <v>42</v>
+      </c>
+      <c r="F1078" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1078" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr"/>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="D1079" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1079" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1079" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1079" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr"/>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>17:14</t>
+        </is>
+      </c>
+      <c r="D1080" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1080" t="n">
+        <v>51</v>
+      </c>
+      <c r="F1080" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1080" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr"/>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>17:23</t>
+        </is>
+      </c>
+      <c r="D1081" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1081" t="n">
+        <v>60</v>
+      </c>
+      <c r="F1081" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1081" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr"/>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>17:25</t>
+        </is>
+      </c>
+      <c r="D1082" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1082" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1082" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1082" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr"/>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>17:27</t>
+        </is>
+      </c>
+      <c r="D1083" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1083" t="n">
+        <v>64</v>
+      </c>
+      <c r="F1083" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1083" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr"/>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="D1084" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1084" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1084" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1084" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr"/>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="D1085" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1085" t="n">
+        <v>71</v>
+      </c>
+      <c r="F1085" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1085" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr"/>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D1086" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1086" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1086" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1086" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr"/>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D1087" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1087" t="n">
+        <v>75</v>
+      </c>
+      <c r="F1087" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1087" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr"/>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="D1088" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1088" t="n">
+        <v>82</v>
+      </c>
+      <c r="F1088" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1088" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr"/>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="D1089" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1089" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1089" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1089" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -33654,7 +34212,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33702,7 +34260,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:59:25</t>
+          <t>Última actualización: 31/12/2025 16:23:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -33715,7 +34273,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 73</t>
+          <t>Total filas: 74</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -35921,6 +36479,37 @@
         <v>5</v>
       </c>
       <c r="G74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>16:23:15</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>88</v>
+      </c>
+      <c r="G75" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -35937,7 +36526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G133"/>
+  <dimension ref="A1:G135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35985,7 +36574,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 15:59:25</t>
+          <t>Última actualización: 31/12/2025 16:23:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -35998,7 +36587,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 132</t>
+          <t>Total filas: 134</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -40038,6 +40627,68 @@
         </is>
       </c>
     </row>
+    <row r="134">
+      <c r="A134" t="inlineStr"/>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>16:23:26</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>16:26</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>3</v>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>16:23:21</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>35</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 19:38 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1089"/>
+  <dimension ref="A1:G1105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:23:26</t>
+          <t>Última actualización: 31/12/2025 16:38:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1088</t>
+          <t>Total filas: 1104</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -34196,6 +34196,502 @@
         </is>
       </c>
       <c r="G1089" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr"/>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>16:51</t>
+        </is>
+      </c>
+      <c r="D1090" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1090" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1090" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1090" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr"/>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>17:03</t>
+        </is>
+      </c>
+      <c r="D1091" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1091" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1091" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1091" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr"/>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="D1092" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1092" t="n">
+        <v>27</v>
+      </c>
+      <c r="F1092" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1092" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr"/>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="D1093" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1093" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1093" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1093" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr"/>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>17:13</t>
+        </is>
+      </c>
+      <c r="D1094" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1094" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1094" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1094" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr"/>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>17:23</t>
+        </is>
+      </c>
+      <c r="D1095" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1095" t="n">
+        <v>46</v>
+      </c>
+      <c r="F1095" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1095" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr"/>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="D1096" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1096" t="n">
+        <v>47</v>
+      </c>
+      <c r="F1096" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1096" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr"/>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>17:27</t>
+        </is>
+      </c>
+      <c r="D1097" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1097" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1097" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1097" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr"/>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="D1098" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1098" t="n">
+        <v>51</v>
+      </c>
+      <c r="F1098" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1098" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr"/>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="D1099" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1099" t="n">
+        <v>57</v>
+      </c>
+      <c r="F1099" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1099" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr"/>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D1100" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1100" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1100" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr"/>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D1101" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1101" t="n">
+        <v>61</v>
+      </c>
+      <c r="F1101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1101" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr"/>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="D1102" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1102" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1102" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr"/>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>17:54</t>
+        </is>
+      </c>
+      <c r="D1103" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1103" t="n">
+        <v>77</v>
+      </c>
+      <c r="F1103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1103" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr"/>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D1104" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1104" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1104" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr"/>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>16:37:58</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D1105" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1105" t="n">
+        <v>87</v>
+      </c>
+      <c r="F1105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1105" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -34260,7 +34756,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:23:26</t>
+          <t>Última actualización: 31/12/2025 16:38:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -36526,7 +37022,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G135"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36574,7 +37070,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:23:26</t>
+          <t>Última actualización: 31/12/2025 16:38:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -36587,7 +37083,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 134</t>
+          <t>Total filas: 135</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -40689,6 +41185,37 @@
         </is>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>16:38:03</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>20</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 19:48 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1105"/>
+  <dimension ref="A1:G1124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:38:09</t>
+          <t>Última actualización: 31/12/2025 16:48:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1104</t>
+          <t>Total filas: 1123</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -34692,6 +34692,595 @@
         </is>
       </c>
       <c r="G1105" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr"/>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>17:03</t>
+        </is>
+      </c>
+      <c r="D1106" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1106" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1106" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr"/>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="D1107" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1107" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1107" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr"/>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="D1108" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1108" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1108" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr"/>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>17:14</t>
+        </is>
+      </c>
+      <c r="D1109" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1109" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1109" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr"/>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>17:23</t>
+        </is>
+      </c>
+      <c r="D1110" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1110" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1110" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr"/>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="D1111" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1111" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1111" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr"/>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>17:27</t>
+        </is>
+      </c>
+      <c r="D1112" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1112" t="n">
+        <v>39</v>
+      </c>
+      <c r="F1112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1112" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr"/>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>17:33</t>
+        </is>
+      </c>
+      <c r="D1113" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1113" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1113" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr"/>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="D1114" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1114" t="n">
+        <v>46</v>
+      </c>
+      <c r="F1114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1114" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr"/>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D1115" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1115" t="n">
+        <v>47</v>
+      </c>
+      <c r="F1115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1115" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr"/>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D1116" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1116" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1116" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr"/>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="D1117" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1117" t="n">
+        <v>59</v>
+      </c>
+      <c r="F1117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1117" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr"/>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="D1118" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1118" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1118" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr"/>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>17:54</t>
+        </is>
+      </c>
+      <c r="D1119" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1119" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1119" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr"/>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>17:59</t>
+        </is>
+      </c>
+      <c r="D1120" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1120" t="n">
+        <v>71</v>
+      </c>
+      <c r="F1120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1120" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr"/>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>18:02</t>
+        </is>
+      </c>
+      <c r="D1121" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1121" t="n">
+        <v>74</v>
+      </c>
+      <c r="F1121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1121" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr"/>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D1122" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1122" t="n">
+        <v>76</v>
+      </c>
+      <c r="F1122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1122" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr"/>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="D1123" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1123" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1123" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr"/>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="D1124" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1124" t="n">
+        <v>99</v>
+      </c>
+      <c r="F1124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1124" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -34708,7 +35297,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34756,7 +35345,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:38:09</t>
+          <t>Última actualización: 31/12/2025 16:48:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -34769,7 +35358,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 74</t>
+          <t>Total filas: 75</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -37006,6 +37595,37 @@
         <v>88</v>
       </c>
       <c r="G75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>16:48:41</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>62</v>
+      </c>
+      <c r="G76" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -37022,7 +37642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37070,7 +37690,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:38:09</t>
+          <t>Última actualización: 31/12/2025 16:48:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -37083,7 +37703,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 135</t>
+          <t>Total filas: 136</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -41216,6 +41836,37 @@
         </is>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" t="inlineStr"/>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>16:48:46</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>9</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 19:59 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1124"/>
+  <dimension ref="A1:G1144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:48:51</t>
+          <t>Última actualización: 31/12/2025 16:59:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1123</t>
+          <t>Total filas: 1143</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -35281,6 +35281,626 @@
         </is>
       </c>
       <c r="G1124" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr"/>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>17:01</t>
+        </is>
+      </c>
+      <c r="D1125" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1125" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1125" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr"/>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>17:03</t>
+        </is>
+      </c>
+      <c r="D1126" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1126" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1126" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr"/>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="D1127" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1127" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1127" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr"/>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>17:13</t>
+        </is>
+      </c>
+      <c r="D1128" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1128" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1128" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr"/>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>17:23</t>
+        </is>
+      </c>
+      <c r="D1129" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1129" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1129" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr"/>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="D1130" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1130" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1130" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr"/>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>17:27</t>
+        </is>
+      </c>
+      <c r="D1131" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1131" t="n">
+        <v>29</v>
+      </c>
+      <c r="F1131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1131" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr"/>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>17:33</t>
+        </is>
+      </c>
+      <c r="D1132" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1132" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1132" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr"/>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="D1133" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1133" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1133" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr"/>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D1134" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1134" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1134" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr"/>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D1135" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1135" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1135" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr"/>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="D1136" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1136" t="n">
+        <v>49</v>
+      </c>
+      <c r="F1136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1136" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr"/>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="D1137" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1137" t="n">
+        <v>52</v>
+      </c>
+      <c r="F1137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1137" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr"/>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>17:54</t>
+        </is>
+      </c>
+      <c r="D1138" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1138" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1138" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr"/>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>17:59</t>
+        </is>
+      </c>
+      <c r="D1139" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1139" t="n">
+        <v>61</v>
+      </c>
+      <c r="F1139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1139" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr"/>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>18:01</t>
+        </is>
+      </c>
+      <c r="D1140" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1140" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1140" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr"/>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D1141" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1141" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1141" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr"/>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="D1142" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1142" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1142" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr"/>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="D1143" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1143" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1143" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr"/>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>18:33</t>
+        </is>
+      </c>
+      <c r="D1144" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1144" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1144" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -35297,7 +35917,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35345,7 +35965,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:48:51</t>
+          <t>Última actualización: 31/12/2025 16:59:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -35358,7 +35978,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 75</t>
+          <t>Total filas: 76</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -37626,6 +38246,37 @@
         <v>62</v>
       </c>
       <c r="G76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>16:58:55</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>52</v>
+      </c>
+      <c r="G77" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -37642,7 +38293,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37690,7 +38341,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:48:51</t>
+          <t>Última actualización: 31/12/2025 16:59:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -37703,7 +38354,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 136</t>
+          <t>Total filas: 138</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -41867,6 +42518,68 @@
         </is>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" t="inlineStr"/>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>16:59:01</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>17:01</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>2</v>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr"/>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>16:59:01</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>83</v>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 20:31 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1144"/>
+  <dimension ref="A1:G1163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:59:06</t>
+          <t>Última actualización: 31/12/2025 17:31:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1143</t>
+          <t>Total filas: 1162</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -35901,6 +35901,595 @@
         </is>
       </c>
       <c r="G1144" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr"/>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="D1145" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1145" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1145" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr"/>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D1146" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1146" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1146" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr"/>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="D1147" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1147" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1147" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr"/>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>17:47</t>
+        </is>
+      </c>
+      <c r="D1148" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1148" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1148" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr"/>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="D1149" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1149" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1149" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr"/>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>17:54</t>
+        </is>
+      </c>
+      <c r="D1150" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1150" t="n">
+        <v>23</v>
+      </c>
+      <c r="F1150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1150" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr"/>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>17:59</t>
+        </is>
+      </c>
+      <c r="D1151" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1151" t="n">
+        <v>28</v>
+      </c>
+      <c r="F1151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1151" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr"/>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="D1152" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1152" t="n">
+        <v>32</v>
+      </c>
+      <c r="F1152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1152" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr"/>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D1153" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1153" t="n">
+        <v>33</v>
+      </c>
+      <c r="F1153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1153" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr"/>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="D1154" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1154" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1154" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr"/>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="D1155" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1155" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1155" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr"/>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="D1156" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1156" t="n">
+        <v>59</v>
+      </c>
+      <c r="F1156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1156" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr"/>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="D1157" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1157" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1157" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr"/>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="D1158" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1158" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1158" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr"/>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="D1159" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1159" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1159" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr"/>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>18:51</t>
+        </is>
+      </c>
+      <c r="D1160" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1160" t="n">
+        <v>80</v>
+      </c>
+      <c r="F1160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1160" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr"/>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="D1161" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1161" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1161" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr"/>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>19:01</t>
+        </is>
+      </c>
+      <c r="D1162" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1162" t="n">
+        <v>90</v>
+      </c>
+      <c r="F1162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1162" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr"/>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="D1163" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1163" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1163" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -35917,7 +36506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35965,7 +36554,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:59:06</t>
+          <t>Última actualización: 31/12/2025 17:31:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -35978,7 +36567,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 76</t>
+          <t>Total filas: 77</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -38277,6 +38866,37 @@
         <v>52</v>
       </c>
       <c r="G77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>17:31:45</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>19</v>
+      </c>
+      <c r="G78" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -38293,7 +38913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38341,7 +38961,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 16:59:06</t>
+          <t>Última actualización: 31/12/2025 17:31:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -38354,7 +38974,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 138</t>
+          <t>Total filas: 139</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -42580,6 +43200,37 @@
         </is>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" t="inlineStr"/>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>17:31:50</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>50</v>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 20:50 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1163"/>
+  <dimension ref="A1:G1181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 17:31:55</t>
+          <t>Última actualización: 31/12/2025 17:50:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1162</t>
+          <t>Total filas: 1180</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -36490,6 +36490,564 @@
         </is>
       </c>
       <c r="G1163" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr"/>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>17:55</t>
+        </is>
+      </c>
+      <c r="D1164" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1164" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1164" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr"/>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D1165" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1165" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1165" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr"/>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D1166" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1166" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1166" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr"/>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="D1167" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1167" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1167" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr"/>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="D1168" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1168" t="n">
+        <v>32</v>
+      </c>
+      <c r="F1168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1168" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr"/>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D1169" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1169" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1169" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr"/>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="D1170" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1170" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1170" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr"/>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="D1171" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1171" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1171" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr"/>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="D1172" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1172" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1172" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr"/>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>18:42</t>
+        </is>
+      </c>
+      <c r="D1173" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1173" t="n">
+        <v>52</v>
+      </c>
+      <c r="F1173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1173" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr"/>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="D1174" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1174" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1174" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr"/>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="D1175" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1175" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1175" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr"/>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="D1176" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1176" t="n">
+        <v>69</v>
+      </c>
+      <c r="F1176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1176" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr"/>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D1177" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1177" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1177" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr"/>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>19:02</t>
+        </is>
+      </c>
+      <c r="D1178" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1178" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1178" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr"/>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>19:07</t>
+        </is>
+      </c>
+      <c r="D1179" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1179" t="n">
+        <v>77</v>
+      </c>
+      <c r="F1179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1179" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr"/>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>19:12</t>
+        </is>
+      </c>
+      <c r="D1180" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1180" t="n">
+        <v>82</v>
+      </c>
+      <c r="F1180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1180" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr"/>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D1181" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1181" t="n">
+        <v>91</v>
+      </c>
+      <c r="F1181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1181" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -36506,7 +37064,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36554,7 +37112,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 17:31:55</t>
+          <t>Última actualización: 31/12/2025 17:50:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -36567,7 +37125,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 77</t>
+          <t>Total filas: 78</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -38897,6 +39455,37 @@
         <v>19</v>
       </c>
       <c r="G78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>17:50:07</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>91</v>
+      </c>
+      <c r="G79" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -38913,7 +39502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:G142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38961,7 +39550,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 17:31:55</t>
+          <t>Última actualización: 31/12/2025 17:50:18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -38974,7 +39563,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 139</t>
+          <t>Total filas: 141</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -43231,6 +43820,68 @@
         </is>
       </c>
     </row>
+    <row r="141">
+      <c r="A141" t="inlineStr"/>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>17:50:13</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>32</v>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr"/>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>17:50:18</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>81</v>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 21:00 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1181"/>
+  <dimension ref="A1:G1201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 17:50:18</t>
+          <t>Última actualización: 31/12/2025 18:00:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1180</t>
+          <t>Total filas: 1200</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -37048,6 +37048,626 @@
         </is>
       </c>
       <c r="G1181" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr"/>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D1182" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1182" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1182" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr"/>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="D1183" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1183" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1183" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr"/>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="D1184" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1184" t="n">
+        <v>21</v>
+      </c>
+      <c r="F1184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1184" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr"/>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D1185" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1185" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1185" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr"/>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="D1186" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1186" t="n">
+        <v>27</v>
+      </c>
+      <c r="F1186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1186" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr"/>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>18:31</t>
+        </is>
+      </c>
+      <c r="D1187" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1187" t="n">
+        <v>31</v>
+      </c>
+      <c r="F1187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1187" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr"/>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="D1188" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1188" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1188" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr"/>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="D1189" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1189" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1189" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr"/>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="D1190" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1190" t="n">
+        <v>41</v>
+      </c>
+      <c r="F1190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1190" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr"/>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="D1191" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1191" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1191" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr"/>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>18:51</t>
+        </is>
+      </c>
+      <c r="D1192" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1192" t="n">
+        <v>51</v>
+      </c>
+      <c r="F1192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1192" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr"/>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>18:53</t>
+        </is>
+      </c>
+      <c r="D1193" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1193" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1193" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr"/>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="D1194" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1194" t="n">
+        <v>59</v>
+      </c>
+      <c r="F1194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1194" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr"/>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>19:01</t>
+        </is>
+      </c>
+      <c r="D1195" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1195" t="n">
+        <v>61</v>
+      </c>
+      <c r="F1195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1195" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr"/>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>19:02</t>
+        </is>
+      </c>
+      <c r="D1196" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1196" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1196" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr"/>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="D1197" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1197" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1197" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr"/>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="D1198" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1198" t="n">
+        <v>71</v>
+      </c>
+      <c r="F1198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1198" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr"/>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D1199" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1199" t="n">
+        <v>81</v>
+      </c>
+      <c r="F1199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1199" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr"/>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="D1200" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1200" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1200" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr"/>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="D1201" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1201" t="n">
+        <v>91</v>
+      </c>
+      <c r="F1201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1201" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -37064,7 +37684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37112,7 +37732,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 17:50:18</t>
+          <t>Última actualización: 31/12/2025 18:00:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -37125,7 +37745,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 78</t>
+          <t>Total filas: 80</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -39486,6 +40106,68 @@
         <v>91</v>
       </c>
       <c r="G79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>81</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>18:00:29</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>91</v>
+      </c>
+      <c r="G81" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -39502,7 +40184,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39550,7 +40232,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 17:50:18</t>
+          <t>Última actualización: 31/12/2025 18:00:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -39563,7 +40245,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 141</t>
+          <t>Total filas: 143</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -43882,6 +44564,68 @@
         </is>
       </c>
     </row>
+    <row r="143">
+      <c r="A143" t="inlineStr"/>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>18:00:35</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>22</v>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>18:00:40</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>71</v>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 21:27 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1201"/>
+  <dimension ref="A1:G1221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:00:40</t>
+          <t>Última actualización: 31/12/2025 18:27:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1200</t>
+          <t>Total filas: 1220</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -37668,6 +37668,626 @@
         </is>
       </c>
       <c r="G1201" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr"/>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>18:31</t>
+        </is>
+      </c>
+      <c r="D1202" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1202" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1202" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr"/>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>18:33</t>
+        </is>
+      </c>
+      <c r="D1203" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1203" t="n">
+        <v>6</v>
+      </c>
+      <c r="F1203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1203" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr"/>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="D1204" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1204" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1204" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr"/>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="D1205" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1205" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1205" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr"/>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>18:44</t>
+        </is>
+      </c>
+      <c r="D1206" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1206" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1206" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr"/>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>18:51</t>
+        </is>
+      </c>
+      <c r="D1207" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1207" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1207" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr"/>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>18:53</t>
+        </is>
+      </c>
+      <c r="D1208" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1208" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1208" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr"/>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>19:01</t>
+        </is>
+      </c>
+      <c r="D1209" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1209" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1209" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr"/>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="D1210" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1210" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1210" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr"/>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="D1211" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1211" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1211" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr"/>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="D1212" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1212" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1212" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr"/>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>19:14</t>
+        </is>
+      </c>
+      <c r="D1213" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1213" t="n">
+        <v>47</v>
+      </c>
+      <c r="F1213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1213" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr"/>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D1214" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1214" t="n">
+        <v>54</v>
+      </c>
+      <c r="F1214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1214" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr"/>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="D1215" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1215" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1215" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr"/>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="D1216" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1216" t="n">
+        <v>64</v>
+      </c>
+      <c r="F1216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1216" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr"/>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>19:32</t>
+        </is>
+      </c>
+      <c r="D1217" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1217" t="n">
+        <v>65</v>
+      </c>
+      <c r="F1217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1217" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr"/>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>19:44</t>
+        </is>
+      </c>
+      <c r="D1218" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1218" t="n">
+        <v>77</v>
+      </c>
+      <c r="F1218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1218" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr"/>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D1219" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1219" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1219" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr"/>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="D1220" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1220" t="n">
+        <v>92</v>
+      </c>
+      <c r="F1220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1220" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr"/>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="D1221" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1221" t="n">
+        <v>94</v>
+      </c>
+      <c r="F1221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1221" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -37684,7 +38304,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37732,7 +38352,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:00:40</t>
+          <t>Última actualización: 31/12/2025 18:27:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -37745,7 +38365,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 80</t>
+          <t>Total filas: 83</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -40168,6 +40788,99 @@
         <v>91</v>
       </c>
       <c r="G81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>54</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>64</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>18:27:23</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>94</v>
+      </c>
+      <c r="G84" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -40184,7 +40897,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40232,7 +40945,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:00:40</t>
+          <t>Última actualización: 31/12/2025 18:27:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -40245,7 +40958,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 143</t>
+          <t>Total filas: 144</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -44626,6 +45339,37 @@
         </is>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>18:27:33</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>44</v>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 21:42 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1221"/>
+  <dimension ref="A1:G1239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:27:34</t>
+          <t>Última actualización: 31/12/2025 18:42:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1220</t>
+          <t>Total filas: 1238</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -38288,6 +38288,564 @@
         </is>
       </c>
       <c r="G1221" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr"/>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="D1222" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1222" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1222" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr"/>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>18:54</t>
+        </is>
+      </c>
+      <c r="D1223" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1223" t="n">
+        <v>12</v>
+      </c>
+      <c r="F1223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1223" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr"/>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D1224" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1224" t="n">
+        <v>18</v>
+      </c>
+      <c r="F1224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1224" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr"/>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>19:02</t>
+        </is>
+      </c>
+      <c r="D1225" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1225" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1225" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr"/>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="D1226" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1226" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1226" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr"/>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="D1227" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1227" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1227" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr"/>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>19:15</t>
+        </is>
+      </c>
+      <c r="D1228" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1228" t="n">
+        <v>33</v>
+      </c>
+      <c r="F1228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1228" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr"/>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>19:18</t>
+        </is>
+      </c>
+      <c r="D1229" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1229" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1229" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr"/>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="D1230" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1230" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1230" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr"/>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>19:32</t>
+        </is>
+      </c>
+      <c r="D1231" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1231" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1231" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr"/>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>19:34</t>
+        </is>
+      </c>
+      <c r="D1232" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1232" t="n">
+        <v>52</v>
+      </c>
+      <c r="F1232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1232" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr"/>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="D1233" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1233" t="n">
+        <v>59</v>
+      </c>
+      <c r="F1233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1233" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr"/>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>19:45</t>
+        </is>
+      </c>
+      <c r="D1234" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1234" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1234" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr"/>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="D1235" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1235" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1235" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr"/>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="D1236" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1236" t="n">
+        <v>77</v>
+      </c>
+      <c r="F1236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1236" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr"/>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>20:02</t>
+        </is>
+      </c>
+      <c r="D1237" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1237" t="n">
+        <v>80</v>
+      </c>
+      <c r="F1237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1237" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr"/>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="D1238" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1238" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1238" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr"/>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>20:15</t>
+        </is>
+      </c>
+      <c r="D1239" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1239" t="n">
+        <v>93</v>
+      </c>
+      <c r="F1239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1239" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -38304,7 +38862,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38352,7 +38910,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:27:34</t>
+          <t>Última actualización: 31/12/2025 18:42:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -38365,7 +38923,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 83</t>
+          <t>Total filas: 86</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -40881,6 +41439,99 @@
         <v>94</v>
       </c>
       <c r="G84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>40</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>19:32</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>50</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>18:42:01</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>20:02</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>80</v>
+      </c>
+      <c r="G87" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -40897,7 +41548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40945,7 +41596,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:27:34</t>
+          <t>Última actualización: 31/12/2025 18:42:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -40958,7 +41609,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 144</t>
+          <t>Total filas: 145</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -45370,6 +46021,37 @@
         </is>
       </c>
     </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>29</v>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 21:55 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1239"/>
+  <dimension ref="A1:G1257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:42:12</t>
+          <t>Última actualización: 31/12/2025 18:55:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1238</t>
+          <t>Total filas: 1256</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -38846,6 +38846,564 @@
         </is>
       </c>
       <c r="G1239" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr"/>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>19:01</t>
+        </is>
+      </c>
+      <c r="D1240" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1240" t="n">
+        <v>6</v>
+      </c>
+      <c r="F1240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1240" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr"/>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="D1241" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1241" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1241" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr"/>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="D1242" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1242" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1242" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr"/>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="D1243" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1243" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1243" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr"/>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>19:14</t>
+        </is>
+      </c>
+      <c r="D1244" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1244" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1244" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr"/>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="D1245" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1245" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1245" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr"/>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="D1246" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1246" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1246" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr"/>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="D1247" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1247" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1247" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr"/>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="D1248" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1248" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1248" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr"/>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>19:33</t>
+        </is>
+      </c>
+      <c r="D1249" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1249" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1249" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr"/>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="D1250" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1250" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1250" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr"/>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>19:44</t>
+        </is>
+      </c>
+      <c r="D1251" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1251" t="n">
+        <v>49</v>
+      </c>
+      <c r="F1251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1251" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr"/>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D1252" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1252" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1252" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr"/>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="D1253" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1253" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1253" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr"/>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D1254" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1254" t="n">
+        <v>65</v>
+      </c>
+      <c r="F1254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1254" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr"/>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="D1255" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1255" t="n">
+        <v>75</v>
+      </c>
+      <c r="F1255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1255" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr"/>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>20:26</t>
+        </is>
+      </c>
+      <c r="D1256" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1256" t="n">
+        <v>91</v>
+      </c>
+      <c r="F1256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1256" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr"/>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="D1257" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1257" t="n">
+        <v>93</v>
+      </c>
+      <c r="F1257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1257" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -38862,7 +39420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38910,7 +39468,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:42:12</t>
+          <t>Última actualización: 31/12/2025 18:55:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -38923,7 +39481,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 86</t>
+          <t>Total filas: 88</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -41532,6 +42090,68 @@
         <v>80</v>
       </c>
       <c r="G87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>25</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>18:55:43</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>65</v>
+      </c>
+      <c r="G89" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -41548,7 +42168,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G146"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41596,7 +42216,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:42:12</t>
+          <t>Última actualización: 31/12/2025 18:55:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -41609,7 +42229,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 145</t>
+          <t>Total filas: 146</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -46052,6 +46672,37 @@
         </is>
       </c>
     </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>18:55:54</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>15</v>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 22:21 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1257"/>
+  <dimension ref="A1:G1273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:55:54</t>
+          <t>Última actualización: 31/12/2025 19:21:43</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1256</t>
+          <t>Total filas: 1272</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -39404,6 +39404,502 @@
         </is>
       </c>
       <c r="G1257" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr"/>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="D1258" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1258" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1258" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr"/>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="D1259" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1259" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1259" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr"/>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="D1260" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1260" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1260" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr"/>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>19:33</t>
+        </is>
+      </c>
+      <c r="D1261" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1261" t="n">
+        <v>12</v>
+      </c>
+      <c r="F1261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1261" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr"/>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="D1262" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1262" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1262" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr"/>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D1263" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1263" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1263" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr"/>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="D1264" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1264" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1264" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr"/>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="D1265" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1265" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1265" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr"/>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="D1266" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1266" t="n">
+        <v>49</v>
+      </c>
+      <c r="F1266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1266" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr"/>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>20:14</t>
+        </is>
+      </c>
+      <c r="D1267" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1267" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1267" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr"/>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>20:26</t>
+        </is>
+      </c>
+      <c r="D1268" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1268" t="n">
+        <v>65</v>
+      </c>
+      <c r="F1268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1268" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr"/>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="D1269" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1269" t="n">
+        <v>67</v>
+      </c>
+      <c r="F1269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1269" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr"/>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="D1270" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1270" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1270" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr"/>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D1271" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1271" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1271" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr"/>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>20:50</t>
+        </is>
+      </c>
+      <c r="D1272" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1272" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1272" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr"/>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>20:53</t>
+        </is>
+      </c>
+      <c r="D1273" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1273" t="n">
+        <v>92</v>
+      </c>
+      <c r="F1273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1273" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -39420,7 +39916,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39468,7 +39964,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:55:54</t>
+          <t>Última actualización: 31/12/2025 19:21:43</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -39481,7 +39977,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 88</t>
+          <t>Total filas: 91</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -42152,6 +42648,99 @@
         <v>65</v>
       </c>
       <c r="G89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>10</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>40</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>19:21:32</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>83</v>
+      </c>
+      <c r="G92" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -42168,7 +42757,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G147"/>
+  <dimension ref="A1:G148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42216,7 +42805,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 18:55:54</t>
+          <t>Última actualización: 31/12/2025 19:21:43</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -42229,7 +42818,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 146</t>
+          <t>Total filas: 147</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -46703,6 +47292,37 @@
         </is>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>19:21:38</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>20:41</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>80</v>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 22:44 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1273"/>
+  <dimension ref="A1:G1285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:21:43</t>
+          <t>Última actualización: 31/12/2025 19:44:59</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1272</t>
+          <t>Total filas: 1284</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -39900,6 +39900,378 @@
         </is>
       </c>
       <c r="G1273" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr"/>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D1274" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1274" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1274" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr"/>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="D1275" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1275" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1275" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr"/>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D1276" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1276" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1276" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr"/>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="D1277" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1277" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1277" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr"/>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="D1278" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1278" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1278" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr"/>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="D1279" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1279" t="n">
+        <v>27</v>
+      </c>
+      <c r="F1279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1279" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr"/>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>20:14</t>
+        </is>
+      </c>
+      <c r="D1280" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1280" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1280" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr"/>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>20:25</t>
+        </is>
+      </c>
+      <c r="D1281" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1281" t="n">
+        <v>41</v>
+      </c>
+      <c r="F1281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1281" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr"/>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="D1282" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1282" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1282" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr"/>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D1283" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1283" t="n">
+        <v>61</v>
+      </c>
+      <c r="F1283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1283" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr"/>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="D1284" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1284" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1284" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr"/>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="D1285" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1285" t="n">
+        <v>68</v>
+      </c>
+      <c r="F1285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1285" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -39916,7 +40288,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39964,7 +40336,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:21:43</t>
+          <t>Última actualización: 31/12/2025 19:44:59</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -39977,7 +40349,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 91</t>
+          <t>Total filas: 92</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -42741,6 +43113,37 @@
         <v>83</v>
       </c>
       <c r="G92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>19:44:48</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>16</v>
+      </c>
+      <c r="G93" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -42757,7 +43160,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G148"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42805,7 +43208,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:21:43</t>
+          <t>Última actualización: 31/12/2025 19:44:59</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -42818,7 +43221,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 147</t>
+          <t>Total filas: 148</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -47323,6 +47726,37 @@
         </is>
       </c>
     </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>19:44:53</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>20:41</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>57</v>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 22:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1285"/>
+  <dimension ref="A1:G1298"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:44:59</t>
+          <t>Última actualización: 31/12/2025 19:56:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1284</t>
+          <t>Total filas: 1297</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -40272,6 +40272,409 @@
         </is>
       </c>
       <c r="G1285" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr"/>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="D1286" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1286" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1286" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr"/>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D1287" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1287" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1287" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr"/>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="D1288" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1288" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1288" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr"/>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="D1289" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1289" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1289" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr"/>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="D1290" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1290" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1290" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr"/>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="D1291" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1291" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1291" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr"/>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>20:25</t>
+        </is>
+      </c>
+      <c r="D1292" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1292" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1292" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr"/>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="D1293" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1293" t="n">
+        <v>33</v>
+      </c>
+      <c r="F1293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1293" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr"/>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="D1294" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1294" t="n">
+        <v>49</v>
+      </c>
+      <c r="F1294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1294" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr"/>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>20:50</t>
+        </is>
+      </c>
+      <c r="D1295" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1295" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1295" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr"/>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="D1296" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1296" t="n">
+        <v>61</v>
+      </c>
+      <c r="F1296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1296" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr"/>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="D1297" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1297" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1297" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr"/>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>21:31</t>
+        </is>
+      </c>
+      <c r="D1298" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1298" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1298" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -40288,7 +40691,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40336,7 +40739,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:44:59</t>
+          <t>Última actualización: 31/12/2025 19:56:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -40349,7 +40752,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 92</t>
+          <t>Total filas: 93</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -43144,6 +43547,37 @@
         <v>16</v>
       </c>
       <c r="G93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>19:55:54</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>5</v>
+      </c>
+      <c r="G94" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -43160,7 +43594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G149"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43208,7 +43642,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:44:59</t>
+          <t>Última actualización: 31/12/2025 19:56:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -43221,7 +43655,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 148</t>
+          <t>Total filas: 150</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -47757,6 +48191,68 @@
         </is>
       </c>
     </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>19:55:59</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>20:41</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>46</v>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>19:55:59</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>21:33</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F151" t="n">
+        <v>98</v>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 23:20 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1298"/>
+  <dimension ref="A1:G1310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:56:04</t>
+          <t>Última actualización: 31/12/2025 20:20:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1297</t>
+          <t>Total filas: 1309</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -40675,6 +40675,378 @@
         </is>
       </c>
       <c r="G1298" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr"/>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>20:25</t>
+        </is>
+      </c>
+      <c r="D1299" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1299" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1299" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr"/>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="D1300" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1300" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1300" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr"/>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>20:36</t>
+        </is>
+      </c>
+      <c r="D1301" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1301" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1301" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr"/>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="D1302" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1302" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1302" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr"/>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D1303" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1303" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1303" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr"/>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>20:50</t>
+        </is>
+      </c>
+      <c r="D1304" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1304" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1304" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr"/>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="D1305" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1305" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1305" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr"/>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="D1306" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1306" t="n">
+        <v>61</v>
+      </c>
+      <c r="F1306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1306" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr"/>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="D1307" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1307" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1307" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr"/>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="D1308" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1308" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1308" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr"/>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>21:49</t>
+        </is>
+      </c>
+      <c r="D1309" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1309" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1309" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr"/>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>21:55</t>
+        </is>
+      </c>
+      <c r="D1310" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E1310" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1310" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -40691,7 +41063,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40739,7 +41111,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:56:04</t>
+          <t>Última actualización: 31/12/2025 20:20:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -40752,7 +41124,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 93</t>
+          <t>Total filas: 94</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -43578,6 +43950,37 @@
         <v>5</v>
       </c>
       <c r="G94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>20:20:46</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>24</v>
+      </c>
+      <c r="G95" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -43594,7 +43997,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43642,7 +44045,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 19:56:04</t>
+          <t>Última actualización: 31/12/2025 20:20:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -43655,7 +44058,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 150</t>
+          <t>Total filas: 152</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -48253,6 +48656,68 @@
         </is>
       </c>
     </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>20:20:52</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>20:41</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>21</v>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>20:20:52</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>21:33</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>73</v>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 23:41 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1310"/>
+  <dimension ref="A1:G1319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:20:57</t>
+          <t>Última actualización: 31/12/2025 20:41:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1309</t>
+          <t>Total filas: 1318</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -41047,6 +41047,285 @@
         </is>
       </c>
       <c r="G1310" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr"/>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="D1311" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1311" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1311" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr"/>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>20:50</t>
+        </is>
+      </c>
+      <c r="D1312" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1312" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1312" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr"/>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="D1313" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1313" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1313" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr"/>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="D1314" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1314" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1314" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr"/>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>21:24</t>
+        </is>
+      </c>
+      <c r="D1315" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1315" t="n">
+        <v>43</v>
+      </c>
+      <c r="F1315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1315" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr"/>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="D1316" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1316" t="n">
+        <v>49</v>
+      </c>
+      <c r="F1316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1316" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr"/>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>21:41</t>
+        </is>
+      </c>
+      <c r="D1317" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1317" t="n">
+        <v>60</v>
+      </c>
+      <c r="F1317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1317" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr"/>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>21:49</t>
+        </is>
+      </c>
+      <c r="D1318" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1318" t="n">
+        <v>68</v>
+      </c>
+      <c r="F1318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1318" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr"/>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>20:41:17</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>21:56</t>
+        </is>
+      </c>
+      <c r="D1319" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E1319" t="n">
+        <v>75</v>
+      </c>
+      <c r="F1319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1319" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -41111,7 +41390,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:20:57</t>
+          <t>Última actualización: 31/12/2025 20:41:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -43997,7 +44276,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44045,7 +44324,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:20:57</t>
+          <t>Última actualización: 31/12/2025 20:41:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44058,7 +44337,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 152</t>
+          <t>Total filas: 155</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -48718,6 +48997,99 @@
         </is>
       </c>
     </row>
+    <row r="154">
+      <c r="A154" t="inlineStr"/>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>20:41:22</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>20:43</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>2</v>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>20:41:22</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F155" t="n">
+        <v>53</v>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>20:41:28</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>22:13</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>92</v>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 31/12 23:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1319"/>
+  <dimension ref="A1:G1329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:41:28</t>
+          <t>Última actualización: 31/12/2025 20:56:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1318</t>
+          <t>Total filas: 1328</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -41326,6 +41326,316 @@
         </is>
       </c>
       <c r="G1319" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr"/>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="D1320" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1320" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1320" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr"/>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="D1321" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1321" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1321" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr"/>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>21:41</t>
+        </is>
+      </c>
+      <c r="D1322" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1322" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1322" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr"/>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>21:41</t>
+        </is>
+      </c>
+      <c r="D1323" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1323" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1323" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr"/>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>21:49</t>
+        </is>
+      </c>
+      <c r="D1324" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1324" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1324" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr"/>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>21:56</t>
+        </is>
+      </c>
+      <c r="D1325" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="E1325" t="n">
+        <v>60</v>
+      </c>
+      <c r="F1325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1325" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr"/>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="D1326" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1326" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1326" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr"/>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>22:24</t>
+        </is>
+      </c>
+      <c r="D1327" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1327" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1327" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr"/>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>22:26</t>
+        </is>
+      </c>
+      <c r="D1328" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1328" t="n">
+        <v>90</v>
+      </c>
+      <c r="F1328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1328" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr"/>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>22:31</t>
+        </is>
+      </c>
+      <c r="D1329" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1329" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1329" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -41342,7 +41652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41390,7 +41700,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:41:28</t>
+          <t>Última actualización: 31/12/2025 20:56:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -41403,7 +41713,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 94</t>
+          <t>Total filas: 95</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -44260,6 +44570,37 @@
         <v>24</v>
       </c>
       <c r="G95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>20:56:13</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>22:31</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>95</v>
+      </c>
+      <c r="G96" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -44276,7 +44617,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G156"/>
+  <dimension ref="A1:G158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44324,7 +44665,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:41:28</t>
+          <t>Última actualización: 31/12/2025 20:56:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44337,7 +44678,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 155</t>
+          <t>Total filas: 157</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -49090,6 +49431,68 @@
         </is>
       </c>
     </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>20:56:19</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F157" t="n">
+        <v>38</v>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>20:56:24</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>22:13</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>77</v>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 02:00 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1329"/>
+  <dimension ref="A1:G1330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:56:24</t>
+          <t>Última actualización: 31/12/2025 23:00:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1328</t>
+          <t>Total filas: 1329</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -41636,6 +41636,37 @@
         </is>
       </c>
       <c r="G1329" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr"/>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>23:00:38</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>23:24</t>
+        </is>
+      </c>
+      <c r="D1330" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1330" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1330" t="inlineStr">
         <is>
           <t>31/12/2025</t>
         </is>
@@ -41700,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:56:24</t>
+          <t>Última actualización: 31/12/2025 23:00:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44665,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 20:56:24</t>
+          <t>Última actualización: 31/12/2025 23:00:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 03:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 23:00:49</t>
+          <t>Última actualización: 01/01/2026 00:56:53</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -41731,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 23:00:49</t>
+          <t>Última actualización: 01/01/2026 00:56:53</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 31/12/2025 23:00:49</t>
+          <t>Última actualización: 01/01/2026 00:56:53</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 04:51 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 00:56:53</t>
+          <t>Última actualización: 01/01/2026 01:51:23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -41731,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 00:56:53</t>
+          <t>Última actualización: 01/01/2026 01:51:23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 00:56:53</t>
+          <t>Última actualización: 01/01/2026 01:51:23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 05:28 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 01:51:23</t>
+          <t>Última actualización: 01/01/2026 02:28:01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -41731,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 01:51:23</t>
+          <t>Última actualización: 01/01/2026 02:28:01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 01:51:23</t>
+          <t>Última actualización: 01/01/2026 02:28:01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 05:51 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 02:28:01</t>
+          <t>Última actualización: 01/01/2026 02:51:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -41731,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 02:28:01</t>
+          <t>Última actualización: 01/01/2026 02:51:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 02:28:01</t>
+          <t>Última actualización: 01/01/2026 02:51:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 06:34 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 02:51:00</t>
+          <t>Última actualización: 01/01/2026 03:34:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -41731,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 02:51:00</t>
+          <t>Última actualización: 01/01/2026 03:34:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 02:51:00</t>
+          <t>Última actualización: 01/01/2026 03:34:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 07:00 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 03:34:15</t>
+          <t>Última actualización: 01/01/2026 04:00:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -41731,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 03:34:15</t>
+          <t>Última actualización: 01/01/2026 04:00:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 03:34:15</t>
+          <t>Última actualización: 01/01/2026 04:00:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 07:31 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:00:05</t>
+          <t>Última actualización: 01/01/2026 04:31:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -41731,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:00:05</t>
+          <t>Última actualización: 01/01/2026 04:31:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:00:05</t>
+          <t>Última actualización: 01/01/2026 04:31:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 07:48 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:31:38</t>
+          <t>Última actualización: 01/01/2026 04:48:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -41731,7 +41731,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:31:38</t>
+          <t>Última actualización: 01/01/2026 04:48:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44696,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:31:38</t>
+          <t>Última actualización: 01/01/2026 04:48:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 07:59 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1330"/>
+  <dimension ref="A1:G1331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:48:51</t>
+          <t>Última actualización: 01/01/2026 04:59:21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1329</t>
+          <t>Total filas: 1330</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -41669,6 +41669,37 @@
       <c r="G1330" t="inlineStr">
         <is>
           <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr"/>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>04:59:11</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="D1331" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1331" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1331" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
         </is>
       </c>
     </row>
@@ -41731,7 +41762,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:48:51</t>
+          <t>Última actualización: 01/01/2026 04:59:21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44696,7 +44727,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:48:51</t>
+          <t>Última actualización: 01/01/2026 04:59:21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 08:39 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1331"/>
+  <dimension ref="A1:G1333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:59:21</t>
+          <t>Última actualización: 01/01/2026 05:39:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1330</t>
+          <t>Total filas: 1332</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -41698,6 +41698,68 @@
         </is>
       </c>
       <c r="G1331" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr"/>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>05:39:23</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="D1332" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1332" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1332" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr"/>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>05:39:23</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>06:41</t>
+        </is>
+      </c>
+      <c r="D1333" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1333" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1333" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -41762,7 +41824,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:59:21</t>
+          <t>Última actualización: 01/01/2026 05:39:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44727,7 +44789,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 04:59:21</t>
+          <t>Última actualización: 01/01/2026 05:39:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 08:58 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1333"/>
+  <dimension ref="A1:G1336"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 05:39:34</t>
+          <t>Última actualización: 01/01/2026 05:58:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1332</t>
+          <t>Total filas: 1335</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -41760,6 +41760,99 @@
         </is>
       </c>
       <c r="G1333" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr"/>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>05:58:41</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="D1334" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1334" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1334" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr"/>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>05:58:41</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>06:41</t>
+        </is>
+      </c>
+      <c r="D1335" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1335" t="n">
+        <v>43</v>
+      </c>
+      <c r="F1335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1335" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr"/>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>05:58:41</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>07:18</t>
+        </is>
+      </c>
+      <c r="D1336" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1336" t="n">
+        <v>80</v>
+      </c>
+      <c r="F1336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1336" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -41824,7 +41917,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 05:39:34</t>
+          <t>Última actualización: 01/01/2026 05:58:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44789,7 +44882,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 05:39:34</t>
+          <t>Última actualización: 01/01/2026 05:58:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 09:34 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1336"/>
+  <dimension ref="A1:G1343"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 05:58:51</t>
+          <t>Última actualización: 01/01/2026 06:34:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1335</t>
+          <t>Total filas: 1342</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -41853,6 +41853,223 @@
         </is>
       </c>
       <c r="G1336" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr"/>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>06:33:50</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>06:40</t>
+        </is>
+      </c>
+      <c r="D1337" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1337" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1337" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr"/>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>06:33:50</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>07:18</t>
+        </is>
+      </c>
+      <c r="D1338" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1338" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1338" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr"/>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>06:33:50</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>07:19</t>
+        </is>
+      </c>
+      <c r="D1339" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1339" t="n">
+        <v>46</v>
+      </c>
+      <c r="F1339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1339" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr"/>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>06:33:50</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>07:23</t>
+        </is>
+      </c>
+      <c r="D1340" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1340" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1340" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr"/>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>06:33:50</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="D1341" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1341" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1341" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr"/>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>06:33:50</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="D1342" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1342" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1342" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr"/>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>06:33:50</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="D1343" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1343" t="n">
+        <v>98</v>
+      </c>
+      <c r="F1343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1343" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -41917,7 +42134,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 05:58:51</t>
+          <t>Última actualización: 01/01/2026 06:34:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44834,7 +45051,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44882,7 +45099,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 05:58:51</t>
+          <t>Última actualización: 01/01/2026 06:34:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44895,7 +45112,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 157</t>
+          <t>Total filas: 158</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -49710,6 +49927,37 @@
         </is>
       </c>
     </row>
+    <row r="159">
+      <c r="A159" t="inlineStr"/>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>06:34:00</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>07:41</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
+        <v>67</v>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 09:51 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1343"/>
+  <dimension ref="A1:G1350"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 06:34:00</t>
+          <t>Última actualización: 01/01/2026 06:51:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1342</t>
+          <t>Total filas: 1349</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -42070,6 +42070,223 @@
         </is>
       </c>
       <c r="G1343" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr"/>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>06:50:55</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>07:18</t>
+        </is>
+      </c>
+      <c r="D1344" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1344" t="n">
+        <v>28</v>
+      </c>
+      <c r="F1344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1344" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr"/>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>06:50:55</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>07:20</t>
+        </is>
+      </c>
+      <c r="D1345" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1345" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1345" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr"/>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>06:50:55</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>07:34</t>
+        </is>
+      </c>
+      <c r="D1346" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1346" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1346" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr"/>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>06:50:55</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>07:54</t>
+        </is>
+      </c>
+      <c r="D1347" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1347" t="n">
+        <v>64</v>
+      </c>
+      <c r="F1347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1347" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr"/>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>06:50:55</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D1348" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1348" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1348" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr"/>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>06:50:55</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="D1349" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1349" t="n">
+        <v>81</v>
+      </c>
+      <c r="F1349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1349" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr"/>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>06:50:55</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>08:28</t>
+        </is>
+      </c>
+      <c r="D1350" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1350" t="n">
+        <v>98</v>
+      </c>
+      <c r="F1350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1350" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -42134,7 +42351,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 06:34:00</t>
+          <t>Última actualización: 01/01/2026 06:51:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45051,7 +45268,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45099,7 +45316,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 06:34:00</t>
+          <t>Última actualización: 01/01/2026 06:51:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45112,7 +45329,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 158</t>
+          <t>Total filas: 159</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -49958,6 +50175,37 @@
         </is>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="inlineStr"/>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>06:51:06</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>07:42</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F160" t="n">
+        <v>51</v>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 10:23 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1350"/>
+  <dimension ref="A1:G1359"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 06:51:06</t>
+          <t>Última actualización: 01/01/2026 07:23:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1349</t>
+          <t>Total filas: 1358</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -42287,6 +42287,285 @@
         </is>
       </c>
       <c r="G1350" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr"/>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>07:34</t>
+        </is>
+      </c>
+      <c r="D1351" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1351" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1351" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr"/>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="D1352" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1352" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1352" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr"/>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>07:55</t>
+        </is>
+      </c>
+      <c r="D1353" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1353" t="n">
+        <v>32</v>
+      </c>
+      <c r="F1353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1353" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr"/>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>07:58</t>
+        </is>
+      </c>
+      <c r="D1354" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1354" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1354" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr"/>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="D1355" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1355" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1355" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr"/>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="D1356" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1356" t="n">
+        <v>48</v>
+      </c>
+      <c r="F1356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1356" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr"/>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="D1357" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1357" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1357" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr"/>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="D1358" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1358" t="n">
+        <v>78</v>
+      </c>
+      <c r="F1358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1358" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr"/>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>07:23:19</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>08:50</t>
+        </is>
+      </c>
+      <c r="D1359" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1359" t="n">
+        <v>87</v>
+      </c>
+      <c r="F1359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1359" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -42351,7 +42630,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 06:51:06</t>
+          <t>Última actualización: 01/01/2026 07:23:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45268,7 +45547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G160"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45316,7 +45595,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 06:51:06</t>
+          <t>Última actualización: 01/01/2026 07:23:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45329,7 +45608,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 159</t>
+          <t>Total filas: 162</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -50206,6 +50485,99 @@
         </is>
       </c>
     </row>
+    <row r="161">
+      <c r="A161" t="inlineStr"/>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>07:23:29</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>14</v>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr"/>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>07:23:29</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
+        <v>81</v>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr"/>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>07:23:24</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F163" t="n">
+        <v>99</v>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 10:47 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1359"/>
+  <dimension ref="A1:G1370"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:23:29</t>
+          <t>Última actualización: 01/01/2026 07:47:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1358</t>
+          <t>Total filas: 1369</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -42566,6 +42566,347 @@
         </is>
       </c>
       <c r="G1359" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr"/>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>07:55</t>
+        </is>
+      </c>
+      <c r="D1360" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1360" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1360" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr"/>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>07:58</t>
+        </is>
+      </c>
+      <c r="D1361" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1361" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1361" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr"/>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="D1362" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1362" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1362" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr"/>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="D1363" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1363" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1363" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr"/>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="D1364" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1364" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1364" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1364" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr"/>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="D1365" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1365" t="n">
+        <v>42</v>
+      </c>
+      <c r="F1365" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1365" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr"/>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="D1366" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1366" t="n">
+        <v>54</v>
+      </c>
+      <c r="F1366" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1366" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr"/>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>08:49</t>
+        </is>
+      </c>
+      <c r="D1367" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1367" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1367" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1367" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr"/>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="D1368" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1368" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1368" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1368" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr"/>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D1369" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1369" t="n">
+        <v>90</v>
+      </c>
+      <c r="F1369" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1369" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr"/>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>07:47:17</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D1370" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1370" t="n">
+        <v>90</v>
+      </c>
+      <c r="F1370" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1370" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -42630,7 +42971,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:23:29</t>
+          <t>Última actualización: 01/01/2026 07:47:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45547,7 +45888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G163"/>
+  <dimension ref="A1:G166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45595,7 +45936,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:23:29</t>
+          <t>Última actualización: 01/01/2026 07:47:28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45608,7 +45949,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 162</t>
+          <t>Total filas: 165</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -50578,6 +50919,99 @@
         </is>
       </c>
     </row>
+    <row r="164">
+      <c r="A164" t="inlineStr"/>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>07:47:27</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>57</v>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr"/>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>07:47:22</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F165" t="n">
+        <v>75</v>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr"/>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>07:47:27</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>93</v>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 10:58 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1370"/>
+  <dimension ref="A1:G1379"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:47:28</t>
+          <t>Última actualización: 01/01/2026 07:58:10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1369</t>
+          <t>Total filas: 1378</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -42907,6 +42907,285 @@
         </is>
       </c>
       <c r="G1370" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr"/>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D1371" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1371" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1371" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1371" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr"/>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>08:07</t>
+        </is>
+      </c>
+      <c r="D1372" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1372" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1372" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1372" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr"/>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="D1373" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1373" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1373" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1373" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr"/>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>08:28</t>
+        </is>
+      </c>
+      <c r="D1374" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1374" t="n">
+        <v>31</v>
+      </c>
+      <c r="F1374" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1374" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr"/>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="D1375" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1375" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1375" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1375" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr"/>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>08:45</t>
+        </is>
+      </c>
+      <c r="D1376" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1376" t="n">
+        <v>48</v>
+      </c>
+      <c r="F1376" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1376" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr"/>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="D1377" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1377" t="n">
+        <v>69</v>
+      </c>
+      <c r="F1377" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1377" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr"/>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>09:12</t>
+        </is>
+      </c>
+      <c r="D1378" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1378" t="n">
+        <v>75</v>
+      </c>
+      <c r="F1378" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1378" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr"/>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>07:57:59</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D1379" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1379" t="n">
+        <v>80</v>
+      </c>
+      <c r="F1379" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1379" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -42971,7 +43250,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:47:28</t>
+          <t>Última actualización: 01/01/2026 07:58:10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45888,7 +46167,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G166"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45936,7 +46215,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:47:28</t>
+          <t>Última actualización: 01/01/2026 07:58:10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45949,7 +46228,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 165</t>
+          <t>Total filas: 168</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -51012,6 +51291,99 @@
         </is>
       </c>
     </row>
+    <row r="167">
+      <c r="A167" t="inlineStr"/>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>07:58:10</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>46</v>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr"/>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>07:58:05</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F168" t="n">
+        <v>64</v>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr"/>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>07:58:10</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F169" t="n">
+        <v>82</v>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 11:24 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1379"/>
+  <dimension ref="A1:G1389"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:58:10</t>
+          <t>Última actualización: 01/01/2026 08:24:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1378</t>
+          <t>Total filas: 1388</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -43186,6 +43186,316 @@
         </is>
       </c>
       <c r="G1379" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr"/>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>08:26</t>
+        </is>
+      </c>
+      <c r="D1380" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1380" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1380" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1380" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr"/>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="D1381" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1381" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1381" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1381" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr"/>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="D1382" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1382" t="n">
+        <v>28</v>
+      </c>
+      <c r="F1382" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1382" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr"/>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>09:05</t>
+        </is>
+      </c>
+      <c r="D1383" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1383" t="n">
+        <v>41</v>
+      </c>
+      <c r="F1383" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1383" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr"/>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D1384" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1384" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1384" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1384" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr"/>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D1385" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1385" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1385" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1385" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr"/>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>09:37</t>
+        </is>
+      </c>
+      <c r="D1386" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1386" t="n">
+        <v>73</v>
+      </c>
+      <c r="F1386" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1386" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr"/>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>09:38</t>
+        </is>
+      </c>
+      <c r="D1387" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1387" t="n">
+        <v>74</v>
+      </c>
+      <c r="F1387" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1387" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr"/>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="D1388" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1388" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1388" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1388" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr"/>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="D1389" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1389" t="n">
+        <v>94</v>
+      </c>
+      <c r="F1389" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1389" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -43202,7 +43512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43250,7 +43560,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:58:10</t>
+          <t>Última actualización: 01/01/2026 08:24:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -43263,7 +43573,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 95</t>
+          <t>Total filas: 96</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -46151,6 +46461,37 @@
         <v>95</v>
       </c>
       <c r="G96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>08:24:02</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>09:38</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>74</v>
+      </c>
+      <c r="G97" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -46167,7 +46508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G169"/>
+  <dimension ref="A1:G172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46215,7 +46556,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 07:58:10</t>
+          <t>Última actualización: 01/01/2026 08:24:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -46228,7 +46569,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 168</t>
+          <t>Total filas: 171</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -51384,6 +51725,99 @@
         </is>
       </c>
     </row>
+    <row r="170">
+      <c r="A170" t="inlineStr"/>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>08:24:13</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F170" t="n">
+        <v>20</v>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr"/>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>08:24:07</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F171" t="n">
+        <v>38</v>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr"/>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>08:24:13</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F172" t="n">
+        <v>56</v>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 11:40 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1389"/>
+  <dimension ref="A1:G1400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:24:13</t>
+          <t>Última actualización: 01/01/2026 08:40:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1388</t>
+          <t>Total filas: 1399</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -43496,6 +43496,347 @@
         </is>
       </c>
       <c r="G1389" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr"/>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>08:52</t>
+        </is>
+      </c>
+      <c r="D1390" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1390" t="n">
+        <v>12</v>
+      </c>
+      <c r="F1390" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1390" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr"/>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>09:05</t>
+        </is>
+      </c>
+      <c r="D1391" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1391" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1391" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1391" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr"/>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="D1392" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1392" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1392" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1392" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr"/>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D1393" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1393" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1393" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1393" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr"/>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D1394" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1394" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1394" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1394" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr"/>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>09:38</t>
+        </is>
+      </c>
+      <c r="D1395" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1395" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1395" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1395" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr"/>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>09:38</t>
+        </is>
+      </c>
+      <c r="D1396" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1396" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1396" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1396" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr"/>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="D1397" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1397" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1397" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1397" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr"/>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="D1398" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1398" t="n">
+        <v>73</v>
+      </c>
+      <c r="F1398" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1398" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr"/>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>09:56</t>
+        </is>
+      </c>
+      <c r="D1399" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1399" t="n">
+        <v>76</v>
+      </c>
+      <c r="F1399" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1399" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr"/>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>10:18</t>
+        </is>
+      </c>
+      <c r="D1400" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1400" t="n">
+        <v>98</v>
+      </c>
+      <c r="F1400" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1400" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -43512,7 +43853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43560,7 +43901,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:24:13</t>
+          <t>Última actualización: 01/01/2026 08:40:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -43573,7 +43914,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 96</t>
+          <t>Total filas: 97</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -46492,6 +46833,37 @@
         <v>74</v>
       </c>
       <c r="G97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>08:40:04</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>09:38</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>58</v>
+      </c>
+      <c r="G98" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -46508,7 +46880,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G172"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46556,7 +46928,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:24:13</t>
+          <t>Última actualización: 01/01/2026 08:40:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -46569,7 +46941,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 171</t>
+          <t>Total filas: 174</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -51818,6 +52190,99 @@
         </is>
       </c>
     </row>
+    <row r="173">
+      <c r="A173" t="inlineStr"/>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>08:40:15</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F173" t="n">
+        <v>4</v>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr"/>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>08:40:10</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>09:02</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F174" t="n">
+        <v>22</v>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr"/>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>08:40:15</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F175" t="n">
+        <v>40</v>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 11:50 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1400"/>
+  <dimension ref="A1:G1412"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:40:15</t>
+          <t>Última actualización: 01/01/2026 08:50:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1399</t>
+          <t>Total filas: 1411</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -43837,6 +43837,378 @@
         </is>
       </c>
       <c r="G1400" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr"/>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>09:05</t>
+        </is>
+      </c>
+      <c r="D1401" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1401" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1401" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1401" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr"/>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="D1402" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1402" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1402" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1402" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr"/>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="D1403" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1403" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1403" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1403" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr"/>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="D1404" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1404" t="n">
+        <v>27</v>
+      </c>
+      <c r="F1404" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1404" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr"/>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>09:35</t>
+        </is>
+      </c>
+      <c r="D1405" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1405" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1405" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1405" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr"/>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>09:37</t>
+        </is>
+      </c>
+      <c r="D1406" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1406" t="n">
+        <v>47</v>
+      </c>
+      <c r="F1406" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1406" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr"/>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="D1407" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1407" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1407" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1407" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr"/>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="D1408" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1408" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1408" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1408" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr"/>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>09:57</t>
+        </is>
+      </c>
+      <c r="D1409" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1409" t="n">
+        <v>67</v>
+      </c>
+      <c r="F1409" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1409" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr"/>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>10:18</t>
+        </is>
+      </c>
+      <c r="D1410" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1410" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1410" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1410" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr"/>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>10:19</t>
+        </is>
+      </c>
+      <c r="D1411" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1411" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1411" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1411" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr"/>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>10:25</t>
+        </is>
+      </c>
+      <c r="D1412" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1412" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1412" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1412" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -43853,7 +44225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43901,7 +44273,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:40:15</t>
+          <t>Última actualización: 01/01/2026 08:50:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -43914,7 +44286,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 97</t>
+          <t>Total filas: 98</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -46864,6 +47236,37 @@
         <v>58</v>
       </c>
       <c r="G98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>08:50:44</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>09:37</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>47</v>
+      </c>
+      <c r="G99" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -46880,7 +47283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46928,7 +47331,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:40:15</t>
+          <t>Última actualización: 01/01/2026 08:50:55</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -46941,7 +47344,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 174</t>
+          <t>Total filas: 176</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -52283,6 +52686,68 @@
         </is>
       </c>
     </row>
+    <row r="176">
+      <c r="A176" t="inlineStr"/>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>08:50:49</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F176" t="n">
+        <v>11</v>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr"/>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>08:50:54</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>09:19</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F177" t="n">
+        <v>29</v>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 12:42 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1412"/>
+  <dimension ref="A1:G1425"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:50:55</t>
+          <t>Última actualización: 01/01/2026 09:42:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1411</t>
+          <t>Total filas: 1424</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -44209,6 +44209,409 @@
         </is>
       </c>
       <c r="G1412" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr"/>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="D1413" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1413" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1413" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1413" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr"/>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>09:57</t>
+        </is>
+      </c>
+      <c r="D1414" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1414" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1414" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1414" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr"/>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>10:18</t>
+        </is>
+      </c>
+      <c r="D1415" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1415" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1415" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1415" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr"/>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="D1416" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1416" t="n">
+        <v>39</v>
+      </c>
+      <c r="F1416" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1416" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr"/>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="D1417" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1417" t="n">
+        <v>47</v>
+      </c>
+      <c r="F1417" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1417" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr"/>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>10:38</t>
+        </is>
+      </c>
+      <c r="D1418" t="inlineStr">
+        <is>
+          <t>15_P INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="E1418" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1418" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1418" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr"/>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="D1419" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1419" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1419" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1419" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr"/>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>10:49</t>
+        </is>
+      </c>
+      <c r="D1420" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1420" t="n">
+        <v>67</v>
+      </c>
+      <c r="F1420" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1420" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr"/>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>10:52</t>
+        </is>
+      </c>
+      <c r="D1421" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1421" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1421" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1421" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr"/>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>11:05</t>
+        </is>
+      </c>
+      <c r="D1422" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1422" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1422" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1422" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr"/>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="D1423" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1423" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1423" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1423" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr"/>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="D1424" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1424" t="n">
+        <v>93</v>
+      </c>
+      <c r="F1424" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1424" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr"/>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>09:42:26</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="D1425" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1425" t="n">
+        <v>97</v>
+      </c>
+      <c r="F1425" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1425" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -44273,7 +44676,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:50:55</t>
+          <t>Última actualización: 01/01/2026 09:42:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -47283,7 +47686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G177"/>
+  <dimension ref="A1:G178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47331,7 +47734,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 08:50:55</t>
+          <t>Última actualización: 01/01/2026 09:42:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -47344,7 +47747,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 176</t>
+          <t>Total filas: 177</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -52748,6 +53151,37 @@
         </is>
       </c>
     </row>
+    <row r="178">
+      <c r="A178" t="inlineStr"/>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>09:42:36</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>10:31</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F178" t="n">
+        <v>49</v>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 13:25 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1425"/>
+  <dimension ref="A1:G1440"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 09:42:36</t>
+          <t>Última actualización: 01/01/2026 10:25:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1424</t>
+          <t>Total filas: 1439</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -44612,6 +44612,471 @@
         </is>
       </c>
       <c r="G1425" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr"/>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="D1426" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1426" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1426" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1426" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr"/>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>10:38</t>
+        </is>
+      </c>
+      <c r="D1427" t="inlineStr">
+        <is>
+          <t>15_P INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="E1427" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1427" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1427" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr"/>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="D1428" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1428" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1428" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1428" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr"/>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>10:51</t>
+        </is>
+      </c>
+      <c r="D1429" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1429" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1429" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1429" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr"/>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="D1430" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1430" t="n">
+        <v>32</v>
+      </c>
+      <c r="F1430" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1430" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr"/>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="D1431" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1431" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1431" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1431" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr"/>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>11:05</t>
+        </is>
+      </c>
+      <c r="D1432" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1432" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1432" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1432" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr"/>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>11:09</t>
+        </is>
+      </c>
+      <c r="D1433" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1433" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1433" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1433" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr"/>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="D1434" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1434" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1434" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1434" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr"/>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="D1435" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1435" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1435" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1435" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr"/>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="D1436" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1436" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1436" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1436" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr"/>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>11:29</t>
+        </is>
+      </c>
+      <c r="D1437" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1437" t="n">
+        <v>64</v>
+      </c>
+      <c r="F1437" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1437" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr"/>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="D1438" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1438" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1438" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1438" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr"/>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="D1439" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1439" t="n">
+        <v>87</v>
+      </c>
+      <c r="F1439" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1439" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr"/>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="D1440" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1440" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1440" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1440" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -44628,7 +45093,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44676,7 +45141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 09:42:36</t>
+          <t>Última actualización: 01/01/2026 10:25:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -44689,7 +45154,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 98</t>
+          <t>Total filas: 99</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -47670,6 +48135,37 @@
         <v>47</v>
       </c>
       <c r="G99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>10:25:08</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>66</v>
+      </c>
+      <c r="G100" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -47686,7 +48182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G178"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47734,7 +48230,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 09:42:36</t>
+          <t>Última actualización: 01/01/2026 10:25:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -47747,7 +48243,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 177</t>
+          <t>Total filas: 180</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -53182,6 +53678,99 @@
         </is>
       </c>
     </row>
+    <row r="179">
+      <c r="A179" t="inlineStr"/>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>10:25:18</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>10:28</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>3</v>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr"/>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>10:25:18</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F180" t="n">
+        <v>5</v>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr"/>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>10:25:13</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F181" t="n">
+        <v>61</v>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 13:51 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1440"/>
+  <dimension ref="A1:G1453"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 10:25:19</t>
+          <t>Última actualización: 01/01/2026 10:51:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1439</t>
+          <t>Total filas: 1452</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -45077,6 +45077,409 @@
         </is>
       </c>
       <c r="G1440" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr"/>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>10:53</t>
+        </is>
+      </c>
+      <c r="D1441" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1441" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1441" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1441" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr"/>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="D1442" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1442" t="n">
+        <v>6</v>
+      </c>
+      <c r="F1442" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1442" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr"/>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>10:58</t>
+        </is>
+      </c>
+      <c r="D1443" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1443" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1443" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1443" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr"/>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>11:07</t>
+        </is>
+      </c>
+      <c r="D1444" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1444" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1444" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1444" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr"/>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="D1445" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1445" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1445" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1445" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr"/>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="D1446" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1446" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1446" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1446" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr"/>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>11:28</t>
+        </is>
+      </c>
+      <c r="D1447" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1447" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1447" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1447" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr"/>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D1448" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1448" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1448" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1448" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr"/>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>11:54</t>
+        </is>
+      </c>
+      <c r="D1449" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1449" t="n">
+        <v>64</v>
+      </c>
+      <c r="F1449" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1449" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr"/>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="D1450" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1450" t="n">
+        <v>71</v>
+      </c>
+      <c r="F1450" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1450" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr"/>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>12:05</t>
+        </is>
+      </c>
+      <c r="D1451" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1451" t="n">
+        <v>75</v>
+      </c>
+      <c r="F1451" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1451" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr"/>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="D1452" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1452" t="n">
+        <v>85</v>
+      </c>
+      <c r="F1452" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1452" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr"/>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>12:16</t>
+        </is>
+      </c>
+      <c r="D1453" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1453" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1453" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1453" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -45093,7 +45496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45141,7 +45544,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 10:25:19</t>
+          <t>Última actualización: 01/01/2026 10:51:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45154,7 +45557,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 99</t>
+          <t>Total filas: 101</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -48166,6 +48569,68 @@
         <v>66</v>
       </c>
       <c r="G100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>40</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>85</v>
+      </c>
+      <c r="G102" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -48182,7 +48647,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48230,7 +48695,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 10:25:19</t>
+          <t>Última actualización: 01/01/2026 10:51:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -48243,7 +48708,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 180</t>
+          <t>Total filas: 181</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -53771,6 +54236,37 @@
         </is>
       </c>
     </row>
+    <row r="182">
+      <c r="A182" t="inlineStr"/>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>10:51:02</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F182" t="n">
+        <v>35</v>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 14:20 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1453"/>
+  <dimension ref="A1:G1466"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 10:51:08</t>
+          <t>Última actualización: 01/01/2026 11:20:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1452</t>
+          <t>Total filas: 1465</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -45480,6 +45480,409 @@
         </is>
       </c>
       <c r="G1453" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr"/>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>11:28</t>
+        </is>
+      </c>
+      <c r="D1454" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1454" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1454" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1454" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr"/>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D1455" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1455" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1455" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1455" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr"/>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="D1456" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1456" t="n">
+        <v>32</v>
+      </c>
+      <c r="F1456" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1456" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr"/>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="D1457" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1457" t="n">
+        <v>42</v>
+      </c>
+      <c r="F1457" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1457" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr"/>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>12:05</t>
+        </is>
+      </c>
+      <c r="D1458" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1458" t="n">
+        <v>46</v>
+      </c>
+      <c r="F1458" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1458" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr"/>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="D1459" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1459" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1459" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1459" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr"/>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="D1460" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1460" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1460" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1460" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr"/>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="D1461" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1461" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1461" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1461" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr"/>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="D1462" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1462" t="n">
+        <v>73</v>
+      </c>
+      <c r="F1462" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1462" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr"/>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="D1463" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1463" t="n">
+        <v>75</v>
+      </c>
+      <c r="F1463" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1463" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr"/>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>12:46</t>
+        </is>
+      </c>
+      <c r="D1464" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1464" t="n">
+        <v>87</v>
+      </c>
+      <c r="F1464" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1464" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr"/>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="D1465" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1465" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1465" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1465" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr"/>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="D1466" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1466" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1466" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1466" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -45496,7 +45899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45544,7 +45947,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 10:51:08</t>
+          <t>Última actualización: 01/01/2026 11:20:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45557,7 +45960,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 101</t>
+          <t>Total filas: 103</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -48631,6 +49034,68 @@
         <v>85</v>
       </c>
       <c r="G102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>11</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>11:19:57</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>56</v>
+      </c>
+      <c r="G104" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -48647,7 +49112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G182"/>
+  <dimension ref="A1:G183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48695,7 +49160,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 10:51:08</t>
+          <t>Última actualización: 01/01/2026 11:20:08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -48708,7 +49173,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 181</t>
+          <t>Total filas: 182</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -54267,6 +54732,37 @@
         </is>
       </c>
     </row>
+    <row r="183">
+      <c r="A183" t="inlineStr"/>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>11:20:03</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F183" t="n">
+        <v>6</v>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 14:41 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1466"/>
+  <dimension ref="A1:G1482"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:20:08</t>
+          <t>Última actualización: 01/01/2026 11:41:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1465</t>
+          <t>Total filas: 1481</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -45883,6 +45883,502 @@
         </is>
       </c>
       <c r="G1466" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr"/>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="D1467" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1467" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1467" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1467" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr"/>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="D1468" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1468" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1468" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1468" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr"/>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>11:53</t>
+        </is>
+      </c>
+      <c r="D1469" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1469" t="n">
+        <v>12</v>
+      </c>
+      <c r="F1469" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1469" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr"/>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="D1470" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1470" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1470" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1470" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr"/>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="D1471" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1471" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1471" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1471" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr"/>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>12:16</t>
+        </is>
+      </c>
+      <c r="D1472" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1472" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1472" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1472" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr"/>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="D1473" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1473" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1473" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1473" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr"/>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="D1474" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1474" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1474" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1474" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr"/>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>12:33</t>
+        </is>
+      </c>
+      <c r="D1475" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1475" t="n">
+        <v>52</v>
+      </c>
+      <c r="F1475" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1475" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr"/>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="D1476" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1476" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1476" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1476" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr"/>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>12:46</t>
+        </is>
+      </c>
+      <c r="D1477" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1477" t="n">
+        <v>65</v>
+      </c>
+      <c r="F1477" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1477" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr"/>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="D1478" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1478" t="n">
+        <v>67</v>
+      </c>
+      <c r="F1478" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1478" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr"/>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D1479" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1479" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1479" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1479" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr"/>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="D1480" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1480" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1480" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1480" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr"/>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="D1481" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1481" t="n">
+        <v>92</v>
+      </c>
+      <c r="F1481" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1481" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr"/>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="D1482" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1482" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1482" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1482" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -45899,7 +46395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45947,7 +46443,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:20:08</t>
+          <t>Última actualización: 01/01/2026 11:41:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -45960,7 +46456,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 103</t>
+          <t>Total filas: 106</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -49096,6 +49592,99 @@
         <v>56</v>
       </c>
       <c r="G104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>4</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>12:16</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>35</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>11:41:03</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>83</v>
+      </c>
+      <c r="G107" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -49112,7 +49701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G183"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49160,7 +49749,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:20:08</t>
+          <t>Última actualización: 01/01/2026 11:41:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -49173,7 +49762,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 182</t>
+          <t>Total filas: 183</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -54763,6 +55352,37 @@
         </is>
       </c>
     </row>
+    <row r="184">
+      <c r="A184" t="inlineStr"/>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>11:41:09</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F184" t="n">
+        <v>85</v>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 14:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1482"/>
+  <dimension ref="A1:G1497"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:41:14</t>
+          <t>Última actualización: 01/01/2026 11:56:56</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1481</t>
+          <t>Total filas: 1496</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -46379,6 +46379,471 @@
         </is>
       </c>
       <c r="G1482" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr"/>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="D1483" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1483" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1483" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1483" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr"/>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="D1484" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1484" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1484" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1484" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr"/>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="D1485" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1485" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1485" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1485" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr"/>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="D1486" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1486" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1486" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1486" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr"/>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="D1487" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1487" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1487" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1487" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr"/>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="D1488" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1488" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1488" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1488" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr"/>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>12:46</t>
+        </is>
+      </c>
+      <c r="D1489" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1489" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1489" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1489" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr"/>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="D1490" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1490" t="n">
+        <v>52</v>
+      </c>
+      <c r="F1490" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1490" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr"/>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="D1491" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1491" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1491" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1491" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr"/>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="D1492" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1492" t="n">
+        <v>67</v>
+      </c>
+      <c r="F1492" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1492" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr"/>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="D1493" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1493" t="n">
+        <v>77</v>
+      </c>
+      <c r="F1493" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1493" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr"/>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="D1494" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1494" t="n">
+        <v>81</v>
+      </c>
+      <c r="F1494" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1494" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr"/>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>13:19</t>
+        </is>
+      </c>
+      <c r="D1495" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1495" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1495" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1495" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr"/>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="D1496" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1496" t="n">
+        <v>89</v>
+      </c>
+      <c r="F1496" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1496" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr"/>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="D1497" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1497" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1497" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1497" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -46395,7 +46860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46443,7 +46908,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:41:14</t>
+          <t>Última actualización: 01/01/2026 11:56:56</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -46456,7 +46921,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 106</t>
+          <t>Total filas: 108</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -49685,6 +50150,68 @@
         <v>83</v>
       </c>
       <c r="G107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>12:15</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>19</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>11:56:45</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>67</v>
+      </c>
+      <c r="G109" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -49701,7 +50228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G184"/>
+  <dimension ref="A1:G186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49749,7 +50276,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:41:14</t>
+          <t>Última actualización: 01/01/2026 11:56:56</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -49762,7 +50289,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 183</t>
+          <t>Total filas: 185</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -55383,6 +55910,68 @@
         </is>
       </c>
     </row>
+    <row r="185">
+      <c r="A185" t="inlineStr"/>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>11:56:50</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>13:05</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F185" t="n">
+        <v>69</v>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr"/>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>11:56:56</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F186" t="n">
+        <v>84</v>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 15:24 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1497"/>
+  <dimension ref="A1:G1510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:56:56</t>
+          <t>Última actualización: 01/01/2026 12:24:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1496</t>
+          <t>Total filas: 1509</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -46844,6 +46844,409 @@
         </is>
       </c>
       <c r="G1497" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr"/>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="D1498" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1498" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1498" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1498" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr"/>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="D1499" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1499" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1499" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1499" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr"/>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="D1500" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1500" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1500" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1500" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr"/>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="D1501" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1501" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1501" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1501" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr"/>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>12:46</t>
+        </is>
+      </c>
+      <c r="D1502" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1502" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1502" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1502" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr"/>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="D1503" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1503" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1503" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1503" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr"/>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="D1504" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1504" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1504" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1504" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr"/>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="D1505" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1505" t="n">
+        <v>49</v>
+      </c>
+      <c r="F1505" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1505" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr"/>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="D1506" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1506" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1506" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1506" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr"/>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="D1507" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1507" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1507" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1507" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr"/>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="D1508" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1508" t="n">
+        <v>61</v>
+      </c>
+      <c r="F1508" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1508" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr"/>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="D1509" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1509" t="n">
+        <v>68</v>
+      </c>
+      <c r="F1509" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1509" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr"/>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="D1510" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1510" t="n">
+        <v>90</v>
+      </c>
+      <c r="F1510" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1510" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -46860,7 +47263,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46908,7 +47311,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:56:56</t>
+          <t>Última actualización: 01/01/2026 12:24:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -46921,7 +47324,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 108</t>
+          <t>Total filas: 109</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -50212,6 +50615,37 @@
         <v>67</v>
       </c>
       <c r="G109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>12:24:26</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>40</v>
+      </c>
+      <c r="G110" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -50228,7 +50662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:G189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50276,7 +50710,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 11:56:56</t>
+          <t>Última actualización: 01/01/2026 12:24:37</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -50289,7 +50723,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 185</t>
+          <t>Total filas: 188</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -55972,6 +56406,99 @@
         </is>
       </c>
     </row>
+    <row r="187">
+      <c r="A187" t="inlineStr"/>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>12:24:32</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F187" t="n">
+        <v>42</v>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr"/>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>12:24:37</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F188" t="n">
+        <v>57</v>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr"/>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>12:24:32</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>13:59</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F189" t="n">
+        <v>95</v>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 15:43 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1510"/>
+  <dimension ref="A1:G1522"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:24:37</t>
+          <t>Última actualización: 01/01/2026 12:43:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1509</t>
+          <t>Total filas: 1521</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -47247,6 +47247,378 @@
         </is>
       </c>
       <c r="G1510" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr"/>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>12:46</t>
+        </is>
+      </c>
+      <c r="D1511" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1511" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1511" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1511" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr"/>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="D1512" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1512" t="n">
+        <v>6</v>
+      </c>
+      <c r="F1512" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1512" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr"/>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="D1513" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1513" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1513" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1513" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr"/>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="D1514" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1514" t="n">
+        <v>21</v>
+      </c>
+      <c r="F1514" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1514" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr"/>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="D1515" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1515" t="n">
+        <v>31</v>
+      </c>
+      <c r="F1515" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1515" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr"/>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="D1516" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1516" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1516" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1516" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr"/>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="D1517" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1517" t="n">
+        <v>39</v>
+      </c>
+      <c r="F1517" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1517" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr"/>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="D1518" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1518" t="n">
+        <v>43</v>
+      </c>
+      <c r="F1518" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1518" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr"/>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="D1519" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1519" t="n">
+        <v>50</v>
+      </c>
+      <c r="F1519" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1519" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr"/>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="D1520" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1520" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1520" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1520" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr"/>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="D1521" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1521" t="n">
+        <v>85</v>
+      </c>
+      <c r="F1521" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1521" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr"/>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="D1522" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1522" t="n">
+        <v>85</v>
+      </c>
+      <c r="F1522" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1522" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -47263,7 +47635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47311,7 +47683,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:24:37</t>
+          <t>Última actualización: 01/01/2026 12:43:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -47324,7 +47696,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 109</t>
+          <t>Total filas: 110</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -50646,6 +51018,37 @@
         <v>40</v>
       </c>
       <c r="G110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>12:42:54</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>21</v>
+      </c>
+      <c r="G111" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -50662,7 +51065,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G189"/>
+  <dimension ref="A1:G192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50710,7 +51113,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:24:37</t>
+          <t>Última actualización: 01/01/2026 12:43:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -50723,7 +51126,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 188</t>
+          <t>Total filas: 191</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -56499,6 +56902,99 @@
         </is>
       </c>
     </row>
+    <row r="190">
+      <c r="A190" t="inlineStr"/>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>12:43:00</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F190" t="n">
+        <v>23</v>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr"/>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>12:43:05</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F191" t="n">
+        <v>38</v>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr"/>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>12:43:00</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>13:59</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F192" t="n">
+        <v>76</v>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 15:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1522"/>
+  <dimension ref="A1:G1532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:43:05</t>
+          <t>Última actualización: 01/01/2026 12:56:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1521</t>
+          <t>Total filas: 1531</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -47619,6 +47619,316 @@
         </is>
       </c>
       <c r="G1522" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr"/>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="D1523" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1523" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1523" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1523" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr"/>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="D1524" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1524" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1524" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1524" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr"/>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="D1525" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1525" t="n">
+        <v>21</v>
+      </c>
+      <c r="F1525" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1525" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr"/>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>13:22</t>
+        </is>
+      </c>
+      <c r="D1526" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1526" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1526" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1526" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr"/>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="D1527" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1527" t="n">
+        <v>29</v>
+      </c>
+      <c r="F1527" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1527" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr"/>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="D1528" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1528" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1528" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1528" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr"/>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="D1529" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1529" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1529" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1529" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr"/>
+      <c r="B1530" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="D1530" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1530" t="n">
+        <v>71</v>
+      </c>
+      <c r="F1530" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1530" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="inlineStr"/>
+      <c r="B1531" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>14:08</t>
+        </is>
+      </c>
+      <c r="D1531" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1531" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1531" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1531" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr"/>
+      <c r="B1532" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="D1532" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1532" t="n">
+        <v>91</v>
+      </c>
+      <c r="F1532" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1532" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -47635,7 +47945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47683,7 +47993,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:43:05</t>
+          <t>Última actualización: 01/01/2026 12:56:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -47696,7 +48006,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 110</t>
+          <t>Total filas: 111</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -51049,6 +51359,37 @@
         <v>21</v>
       </c>
       <c r="G111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>12:56:15</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>8</v>
+      </c>
+      <c r="G112" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -51065,7 +51406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G192"/>
+  <dimension ref="A1:G196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51113,7 +51454,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:43:05</t>
+          <t>Última actualización: 01/01/2026 12:56:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -51126,7 +51467,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 191</t>
+          <t>Total filas: 195</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -56995,6 +57336,130 @@
         </is>
       </c>
     </row>
+    <row r="193">
+      <c r="A193" t="inlineStr"/>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>12:56:21</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F193" t="n">
+        <v>10</v>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr"/>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>12:56:26</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F194" t="n">
+        <v>25</v>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr"/>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>12:56:21</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>13:59</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F195" t="n">
+        <v>63</v>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr"/>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>12:56:21</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F196" t="n">
+        <v>91</v>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 16:30 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1532"/>
+  <dimension ref="A1:G1540"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:56:26</t>
+          <t>Última actualización: 01/01/2026 13:30:02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1531</t>
+          <t>Total filas: 1539</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -47929,6 +47929,254 @@
         </is>
       </c>
       <c r="G1532" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" t="inlineStr"/>
+      <c r="B1533" t="inlineStr">
+        <is>
+          <t>13:29:51</t>
+        </is>
+      </c>
+      <c r="C1533" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="D1533" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1533" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1533" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1533" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" t="inlineStr"/>
+      <c r="B1534" t="inlineStr">
+        <is>
+          <t>13:29:51</t>
+        </is>
+      </c>
+      <c r="C1534" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="D1534" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1534" t="n">
+        <v>18</v>
+      </c>
+      <c r="F1534" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1534" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" t="inlineStr"/>
+      <c r="B1535" t="inlineStr">
+        <is>
+          <t>13:29:51</t>
+        </is>
+      </c>
+      <c r="C1535" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="D1535" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1535" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1535" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1535" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" t="inlineStr"/>
+      <c r="B1536" t="inlineStr">
+        <is>
+          <t>13:29:51</t>
+        </is>
+      </c>
+      <c r="C1536" t="inlineStr">
+        <is>
+          <t>14:06</t>
+        </is>
+      </c>
+      <c r="D1536" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1536" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1536" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1536" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" t="inlineStr"/>
+      <c r="B1537" t="inlineStr">
+        <is>
+          <t>13:29:51</t>
+        </is>
+      </c>
+      <c r="C1537" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="D1537" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1537" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1537" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1537" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" t="inlineStr"/>
+      <c r="B1538" t="inlineStr">
+        <is>
+          <t>13:29:51</t>
+        </is>
+      </c>
+      <c r="C1538" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="D1538" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1538" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1538" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1538" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1539">
+      <c r="A1539" t="inlineStr"/>
+      <c r="B1539" t="inlineStr">
+        <is>
+          <t>13:29:51</t>
+        </is>
+      </c>
+      <c r="C1539" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="D1539" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1539" t="n">
+        <v>82</v>
+      </c>
+      <c r="F1539" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1539" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1540">
+      <c r="A1540" t="inlineStr"/>
+      <c r="B1540" t="inlineStr">
+        <is>
+          <t>13:29:51</t>
+        </is>
+      </c>
+      <c r="C1540" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="D1540" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1540" t="n">
+        <v>93</v>
+      </c>
+      <c r="F1540" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1540" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -47993,7 +48241,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:56:26</t>
+          <t>Última actualización: 01/01/2026 13:30:02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -51406,7 +51654,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G196"/>
+  <dimension ref="A1:G198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51454,7 +51702,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 12:56:26</t>
+          <t>Última actualización: 01/01/2026 13:30:02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -51467,7 +51715,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 195</t>
+          <t>Total filas: 197</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -57460,6 +57708,68 @@
         </is>
       </c>
     </row>
+    <row r="197">
+      <c r="A197" t="inlineStr"/>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>13:29:57</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>13:58</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F197" t="n">
+        <v>29</v>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr"/>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>13:29:57</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>14:52</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F198" t="n">
+        <v>83</v>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 16:53 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1540"/>
+  <dimension ref="A1:G1548"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 13:30:02</t>
+          <t>Última actualización: 01/01/2026 13:53:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1539</t>
+          <t>Total filas: 1547</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -48177,6 +48177,254 @@
         </is>
       </c>
       <c r="G1540" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1541">
+      <c r="A1541" t="inlineStr"/>
+      <c r="B1541" t="inlineStr">
+        <is>
+          <t>13:53:33</t>
+        </is>
+      </c>
+      <c r="C1541" t="inlineStr">
+        <is>
+          <t>14:02</t>
+        </is>
+      </c>
+      <c r="D1541" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1541" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1541" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1541" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1542">
+      <c r="A1542" t="inlineStr"/>
+      <c r="B1542" t="inlineStr">
+        <is>
+          <t>13:53:33</t>
+        </is>
+      </c>
+      <c r="C1542" t="inlineStr">
+        <is>
+          <t>14:06</t>
+        </is>
+      </c>
+      <c r="D1542" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1542" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1542" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1542" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1543">
+      <c r="A1543" t="inlineStr"/>
+      <c r="B1543" t="inlineStr">
+        <is>
+          <t>13:53:33</t>
+        </is>
+      </c>
+      <c r="C1543" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="D1543" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1543" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1543" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1543" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1544">
+      <c r="A1544" t="inlineStr"/>
+      <c r="B1544" t="inlineStr">
+        <is>
+          <t>13:53:33</t>
+        </is>
+      </c>
+      <c r="C1544" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="D1544" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1544" t="n">
+        <v>46</v>
+      </c>
+      <c r="F1544" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1544" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1545">
+      <c r="A1545" t="inlineStr"/>
+      <c r="B1545" t="inlineStr">
+        <is>
+          <t>13:53:33</t>
+        </is>
+      </c>
+      <c r="C1545" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="D1545" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1545" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1545" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1545" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1546">
+      <c r="A1546" t="inlineStr"/>
+      <c r="B1546" t="inlineStr">
+        <is>
+          <t>13:53:33</t>
+        </is>
+      </c>
+      <c r="C1546" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="D1546" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1546" t="n">
+        <v>69</v>
+      </c>
+      <c r="F1546" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1546" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1547">
+      <c r="A1547" t="inlineStr"/>
+      <c r="B1547" t="inlineStr">
+        <is>
+          <t>13:53:33</t>
+        </is>
+      </c>
+      <c r="C1547" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D1547" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1547" t="n">
+        <v>80</v>
+      </c>
+      <c r="F1547" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1547" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1548">
+      <c r="A1548" t="inlineStr"/>
+      <c r="B1548" t="inlineStr">
+        <is>
+          <t>13:53:33</t>
+        </is>
+      </c>
+      <c r="C1548" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="D1548" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1548" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1548" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1548" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -48241,7 +48489,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 13:30:02</t>
+          <t>Última actualización: 01/01/2026 13:53:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -51654,7 +51902,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G198"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51702,7 +51950,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 13:30:02</t>
+          <t>Última actualización: 01/01/2026 13:53:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -51715,7 +51963,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 197</t>
+          <t>Total filas: 199</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -57770,6 +58018,68 @@
         </is>
       </c>
     </row>
+    <row r="199">
+      <c r="A199" t="inlineStr"/>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>13:53:39</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>13:58</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F199" t="n">
+        <v>5</v>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr"/>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>13:53:39</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>14:55</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F200" t="n">
+        <v>62</v>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 17:20 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1548"/>
+  <dimension ref="A1:G1558"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 13:53:44</t>
+          <t>Última actualización: 01/01/2026 14:20:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1547</t>
+          <t>Total filas: 1557</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -48425,6 +48425,316 @@
         </is>
       </c>
       <c r="G1548" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1549">
+      <c r="A1549" t="inlineStr"/>
+      <c r="B1549" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1549" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="D1549" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1549" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1549" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1549" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1550">
+      <c r="A1550" t="inlineStr"/>
+      <c r="B1550" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1550" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="D1550" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1550" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1550" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1550" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1551">
+      <c r="A1551" t="inlineStr"/>
+      <c r="B1551" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1551" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="D1551" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1551" t="n">
+        <v>31</v>
+      </c>
+      <c r="F1551" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1551" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1552">
+      <c r="A1552" t="inlineStr"/>
+      <c r="B1552" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1552" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="D1552" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1552" t="n">
+        <v>42</v>
+      </c>
+      <c r="F1552" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1552" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1553">
+      <c r="A1553" t="inlineStr"/>
+      <c r="B1553" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1553" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D1553" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1553" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1553" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1553" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1554">
+      <c r="A1554" t="inlineStr"/>
+      <c r="B1554" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1554" t="inlineStr">
+        <is>
+          <t>15:16</t>
+        </is>
+      </c>
+      <c r="D1554" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1554" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1554" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1554" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1555">
+      <c r="A1555" t="inlineStr"/>
+      <c r="B1555" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1555" t="inlineStr">
+        <is>
+          <t>15:18</t>
+        </is>
+      </c>
+      <c r="D1555" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1555" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1555" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1555" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1556">
+      <c r="A1556" t="inlineStr"/>
+      <c r="B1556" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1556" t="inlineStr">
+        <is>
+          <t>15:43</t>
+        </is>
+      </c>
+      <c r="D1556" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1556" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1556" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1556" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1557">
+      <c r="A1557" t="inlineStr"/>
+      <c r="B1557" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1557" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="D1557" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1557" t="n">
+        <v>93</v>
+      </c>
+      <c r="F1557" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1557" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1558">
+      <c r="A1558" t="inlineStr"/>
+      <c r="B1558" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C1558" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="D1558" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1558" t="n">
+        <v>97</v>
+      </c>
+      <c r="F1558" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1558" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -48441,7 +48751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48489,7 +48799,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 13:53:44</t>
+          <t>Última actualización: 01/01/2026 14:20:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -48502,7 +48812,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 111</t>
+          <t>Total filas: 112</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -51886,6 +52196,37 @@
         <v>8</v>
       </c>
       <c r="G112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>15:43</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>83</v>
+      </c>
+      <c r="G113" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -51950,7 +52291,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 13:53:44</t>
+          <t>Última actualización: 01/01/2026 14:20:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>

</xml_diff>

<commit_message>
🚌 141: 01/01 17:40 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1558"/>
+  <dimension ref="A1:G1568"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:20:19</t>
+          <t>Última actualización: 01/01/2026 14:40:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1557</t>
+          <t>Total filas: 1567</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -48735,6 +48735,316 @@
         </is>
       </c>
       <c r="G1558" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1559">
+      <c r="A1559" t="inlineStr"/>
+      <c r="B1559" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1559" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="D1559" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1559" t="n">
+        <v>12</v>
+      </c>
+      <c r="F1559" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1559" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1560">
+      <c r="A1560" t="inlineStr"/>
+      <c r="B1560" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1560" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="D1560" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1560" t="n">
+        <v>12</v>
+      </c>
+      <c r="F1560" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1560" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1561">
+      <c r="A1561" t="inlineStr"/>
+      <c r="B1561" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1561" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D1561" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1561" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1561" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1561" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1562">
+      <c r="A1562" t="inlineStr"/>
+      <c r="B1562" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1562" t="inlineStr">
+        <is>
+          <t>15:16</t>
+        </is>
+      </c>
+      <c r="D1562" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1562" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1562" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1562" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1563">
+      <c r="A1563" t="inlineStr"/>
+      <c r="B1563" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1563" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="D1563" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1563" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1563" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1563" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1564">
+      <c r="A1564" t="inlineStr"/>
+      <c r="B1564" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1564" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="D1564" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1564" t="n">
+        <v>74</v>
+      </c>
+      <c r="F1564" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1564" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1565">
+      <c r="A1565" t="inlineStr"/>
+      <c r="B1565" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1565" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="D1565" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1565" t="n">
+        <v>77</v>
+      </c>
+      <c r="F1565" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1565" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1566">
+      <c r="A1566" t="inlineStr"/>
+      <c r="B1566" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1566" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="D1566" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1566" t="n">
+        <v>81</v>
+      </c>
+      <c r="F1566" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1566" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1567">
+      <c r="A1567" t="inlineStr"/>
+      <c r="B1567" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1567" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="D1567" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1567" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1567" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1567" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1568">
+      <c r="A1568" t="inlineStr"/>
+      <c r="B1568" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="C1568" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="D1568" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1568" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1568" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1568" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -48751,7 +49061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48799,7 +49109,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:20:19</t>
+          <t>Última actualización: 01/01/2026 14:40:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -48812,7 +49122,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 112</t>
+          <t>Total filas: 113</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -52227,6 +52537,37 @@
         <v>83</v>
       </c>
       <c r="G113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>14:39:55</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>81</v>
+      </c>
+      <c r="G114" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -52243,7 +52584,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52291,7 +52632,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:20:19</t>
+          <t>Última actualización: 01/01/2026 14:40:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -52304,7 +52645,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 199</t>
+          <t>Total filas: 200</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -58421,6 +58762,37 @@
         </is>
       </c>
     </row>
+    <row r="201">
+      <c r="A201" t="inlineStr"/>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>14:40:00</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>16:02</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F201" t="n">
+        <v>82</v>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 17:51 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1568"/>
+  <dimension ref="A1:G1577"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:40:05</t>
+          <t>Última actualización: 01/01/2026 14:51:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1567</t>
+          <t>Total filas: 1576</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -49045,6 +49045,285 @@
         </is>
       </c>
       <c r="G1568" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1569">
+      <c r="A1569" t="inlineStr"/>
+      <c r="B1569" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1569" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="D1569" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1569" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1569" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1569" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1570">
+      <c r="A1570" t="inlineStr"/>
+      <c r="B1570" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1570" t="inlineStr">
+        <is>
+          <t>15:16</t>
+        </is>
+      </c>
+      <c r="D1570" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1570" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1570" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1570" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1571">
+      <c r="A1571" t="inlineStr"/>
+      <c r="B1571" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1571" t="inlineStr">
+        <is>
+          <t>15:17</t>
+        </is>
+      </c>
+      <c r="D1571" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1571" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1571" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1571" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1572">
+      <c r="A1572" t="inlineStr"/>
+      <c r="B1572" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1572" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="D1572" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1572" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1572" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1572" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1573">
+      <c r="A1573" t="inlineStr"/>
+      <c r="B1573" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1573" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="D1573" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1573" t="n">
+        <v>65</v>
+      </c>
+      <c r="F1573" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1573" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1574">
+      <c r="A1574" t="inlineStr"/>
+      <c r="B1574" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1574" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="D1574" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1574" t="n">
+        <v>74</v>
+      </c>
+      <c r="F1574" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1574" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1575">
+      <c r="A1575" t="inlineStr"/>
+      <c r="B1575" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1575" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="D1575" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1575" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1575" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1575" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1576">
+      <c r="A1576" t="inlineStr"/>
+      <c r="B1576" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1576" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="D1576" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1576" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1576" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1576" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1577">
+      <c r="A1577" t="inlineStr"/>
+      <c r="B1577" t="inlineStr">
+        <is>
+          <t>14:51:41</t>
+        </is>
+      </c>
+      <c r="C1577" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="D1577" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1577" t="n">
+        <v>86</v>
+      </c>
+      <c r="F1577" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1577" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -49109,7 +49388,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:40:05</t>
+          <t>Última actualización: 01/01/2026 14:51:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -52584,7 +52863,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G201"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52632,7 +52911,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:40:05</t>
+          <t>Última actualización: 01/01/2026 14:51:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -52645,7 +52924,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 200</t>
+          <t>Total filas: 202</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -58793,6 +59072,68 @@
         </is>
       </c>
     </row>
+    <row r="202">
+      <c r="A202" t="inlineStr"/>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>14:51:47</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F202" t="n">
+        <v>3</v>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr"/>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>14:51:47</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F203" t="n">
+        <v>70</v>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 18:30 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1577"/>
+  <dimension ref="A1:G1586"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:51:52</t>
+          <t>Última actualización: 01/01/2026 15:30:56</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1576</t>
+          <t>Total filas: 1585</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -49324,6 +49324,285 @@
         </is>
       </c>
       <c r="G1577" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1578">
+      <c r="A1578" t="inlineStr"/>
+      <c r="B1578" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1578" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="D1578" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1578" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1578" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1578" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1579">
+      <c r="A1579" t="inlineStr"/>
+      <c r="B1579" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1579" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="D1579" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1579" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1579" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1579" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1580">
+      <c r="A1580" t="inlineStr"/>
+      <c r="B1580" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1580" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="D1580" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1580" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1580" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1580" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1581">
+      <c r="A1581" t="inlineStr"/>
+      <c r="B1581" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1581" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="D1581" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1581" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1581" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1581" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1582">
+      <c r="A1582" t="inlineStr"/>
+      <c r="B1582" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1582" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="D1582" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1582" t="n">
+        <v>46</v>
+      </c>
+      <c r="F1582" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1582" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1583">
+      <c r="A1583" t="inlineStr"/>
+      <c r="B1583" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1583" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="D1583" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1583" t="n">
+        <v>47</v>
+      </c>
+      <c r="F1583" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1583" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1584">
+      <c r="A1584" t="inlineStr"/>
+      <c r="B1584" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1584" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D1584" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1584" t="n">
+        <v>60</v>
+      </c>
+      <c r="F1584" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1584" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1585">
+      <c r="A1585" t="inlineStr"/>
+      <c r="B1585" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1585" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="D1585" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1585" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1585" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1585" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1586">
+      <c r="A1586" t="inlineStr"/>
+      <c r="B1586" t="inlineStr">
+        <is>
+          <t>15:30:46</t>
+        </is>
+      </c>
+      <c r="C1586" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="D1586" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1586" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1586" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1586" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -49388,7 +49667,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:51:52</t>
+          <t>Última actualización: 01/01/2026 15:30:56</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -52863,7 +53142,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G203"/>
+  <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52911,7 +53190,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 14:51:52</t>
+          <t>Última actualización: 01/01/2026 15:30:56</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -52924,7 +53203,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 202</t>
+          <t>Total filas: 204</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -59134,6 +59413,68 @@
         </is>
       </c>
     </row>
+    <row r="204">
+      <c r="A204" t="inlineStr"/>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>15:30:51</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F204" t="n">
+        <v>31</v>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr"/>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>15:30:56</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F205" t="n">
+        <v>70</v>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 18:56 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1586"/>
+  <dimension ref="A1:G1595"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 15:30:56</t>
+          <t>Última actualización: 01/01/2026 15:56:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1585</t>
+          <t>Total filas: 1594</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -49603,6 +49603,285 @@
         </is>
       </c>
       <c r="G1586" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1587">
+      <c r="A1587" t="inlineStr"/>
+      <c r="B1587" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1587" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="D1587" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1587" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1587" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1587" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1588">
+      <c r="A1588" t="inlineStr"/>
+      <c r="B1588" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1588" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="D1588" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1588" t="n">
+        <v>18</v>
+      </c>
+      <c r="F1588" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1588" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1589">
+      <c r="A1589" t="inlineStr"/>
+      <c r="B1589" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1589" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="D1589" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1589" t="n">
+        <v>21</v>
+      </c>
+      <c r="F1589" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1589" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1590">
+      <c r="A1590" t="inlineStr"/>
+      <c r="B1590" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1590" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="D1590" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1590" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1590" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1590" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1591">
+      <c r="A1591" t="inlineStr"/>
+      <c r="B1591" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1591" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D1591" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1591" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1591" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1591" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1592">
+      <c r="A1592" t="inlineStr"/>
+      <c r="B1592" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1592" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="D1592" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1592" t="n">
+        <v>57</v>
+      </c>
+      <c r="F1592" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1592" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1593">
+      <c r="A1593" t="inlineStr"/>
+      <c r="B1593" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1593" t="inlineStr">
+        <is>
+          <t>16:55</t>
+        </is>
+      </c>
+      <c r="D1593" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1593" t="n">
+        <v>59</v>
+      </c>
+      <c r="F1593" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1593" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1594">
+      <c r="A1594" t="inlineStr"/>
+      <c r="B1594" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1594" t="inlineStr">
+        <is>
+          <t>17:11</t>
+        </is>
+      </c>
+      <c r="D1594" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1594" t="n">
+        <v>75</v>
+      </c>
+      <c r="F1594" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1594" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1595">
+      <c r="A1595" t="inlineStr"/>
+      <c r="B1595" t="inlineStr">
+        <is>
+          <t>15:56:31</t>
+        </is>
+      </c>
+      <c r="C1595" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D1595" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1595" t="n">
+        <v>85</v>
+      </c>
+      <c r="F1595" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1595" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -49667,7 +49946,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 15:30:56</t>
+          <t>Última actualización: 01/01/2026 15:56:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -53142,7 +53421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G205"/>
+  <dimension ref="A1:G208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -53190,7 +53469,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 15:30:56</t>
+          <t>Última actualización: 01/01/2026 15:56:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -53203,7 +53482,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 204</t>
+          <t>Total filas: 207</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -59475,6 +59754,99 @@
         </is>
       </c>
     </row>
+    <row r="206">
+      <c r="A206" t="inlineStr"/>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>15:56:37</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>16:02</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F206" t="n">
+        <v>6</v>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr"/>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>15:56:42</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F207" t="n">
+        <v>45</v>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr"/>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>15:56:37</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F208" t="n">
+        <v>70</v>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 19:19 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1595"/>
+  <dimension ref="A1:G1603"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 15:56:42</t>
+          <t>Última actualización: 01/01/2026 16:19:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1594</t>
+          <t>Total filas: 1602</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -49882,6 +49882,254 @@
         </is>
       </c>
       <c r="G1595" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1596">
+      <c r="A1596" t="inlineStr"/>
+      <c r="B1596" t="inlineStr">
+        <is>
+          <t>16:19:23</t>
+        </is>
+      </c>
+      <c r="C1596" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="D1596" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1596" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1596" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1596" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1597">
+      <c r="A1597" t="inlineStr"/>
+      <c r="B1597" t="inlineStr">
+        <is>
+          <t>16:19:23</t>
+        </is>
+      </c>
+      <c r="C1597" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D1597" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1597" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1597" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1597" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1598">
+      <c r="A1598" t="inlineStr"/>
+      <c r="B1598" t="inlineStr">
+        <is>
+          <t>16:19:23</t>
+        </is>
+      </c>
+      <c r="C1598" t="inlineStr">
+        <is>
+          <t>16:55</t>
+        </is>
+      </c>
+      <c r="D1598" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1598" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1598" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1598" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1599">
+      <c r="A1599" t="inlineStr"/>
+      <c r="B1599" t="inlineStr">
+        <is>
+          <t>16:19:23</t>
+        </is>
+      </c>
+      <c r="C1599" t="inlineStr">
+        <is>
+          <t>17:08</t>
+        </is>
+      </c>
+      <c r="D1599" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1599" t="n">
+        <v>49</v>
+      </c>
+      <c r="F1599" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1599" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1600">
+      <c r="A1600" t="inlineStr"/>
+      <c r="B1600" t="inlineStr">
+        <is>
+          <t>16:19:23</t>
+        </is>
+      </c>
+      <c r="C1600" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D1600" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1600" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1600" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1600" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1601">
+      <c r="A1601" t="inlineStr"/>
+      <c r="B1601" t="inlineStr">
+        <is>
+          <t>16:19:23</t>
+        </is>
+      </c>
+      <c r="C1601" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D1601" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1601" t="n">
+        <v>78</v>
+      </c>
+      <c r="F1601" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1601" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1602">
+      <c r="A1602" t="inlineStr"/>
+      <c r="B1602" t="inlineStr">
+        <is>
+          <t>16:19:23</t>
+        </is>
+      </c>
+      <c r="C1602" t="inlineStr">
+        <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="D1602" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1602" t="n">
+        <v>82</v>
+      </c>
+      <c r="F1602" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1602" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1603">
+      <c r="A1603" t="inlineStr"/>
+      <c r="B1603" t="inlineStr">
+        <is>
+          <t>16:19:23</t>
+        </is>
+      </c>
+      <c r="C1603" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="D1603" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1603" t="n">
+        <v>92</v>
+      </c>
+      <c r="F1603" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1603" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -49946,7 +50194,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 15:56:42</t>
+          <t>Última actualización: 01/01/2026 16:19:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -53421,7 +53669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G208"/>
+  <dimension ref="A1:G210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -53469,7 +53717,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 15:56:42</t>
+          <t>Última actualización: 01/01/2026 16:19:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -53482,7 +53730,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 207</t>
+          <t>Total filas: 209</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -59847,6 +60095,68 @@
         </is>
       </c>
     </row>
+    <row r="209">
+      <c r="A209" t="inlineStr"/>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>16:19:34</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F209" t="n">
+        <v>22</v>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr"/>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>16:19:29</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F210" t="n">
+        <v>47</v>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 19:32 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1603"/>
+  <dimension ref="A1:G1612"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:19:34</t>
+          <t>Última actualización: 01/01/2026 16:32:59</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1602</t>
+          <t>Total filas: 1611</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -50130,6 +50130,285 @@
         </is>
       </c>
       <c r="G1603" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1604">
+      <c r="A1604" t="inlineStr"/>
+      <c r="B1604" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1604" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="D1604" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1604" t="n">
+        <v>21</v>
+      </c>
+      <c r="F1604" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1604" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1605">
+      <c r="A1605" t="inlineStr"/>
+      <c r="B1605" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1605" t="inlineStr">
+        <is>
+          <t>16:55</t>
+        </is>
+      </c>
+      <c r="D1605" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1605" t="n">
+        <v>23</v>
+      </c>
+      <c r="F1605" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1605" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1606">
+      <c r="A1606" t="inlineStr"/>
+      <c r="B1606" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1606" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="D1606" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1606" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1606" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1606" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1607">
+      <c r="A1607" t="inlineStr"/>
+      <c r="B1607" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1607" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D1607" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1607" t="n">
+        <v>49</v>
+      </c>
+      <c r="F1607" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1607" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1608">
+      <c r="A1608" t="inlineStr"/>
+      <c r="B1608" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1608" t="inlineStr">
+        <is>
+          <t>17:35</t>
+        </is>
+      </c>
+      <c r="D1608" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1608" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1608" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1608" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1609">
+      <c r="A1609" t="inlineStr"/>
+      <c r="B1609" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1609" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D1609" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1609" t="n">
+        <v>65</v>
+      </c>
+      <c r="F1609" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1609" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1610">
+      <c r="A1610" t="inlineStr"/>
+      <c r="B1610" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1610" t="inlineStr">
+        <is>
+          <t>17:49</t>
+        </is>
+      </c>
+      <c r="D1610" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1610" t="n">
+        <v>77</v>
+      </c>
+      <c r="F1610" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1610" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1611">
+      <c r="A1611" t="inlineStr"/>
+      <c r="B1611" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1611" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="D1611" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1611" t="n">
+        <v>93</v>
+      </c>
+      <c r="F1611" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1611" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1612">
+      <c r="A1612" t="inlineStr"/>
+      <c r="B1612" t="inlineStr">
+        <is>
+          <t>16:32:48</t>
+        </is>
+      </c>
+      <c r="C1612" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="D1612" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1612" t="n">
+        <v>98</v>
+      </c>
+      <c r="F1612" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1612" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -50194,7 +50473,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:19:34</t>
+          <t>Última actualización: 01/01/2026 16:32:59</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -53669,7 +53948,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G210"/>
+  <dimension ref="A1:G212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -53717,7 +53996,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:19:34</t>
+          <t>Última actualización: 01/01/2026 16:32:59</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -53730,7 +54009,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 209</t>
+          <t>Total filas: 211</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -60157,6 +60436,68 @@
         </is>
       </c>
     </row>
+    <row r="211">
+      <c r="A211" t="inlineStr"/>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>16:32:58</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="F211" t="n">
+        <v>9</v>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr"/>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>16:32:53</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F212" t="n">
+        <v>33</v>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 19:46 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1612"/>
+  <dimension ref="A1:G1621"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:32:59</t>
+          <t>Última actualización: 01/01/2026 16:46:27</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1611</t>
+          <t>Total filas: 1620</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -50409,6 +50409,285 @@
         </is>
       </c>
       <c r="G1612" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1613">
+      <c r="A1613" t="inlineStr"/>
+      <c r="B1613" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1613" t="inlineStr">
+        <is>
+          <t>16:54</t>
+        </is>
+      </c>
+      <c r="D1613" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1613" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1613" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1613" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1614">
+      <c r="A1614" t="inlineStr"/>
+      <c r="B1614" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1614" t="inlineStr">
+        <is>
+          <t>16:55</t>
+        </is>
+      </c>
+      <c r="D1614" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1614" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1614" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1614" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1615">
+      <c r="A1615" t="inlineStr"/>
+      <c r="B1615" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1615" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="D1615" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1615" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1615" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1615" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1616">
+      <c r="A1616" t="inlineStr"/>
+      <c r="B1616" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1616" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D1616" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1616" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1616" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1616" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1617">
+      <c r="A1617" t="inlineStr"/>
+      <c r="B1617" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1617" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D1617" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1617" t="n">
+        <v>51</v>
+      </c>
+      <c r="F1617" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1617" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1618">
+      <c r="A1618" t="inlineStr"/>
+      <c r="B1618" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1618" t="inlineStr">
+        <is>
+          <t>17:49</t>
+        </is>
+      </c>
+      <c r="D1618" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1618" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1618" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1618" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1619">
+      <c r="A1619" t="inlineStr"/>
+      <c r="B1619" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1619" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="D1619" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1619" t="n">
+        <v>80</v>
+      </c>
+      <c r="F1619" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1619" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1620">
+      <c r="A1620" t="inlineStr"/>
+      <c r="B1620" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1620" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="D1620" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1620" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1620" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1620" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1621">
+      <c r="A1621" t="inlineStr"/>
+      <c r="B1621" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="C1621" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="D1621" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1621" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1621" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1621" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -50425,7 +50704,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50473,7 +50752,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:32:59</t>
+          <t>Última actualización: 01/01/2026 16:46:27</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -50486,7 +50765,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 113</t>
+          <t>Total filas: 114</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -53932,6 +54211,37 @@
         <v>81</v>
       </c>
       <c r="G114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>16:46:16</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>96</v>
+      </c>
+      <c r="G115" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -53948,7 +54258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G212"/>
+  <dimension ref="A1:G213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -53996,7 +54306,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:32:59</t>
+          <t>Última actualización: 01/01/2026 16:46:27</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -54009,7 +54319,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 211</t>
+          <t>Total filas: 212</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -60498,6 +60808,37 @@
         </is>
       </c>
     </row>
+    <row r="213">
+      <c r="A213" t="inlineStr"/>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>16:46:22</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F213" t="n">
+        <v>20</v>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 19:57 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1621"/>
+  <dimension ref="A1:G1629"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:46:27</t>
+          <t>Última actualización: 01/01/2026 16:57:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1620</t>
+          <t>Total filas: 1628</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -50688,6 +50688,254 @@
         </is>
       </c>
       <c r="G1621" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1622">
+      <c r="A1622" t="inlineStr"/>
+      <c r="B1622" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="C1622" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="D1622" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1622" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1622" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1622" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1623">
+      <c r="A1623" t="inlineStr"/>
+      <c r="B1623" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="C1623" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="D1623" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1623" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1623" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1623" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1624">
+      <c r="A1624" t="inlineStr"/>
+      <c r="B1624" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="C1624" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D1624" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1624" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1624" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1624" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1625">
+      <c r="A1625" t="inlineStr"/>
+      <c r="B1625" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="C1625" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="D1625" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1625" t="n">
+        <v>48</v>
+      </c>
+      <c r="F1625" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1625" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1626">
+      <c r="A1626" t="inlineStr"/>
+      <c r="B1626" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="C1626" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="D1626" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1626" t="n">
+        <v>69</v>
+      </c>
+      <c r="F1626" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1626" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1627">
+      <c r="A1627" t="inlineStr"/>
+      <c r="B1627" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="C1627" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="D1627" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1627" t="n">
+        <v>73</v>
+      </c>
+      <c r="F1627" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1627" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1628">
+      <c r="A1628" t="inlineStr"/>
+      <c r="B1628" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="C1628" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="D1628" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1628" t="n">
+        <v>85</v>
+      </c>
+      <c r="F1628" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1628" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1629">
+      <c r="A1629" t="inlineStr"/>
+      <c r="B1629" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="C1629" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D1629" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1629" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1629" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1629" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -50704,7 +50952,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50752,7 +51000,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:46:27</t>
+          <t>Última actualización: 01/01/2026 16:57:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -50765,7 +51013,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 114</t>
+          <t>Total filas: 115</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -54242,6 +54490,37 @@
         <v>96</v>
       </c>
       <c r="G115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>16:57:03</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>85</v>
+      </c>
+      <c r="G116" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -54258,7 +54537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G213"/>
+  <dimension ref="A1:G214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54306,7 +54585,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:46:27</t>
+          <t>Última actualización: 01/01/2026 16:57:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -54319,7 +54598,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 212</t>
+          <t>Total filas: 213</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -60839,6 +61118,37 @@
         </is>
       </c>
     </row>
+    <row r="214">
+      <c r="A214" t="inlineStr"/>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>16:57:09</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>17:06</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F214" t="n">
+        <v>9</v>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 20:29 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1629"/>
+  <dimension ref="A1:G1642"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:57:14</t>
+          <t>Última actualización: 01/01/2026 17:29:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1628</t>
+          <t>Total filas: 1641</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -50936,6 +50936,409 @@
         </is>
       </c>
       <c r="G1629" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1630">
+      <c r="A1630" t="inlineStr"/>
+      <c r="B1630" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1630" t="inlineStr">
+        <is>
+          <t>17:31</t>
+        </is>
+      </c>
+      <c r="D1630" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1630" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1630" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1630" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1631">
+      <c r="A1631" t="inlineStr"/>
+      <c r="B1631" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1631" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="D1631" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1631" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1631" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1631" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1632">
+      <c r="A1632" t="inlineStr"/>
+      <c r="B1632" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1632" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="D1632" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1632" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1632" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1632" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1633">
+      <c r="A1633" t="inlineStr"/>
+      <c r="B1633" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1633" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="D1633" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1633" t="n">
+        <v>41</v>
+      </c>
+      <c r="F1633" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1633" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1634">
+      <c r="A1634" t="inlineStr"/>
+      <c r="B1634" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1634" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="D1634" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1634" t="n">
+        <v>53</v>
+      </c>
+      <c r="F1634" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1634" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1635">
+      <c r="A1635" t="inlineStr"/>
+      <c r="B1635" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1635" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D1635" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1635" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1635" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1635" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1636">
+      <c r="A1636" t="inlineStr"/>
+      <c r="B1636" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1636" t="inlineStr">
+        <is>
+          <t>18:35</t>
+        </is>
+      </c>
+      <c r="D1636" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1636" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1636" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1636" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1637">
+      <c r="A1637" t="inlineStr"/>
+      <c r="B1637" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1637" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="D1637" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1637" t="n">
+        <v>76</v>
+      </c>
+      <c r="F1637" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1637" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1638">
+      <c r="A1638" t="inlineStr"/>
+      <c r="B1638" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1638" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="D1638" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1638" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1638" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1638" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1639">
+      <c r="A1639" t="inlineStr"/>
+      <c r="B1639" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1639" t="inlineStr">
+        <is>
+          <t>18:53</t>
+        </is>
+      </c>
+      <c r="D1639" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1639" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1639" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1639" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1640">
+      <c r="A1640" t="inlineStr"/>
+      <c r="B1640" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1640" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="D1640" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1640" t="n">
+        <v>88</v>
+      </c>
+      <c r="F1640" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1640" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1641">
+      <c r="A1641" t="inlineStr"/>
+      <c r="B1641" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1641" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="D1641" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1641" t="n">
+        <v>90</v>
+      </c>
+      <c r="F1641" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1641" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1642">
+      <c r="A1642" t="inlineStr"/>
+      <c r="B1642" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="C1642" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="D1642" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1642" t="n">
+        <v>97</v>
+      </c>
+      <c r="F1642" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1642" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -50952,7 +51355,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51000,7 +51403,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:57:14</t>
+          <t>Última actualización: 01/01/2026 17:29:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -51013,7 +51416,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 115</t>
+          <t>Total filas: 117</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -54521,6 +54924,68 @@
         <v>85</v>
       </c>
       <c r="G116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>53</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>17:29:27</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>97</v>
+      </c>
+      <c r="G118" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -54537,7 +55002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G214"/>
+  <dimension ref="A1:G215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54585,7 +55050,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 16:57:14</t>
+          <t>Última actualización: 01/01/2026 17:29:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -54598,7 +55063,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 213</t>
+          <t>Total filas: 214</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -61149,6 +61614,37 @@
         </is>
       </c>
     </row>
+    <row r="215">
+      <c r="A215" t="inlineStr"/>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>17:29:32</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F215" t="n">
+        <v>67</v>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 20:47 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1642"/>
+  <dimension ref="A1:G1656"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:29:38</t>
+          <t>Última actualización: 01/01/2026 17:47:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1641</t>
+          <t>Total filas: 1655</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -51339,6 +51339,440 @@
         </is>
       </c>
       <c r="G1642" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1643">
+      <c r="A1643" t="inlineStr"/>
+      <c r="B1643" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1643" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="D1643" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1643" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1643" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1643" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1644">
+      <c r="A1644" t="inlineStr"/>
+      <c r="B1644" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1644" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="D1644" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1644" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1644" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1644" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1645">
+      <c r="A1645" t="inlineStr"/>
+      <c r="B1645" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1645" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="D1645" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1645" t="n">
+        <v>23</v>
+      </c>
+      <c r="F1645" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1645" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1646">
+      <c r="A1646" t="inlineStr"/>
+      <c r="B1646" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1646" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="D1646" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1646" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1646" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1646" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1647">
+      <c r="A1647" t="inlineStr"/>
+      <c r="B1647" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1647" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D1647" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1647" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1647" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1647" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1648">
+      <c r="A1648" t="inlineStr"/>
+      <c r="B1648" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1648" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="D1648" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1648" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1648" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1648" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1649">
+      <c r="A1649" t="inlineStr"/>
+      <c r="B1649" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1649" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="D1649" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1649" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1649" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1649" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1650">
+      <c r="A1650" t="inlineStr"/>
+      <c r="B1650" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1650" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="D1650" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1650" t="n">
+        <v>65</v>
+      </c>
+      <c r="F1650" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1650" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1651">
+      <c r="A1651" t="inlineStr"/>
+      <c r="B1651" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1651" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="D1651" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1651" t="n">
+        <v>70</v>
+      </c>
+      <c r="F1651" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1651" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1652">
+      <c r="A1652" t="inlineStr"/>
+      <c r="B1652" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1652" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D1652" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1652" t="n">
+        <v>73</v>
+      </c>
+      <c r="F1652" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1652" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1653">
+      <c r="A1653" t="inlineStr"/>
+      <c r="B1653" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1653" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="D1653" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1653" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1653" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1653" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1654">
+      <c r="A1654" t="inlineStr"/>
+      <c r="B1654" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1654" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="D1654" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1654" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1654" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1654" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1655">
+      <c r="A1655" t="inlineStr"/>
+      <c r="B1655" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1655" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="D1655" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1655" t="n">
+        <v>90</v>
+      </c>
+      <c r="F1655" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1655" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1656">
+      <c r="A1656" t="inlineStr"/>
+      <c r="B1656" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="C1656" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="D1656" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1656" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1656" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1656" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -51355,7 +51789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51403,7 +51837,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:29:38</t>
+          <t>Última actualización: 01/01/2026 17:47:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -51416,7 +51850,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 117</t>
+          <t>Total filas: 120</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -54986,6 +55420,99 @@
         <v>97</v>
       </c>
       <c r="G118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>3</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>35</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>17:47:27</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>79</v>
+      </c>
+      <c r="G121" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -55002,7 +55529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G215"/>
+  <dimension ref="A1:G217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55050,7 +55577,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:29:38</t>
+          <t>Última actualización: 01/01/2026 17:47:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -55063,7 +55590,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 214</t>
+          <t>Total filas: 216</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -61645,6 +62172,68 @@
         </is>
       </c>
     </row>
+    <row r="216">
+      <c r="A216" t="inlineStr"/>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>17:47:33</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F216" t="n">
+        <v>49</v>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr"/>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>17:47:38</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F217" t="n">
+        <v>97</v>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 20:58 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1656"/>
+  <dimension ref="A1:G1672"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:47:38</t>
+          <t>Última actualización: 01/01/2026 17:58:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1655</t>
+          <t>Total filas: 1671</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -51773,6 +51773,502 @@
         </is>
       </c>
       <c r="G1656" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1657">
+      <c r="A1657" t="inlineStr"/>
+      <c r="B1657" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1657" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="D1657" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="E1657" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1657" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1657" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1658">
+      <c r="A1658" t="inlineStr"/>
+      <c r="B1658" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1658" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="D1658" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1658" t="n">
+        <v>12</v>
+      </c>
+      <c r="F1658" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1658" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1659">
+      <c r="A1659" t="inlineStr"/>
+      <c r="B1659" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1659" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="D1659" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1659" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1659" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1659" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1660">
+      <c r="A1660" t="inlineStr"/>
+      <c r="B1660" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1660" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="D1660" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1660" t="n">
+        <v>27</v>
+      </c>
+      <c r="F1660" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1660" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1661">
+      <c r="A1661" t="inlineStr"/>
+      <c r="B1661" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1661" t="inlineStr">
+        <is>
+          <t>18:37</t>
+        </is>
+      </c>
+      <c r="D1661" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1661" t="n">
+        <v>39</v>
+      </c>
+      <c r="F1661" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1661" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1662">
+      <c r="A1662" t="inlineStr"/>
+      <c r="B1662" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1662" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="D1662" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1662" t="n">
+        <v>47</v>
+      </c>
+      <c r="F1662" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1662" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1663">
+      <c r="A1663" t="inlineStr"/>
+      <c r="B1663" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1663" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="D1663" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1663" t="n">
+        <v>54</v>
+      </c>
+      <c r="F1663" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1663" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1664">
+      <c r="A1664" t="inlineStr"/>
+      <c r="B1664" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1664" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="D1664" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1664" t="n">
+        <v>59</v>
+      </c>
+      <c r="F1664" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1664" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1665">
+      <c r="A1665" t="inlineStr"/>
+      <c r="B1665" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1665" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D1665" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1665" t="n">
+        <v>62</v>
+      </c>
+      <c r="F1665" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1665" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1666">
+      <c r="A1666" t="inlineStr"/>
+      <c r="B1666" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1666" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="D1666" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1666" t="n">
+        <v>68</v>
+      </c>
+      <c r="F1666" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1666" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1667">
+      <c r="A1667" t="inlineStr"/>
+      <c r="B1667" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1667" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="D1667" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1667" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1667" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1667" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1668">
+      <c r="A1668" t="inlineStr"/>
+      <c r="B1668" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1668" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="D1668" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1668" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1668" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1668" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1669">
+      <c r="A1669" t="inlineStr"/>
+      <c r="B1669" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1669" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="D1669" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1669" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1669" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1669" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1670">
+      <c r="A1670" t="inlineStr"/>
+      <c r="B1670" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1670" t="inlineStr">
+        <is>
+          <t>19:23</t>
+        </is>
+      </c>
+      <c r="D1670" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1670" t="n">
+        <v>85</v>
+      </c>
+      <c r="F1670" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1670" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1671">
+      <c r="A1671" t="inlineStr"/>
+      <c r="B1671" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1671" t="inlineStr">
+        <is>
+          <t>19:33</t>
+        </is>
+      </c>
+      <c r="D1671" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="E1671" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1671" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1671" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1672">
+      <c r="A1672" t="inlineStr"/>
+      <c r="B1672" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="C1672" t="inlineStr">
+        <is>
+          <t>19:34</t>
+        </is>
+      </c>
+      <c r="D1672" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1672" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1672" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1672" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -51789,7 +52285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51837,7 +52333,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:47:38</t>
+          <t>Última actualización: 01/01/2026 17:58:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -51850,7 +52346,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 120</t>
+          <t>Total filas: 123</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -55513,6 +56009,99 @@
         <v>79</v>
       </c>
       <c r="G121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>24</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>68</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>17:58:08</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>19:34</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>96</v>
+      </c>
+      <c r="G124" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -55529,7 +56118,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G217"/>
+  <dimension ref="A1:G219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55577,7 +56166,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:47:38</t>
+          <t>Última actualización: 01/01/2026 17:58:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -55590,7 +56179,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 216</t>
+          <t>Total filas: 218</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -62234,6 +62823,68 @@
         </is>
       </c>
     </row>
+    <row r="218">
+      <c r="A218" t="inlineStr"/>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>17:58:13</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F218" t="n">
+        <v>38</v>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr"/>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>17:58:18</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F219" t="n">
+        <v>86</v>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 21:26 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1672"/>
+  <dimension ref="A1:G1686"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:58:19</t>
+          <t>Última actualización: 01/01/2026 18:26:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1671</t>
+          <t>Total filas: 1685</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -52269,6 +52269,440 @@
         </is>
       </c>
       <c r="G1672" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1673">
+      <c r="A1673" t="inlineStr"/>
+      <c r="B1673" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1673" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="D1673" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1673" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1673" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1673" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1674">
+      <c r="A1674" t="inlineStr"/>
+      <c r="B1674" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1674" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="D1674" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1674" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1674" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1674" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1675">
+      <c r="A1675" t="inlineStr"/>
+      <c r="B1675" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1675" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="D1675" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1675" t="n">
+        <v>31</v>
+      </c>
+      <c r="F1675" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1675" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1676">
+      <c r="A1676" t="inlineStr"/>
+      <c r="B1676" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1676" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D1676" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1676" t="n">
+        <v>34</v>
+      </c>
+      <c r="F1676" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1676" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1677">
+      <c r="A1677" t="inlineStr"/>
+      <c r="B1677" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1677" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="D1677" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1677" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1677" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1677" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1678">
+      <c r="A1678" t="inlineStr"/>
+      <c r="B1678" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1678" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="D1678" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1678" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1678" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1678" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1679">
+      <c r="A1679" t="inlineStr"/>
+      <c r="B1679" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1679" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="D1679" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1679" t="n">
+        <v>51</v>
+      </c>
+      <c r="F1679" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1679" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1680">
+      <c r="A1680" t="inlineStr"/>
+      <c r="B1680" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1680" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D1680" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1680" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1680" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1680" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1681">
+      <c r="A1681" t="inlineStr"/>
+      <c r="B1681" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1681" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="D1681" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1681" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1681" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1681" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1682">
+      <c r="A1682" t="inlineStr"/>
+      <c r="B1682" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1682" t="inlineStr">
+        <is>
+          <t>19:23</t>
+        </is>
+      </c>
+      <c r="D1682" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1682" t="n">
+        <v>57</v>
+      </c>
+      <c r="F1682" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1682" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1683">
+      <c r="A1683" t="inlineStr"/>
+      <c r="B1683" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1683" t="inlineStr">
+        <is>
+          <t>19:34</t>
+        </is>
+      </c>
+      <c r="D1683" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1683" t="n">
+        <v>68</v>
+      </c>
+      <c r="F1683" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1683" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1684">
+      <c r="A1684" t="inlineStr"/>
+      <c r="B1684" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1684" t="inlineStr">
+        <is>
+          <t>19:47</t>
+        </is>
+      </c>
+      <c r="D1684" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1684" t="n">
+        <v>81</v>
+      </c>
+      <c r="F1684" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1684" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1685">
+      <c r="A1685" t="inlineStr"/>
+      <c r="B1685" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1685" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="D1685" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1685" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1685" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1685" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1686">
+      <c r="A1686" t="inlineStr"/>
+      <c r="B1686" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="C1686" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="D1686" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1686" t="n">
+        <v>87</v>
+      </c>
+      <c r="F1686" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1686" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -52285,7 +52719,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52333,7 +52767,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:58:19</t>
+          <t>Última actualización: 01/01/2026 18:26:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -52346,7 +52780,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 123</t>
+          <t>Total filas: 125</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -56102,6 +56536,68 @@
         <v>96</v>
       </c>
       <c r="G124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>40</v>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr"/>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>18:26:27</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>19:34</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>68</v>
+      </c>
+      <c r="G126" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -56118,7 +56614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G219"/>
+  <dimension ref="A1:G222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56166,7 +56662,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 17:58:19</t>
+          <t>Última actualización: 01/01/2026 18:26:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -56179,7 +56675,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 218</t>
+          <t>Total filas: 221</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -62885,6 +63381,99 @@
         </is>
       </c>
     </row>
+    <row r="220">
+      <c r="A220" t="inlineStr"/>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>18:26:32</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F220" t="n">
+        <v>10</v>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr"/>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>18:26:37</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F221" t="n">
+        <v>58</v>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr"/>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>18:26:32</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F222" t="n">
+        <v>95</v>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 21:42 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1686"/>
+  <dimension ref="A1:G1700"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 18:26:38</t>
+          <t>Última actualización: 01/01/2026 18:42:23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1685</t>
+          <t>Total filas: 1699</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -52703,6 +52703,440 @@
         </is>
       </c>
       <c r="G1686" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1687">
+      <c r="A1687" t="inlineStr"/>
+      <c r="B1687" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1687" t="inlineStr">
+        <is>
+          <t>18:46</t>
+        </is>
+      </c>
+      <c r="D1687" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1687" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1687" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1687" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1688">
+      <c r="A1688" t="inlineStr"/>
+      <c r="B1688" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1688" t="inlineStr">
+        <is>
+          <t>18:53</t>
+        </is>
+      </c>
+      <c r="D1688" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1688" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1688" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1688" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1689">
+      <c r="A1689" t="inlineStr"/>
+      <c r="B1689" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1689" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="D1689" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1689" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1689" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1689" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1690">
+      <c r="A1690" t="inlineStr"/>
+      <c r="B1690" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1690" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="D1690" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1690" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1690" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1690" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1691">
+      <c r="A1691" t="inlineStr"/>
+      <c r="B1691" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1691" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="D1691" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1691" t="n">
+        <v>29</v>
+      </c>
+      <c r="F1691" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1691" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1692">
+      <c r="A1692" t="inlineStr"/>
+      <c r="B1692" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1692" t="inlineStr">
+        <is>
+          <t>19:18</t>
+        </is>
+      </c>
+      <c r="D1692" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1692" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1692" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1692" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1693">
+      <c r="A1693" t="inlineStr"/>
+      <c r="B1693" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1693" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="D1693" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="E1693" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1693" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1693" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1694">
+      <c r="A1694" t="inlineStr"/>
+      <c r="B1694" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1694" t="inlineStr">
+        <is>
+          <t>19:22</t>
+        </is>
+      </c>
+      <c r="D1694" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1694" t="n">
+        <v>40</v>
+      </c>
+      <c r="F1694" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1694" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1695">
+      <c r="A1695" t="inlineStr"/>
+      <c r="B1695" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1695" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="D1695" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1695" t="n">
+        <v>42</v>
+      </c>
+      <c r="F1695" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1695" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1696">
+      <c r="A1696" t="inlineStr"/>
+      <c r="B1696" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1696" t="inlineStr">
+        <is>
+          <t>19:34</t>
+        </is>
+      </c>
+      <c r="D1696" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1696" t="n">
+        <v>52</v>
+      </c>
+      <c r="F1696" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1696" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1697">
+      <c r="A1697" t="inlineStr"/>
+      <c r="B1697" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1697" t="inlineStr">
+        <is>
+          <t>19:48</t>
+        </is>
+      </c>
+      <c r="D1697" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1697" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1697" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1697" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1698">
+      <c r="A1698" t="inlineStr"/>
+      <c r="B1698" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1698" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="D1698" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1698" t="n">
+        <v>71</v>
+      </c>
+      <c r="F1698" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1698" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1699">
+      <c r="A1699" t="inlineStr"/>
+      <c r="B1699" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1699" t="inlineStr">
+        <is>
+          <t>20:16</t>
+        </is>
+      </c>
+      <c r="D1699" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1699" t="n">
+        <v>94</v>
+      </c>
+      <c r="F1699" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1699" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1700">
+      <c r="A1700" t="inlineStr"/>
+      <c r="B1700" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="C1700" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="D1700" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1700" t="n">
+        <v>98</v>
+      </c>
+      <c r="F1700" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1700" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -52719,7 +53153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52767,7 +53201,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 18:26:38</t>
+          <t>Última actualización: 01/01/2026 18:42:23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -52780,7 +53214,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 125</t>
+          <t>Total filas: 128</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -56598,6 +57032,99 @@
         <v>68</v>
       </c>
       <c r="G126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>19:06</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>24</v>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr"/>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>19:34</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>52</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>18:42:12</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>20:16</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>94</v>
+      </c>
+      <c r="G129" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -56614,7 +57141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G222"/>
+  <dimension ref="A1:G224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56662,7 +57189,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 18:26:38</t>
+          <t>Última actualización: 01/01/2026 18:42:23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -56675,7 +57202,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 221</t>
+          <t>Total filas: 223</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -63474,6 +64001,68 @@
         </is>
       </c>
     </row>
+    <row r="223">
+      <c r="A223" t="inlineStr"/>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>18:42:22</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F223" t="n">
+        <v>42</v>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr"/>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>18:42:17</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>20:01</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F224" t="n">
+        <v>79</v>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🚌 141: 01/01 21:55 LP1912+6203+6173
</commit_message>
<xml_diff>
--- a/horarios-141-completo.xlsx
+++ b/horarios-141-completo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1700"/>
+  <dimension ref="A1:G1714"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 18:42:23</t>
+          <t>Última actualización: 01/01/2026 18:55:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 1699</t>
+          <t>Total filas: 1713</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -53137,6 +53137,440 @@
         </is>
       </c>
       <c r="G1700" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1701">
+      <c r="A1701" t="inlineStr"/>
+      <c r="B1701" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1701" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="D1701" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1701" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1701" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1701" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1702">
+      <c r="A1702" t="inlineStr"/>
+      <c r="B1702" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1702" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="D1702" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="E1702" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1702" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1702" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1703">
+      <c r="A1703" t="inlineStr"/>
+      <c r="B1703" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1703" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="D1703" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1703" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1703" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1703" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1704">
+      <c r="A1704" t="inlineStr"/>
+      <c r="B1704" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1704" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="D1704" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1704" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1704" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1704" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1705">
+      <c r="A1705" t="inlineStr"/>
+      <c r="B1705" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1705" t="inlineStr">
+        <is>
+          <t>19:23</t>
+        </is>
+      </c>
+      <c r="D1705" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1705" t="n">
+        <v>28</v>
+      </c>
+      <c r="F1705" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1705" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1706">
+      <c r="A1706" t="inlineStr"/>
+      <c r="B1706" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1706" t="inlineStr">
+        <is>
+          <t>19:33</t>
+        </is>
+      </c>
+      <c r="D1706" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1706" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1706" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1706" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1707">
+      <c r="A1707" t="inlineStr"/>
+      <c r="B1707" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1707" t="inlineStr">
+        <is>
+          <t>19:47</t>
+        </is>
+      </c>
+      <c r="D1707" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1707" t="n">
+        <v>52</v>
+      </c>
+      <c r="F1707" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1707" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1708">
+      <c r="A1708" t="inlineStr"/>
+      <c r="B1708" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1708" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="D1708" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1708" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1708" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1708" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1709">
+      <c r="A1709" t="inlineStr"/>
+      <c r="B1709" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1709" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="D1709" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="E1709" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1709" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1709" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1710">
+      <c r="A1710" t="inlineStr"/>
+      <c r="B1710" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1710" t="inlineStr">
+        <is>
+          <t>20:15</t>
+        </is>
+      </c>
+      <c r="D1710" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="E1710" t="n">
+        <v>80</v>
+      </c>
+      <c r="F1710" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1710" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1711">
+      <c r="A1711" t="inlineStr"/>
+      <c r="B1711" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1711" t="inlineStr">
+        <is>
+          <t>20:19</t>
+        </is>
+      </c>
+      <c r="D1711" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="E1711" t="n">
+        <v>84</v>
+      </c>
+      <c r="F1711" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1711" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1712">
+      <c r="A1712" t="inlineStr"/>
+      <c r="B1712" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1712" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="D1712" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="E1712" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1712" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1712" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1713">
+      <c r="A1713" t="inlineStr"/>
+      <c r="B1713" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1713" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="D1713" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="E1713" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1713" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1713" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1714">
+      <c r="A1714" t="inlineStr"/>
+      <c r="B1714" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="C1714" t="inlineStr">
+        <is>
+          <t>20:34</t>
+        </is>
+      </c>
+      <c r="D1714" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="E1714" t="n">
+        <v>99</v>
+      </c>
+      <c r="F1714" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+      <c r="G1714" t="inlineStr">
         <is>
           <t>01/01/2026</t>
         </is>
@@ -53153,7 +53587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -53201,7 +53635,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 18:42:23</t>
+          <t>Última actualización: 01/01/2026 18:55:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -53214,7 +53648,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 128</t>
+          <t>Total filas: 131</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -57125,6 +57559,99 @@
         <v>94</v>
       </c>
       <c r="G129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>10</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>19:33</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>38</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>18:55:46</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>20:15</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>80</v>
+      </c>
+      <c r="G132" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -57141,7 +57668,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G224"/>
+  <dimension ref="A1:G226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -57189,7 +57716,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Última actualización: 01/01/2026 18:42:23</t>
+          <t>Última actualización: 01/01/2026 18:55:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -57202,7 +57729,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total filas: 223</t>
+          <t>Total filas: 225</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -64063,6 +64590,68 @@
         </is>
       </c>
     </row>
+    <row r="225">
+      <c r="A225" t="inlineStr"/>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>18:55:57</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>19:23</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="F225" t="n">
+        <v>28</v>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr"/>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>18:55:52</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="F226" t="n">
+        <v>65</v>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>